<commit_message>
remove SH file, add to variable key
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -5,31 +5,32 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/00042030/AED Dropbox/AED_Cockburn_db/CSIEM/Data/Matt/csiem-data/data-governance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SSD2/AED Dropbox/AED_Cockburn_db/CSIEM/Data/Matt/csiem-data/data-governance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45ABD98D-5318-6740-95A4-DE3314F62E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0E2702-4C5B-B24E-A294-72E5D0A60508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17960" tabRatio="671" xr2:uid="{6DF7D7CC-01DB-4B77-91E2-7CCE474EE386}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17960" tabRatio="671" activeTab="1" xr2:uid="{6DF7D7CC-01DB-4B77-91E2-7CCE474EE386}"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER KEY" sheetId="1" r:id="rId1"/>
-    <sheet name="Model_TFV" sheetId="5" r:id="rId2"/>
-    <sheet name="MAFRL" sheetId="8" r:id="rId3"/>
-    <sheet name="IMOSBGC" sheetId="9" r:id="rId4"/>
-    <sheet name="IMOSPROFILE" sheetId="10" r:id="rId5"/>
-    <sheet name="DWER" sheetId="2" r:id="rId6"/>
-    <sheet name="DWERMOORING" sheetId="11" r:id="rId7"/>
-    <sheet name="BOM" sheetId="3" r:id="rId8"/>
-    <sheet name="DOT" sheetId="4" r:id="rId9"/>
-    <sheet name="THEME5" sheetId="7" r:id="rId10"/>
-    <sheet name="WWMSP5" sheetId="16" r:id="rId11"/>
-    <sheet name="JPPLAWAC" sheetId="12" r:id="rId12"/>
-    <sheet name="UWA" sheetId="15" r:id="rId13"/>
-    <sheet name="BMTBNA" sheetId="17" r:id="rId14"/>
-    <sheet name="FPA_BMT" sheetId="14" r:id="rId15"/>
-    <sheet name="WC_BMT" sheetId="13" r:id="rId16"/>
-    <sheet name="Information" sheetId="6" r:id="rId17"/>
+    <sheet name="SentientHubs" sheetId="18" r:id="rId2"/>
+    <sheet name="Model_TFV" sheetId="5" r:id="rId3"/>
+    <sheet name="MAFRL" sheetId="8" r:id="rId4"/>
+    <sheet name="IMOSBGC" sheetId="9" r:id="rId5"/>
+    <sheet name="IMOSPROFILE" sheetId="10" r:id="rId6"/>
+    <sheet name="DWER" sheetId="2" r:id="rId7"/>
+    <sheet name="DWERMOORING" sheetId="11" r:id="rId8"/>
+    <sheet name="BOM" sheetId="3" r:id="rId9"/>
+    <sheet name="DOT" sheetId="4" r:id="rId10"/>
+    <sheet name="THEME5" sheetId="7" r:id="rId11"/>
+    <sheet name="WWMSP5" sheetId="16" r:id="rId12"/>
+    <sheet name="JPPLAWAC" sheetId="12" r:id="rId13"/>
+    <sheet name="UWA" sheetId="15" r:id="rId14"/>
+    <sheet name="BMTBNA" sheetId="17" r:id="rId15"/>
+    <sheet name="FPA_BMT" sheetId="14" r:id="rId16"/>
+    <sheet name="WC_BMT" sheetId="13" r:id="rId17"/>
+    <sheet name="Information" sheetId="6" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'MASTER KEY'!$A$1:$J$285</definedName>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3586" uniqueCount="1426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3822" uniqueCount="1649">
   <si>
     <t>Units</t>
   </si>
@@ -4377,6 +4378,675 @@
       </rPr>
       <t>N)</t>
     </r>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        // General</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        //</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_ALBIDO,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_AREA,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_BOOLEAN,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_CAPACITY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_COEFFICIENT,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_CONCENTRATION,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_COLOR,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_CONSUMPTION,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_DEMAND,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_DENSITY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_DEPTH,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_DISTANCE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_DIR,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_ELEVATION,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_EMISSIVITY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_EVAPORATION,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_EVAPOTRANSPIRATION,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       GEN_FLOW,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_FACTOR,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_FRACTION,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_FLUX,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_HEIGHT,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_INDEX,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_INTESITY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_LAT,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_LENGTH,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_LIGHT,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_LNG,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_MOISTURE_CONTENT,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_ODOR,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_PRESSURE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_QUANTITY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_SIZE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_SOLIDS,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_SOLIDS_DISSOLVED,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_SOLIDS_SUSPENDED,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_SPD,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_TEMP,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_TIME,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_UTM,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_VELOCITY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_VELOCITY_U,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_VELOCITY_V,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_VELOCITY_W,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_VOLUME,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_WIDTH,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_X,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_Y,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEN_OTHER,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Biology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_AGE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_ANABAENA,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_BIOMASS,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_BLUE_GREEN_ALGAE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_CHLOROPHYLL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_CHLOROPHYLL_A,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_CHLOROPHYLL_B,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_CHLOROPHYLL_C,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_CHLOROPHYLL_TOTAL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_CHYTRID,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_COUNT,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_CRYPTOPHYTES,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_CYANOBACTERIA,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_DIATOMS,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_DINOFLAGELLETES,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_DREISSENA,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_FISH,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_FRESH_WATER_DIATOMS,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_GREEN_ALGAE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_INVERTEBRATES,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_MACROPHYTES,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_MARINE_DIATOMS,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_MICROCYSTIS,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_PERIPHYTON,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_PHEOPHYTIN,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_PHEOPHYTIN_A,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_PHYCOCYANINS,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_PHYTOPLANKTON,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_PHOSPHORUS,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_PLANKTON,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_PLANKTOTHRIX,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_PRODUCTIVITY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_PRODUCTIVITY_CARBON,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_PRODUCTIVITY_GROSS,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_PRODUCTIVITY_NET,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_RESPIRATION,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_SIZE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_WEIGHT,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_ZOOPLANKTON,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        BIO_OTHER,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Geography</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEO_LAND_MASK,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEO_CATEGORY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEO_RUNOFF,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEO_TEMP,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        GEO_HEIGHT,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Met</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_AIR_TEMP,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_AIR_TEMP_POT,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_AEROSOL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_CLOUD_COVER,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_EVAPORATION,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_FROST,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_ICE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_GRAUPEL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_HUM,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_LIGHT,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_OZONE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_PRESSURE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_RAD,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_RAD_LW,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_RAD_NET,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_RAD_SOLAR,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_RAIN,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_REL_HUM,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_SNOW,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_SNOW_DEPTH,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_TEMP,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_VELOCITY_U,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_VELOCITY_V,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_VELOCITY_W,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_VISIBILITY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_WIND_DIR,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_WIND_SPD,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MET_OTHER,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         NUTRIENTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_AMMONIA,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_AMMONIA_DISOLVED,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_AMMONIA_SUSPENDED,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_AMMONIA_TOTAL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_AMMONIUM,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_AMMONIUM_TOTAL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_CARBON,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITRATE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITRATE_DISOLVED,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITRATE_TOTAL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITRITE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITRITE_DISOLVED,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITRITE_TOTAL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITROGEN,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITROGEN_DISOLVED,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITROGEN_DISOLVED_INORGANIC,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITROGEN_DISOLVED_ORGANIC,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITROGEN_INORGANIC,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITROGEN_ORGANIC,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITROGEN_PARTICULATE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITROGEN_PARTICULATE_ORGANIC,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITROGEN_PARTICULATE_INORGANIC,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITROGEN_SUSPENDED,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITROGEN_SUSPENDED_ORGANIC,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITROGEN_SUSPENDED_INORGANIC,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITROGEN_TOTAL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITROGEN_TOTAL_ORGANIC,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITROGEN_TOTAL_INORGANIC,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITROUS_OXIDE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_NITROUS_OXIDE_TOTAL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_ORTHOPHOSPHATE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_ORTHOPHOSPHATE_DISSOLVED,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_ORTHOPHOSPHATE_TOTAL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_PHOSPHATE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_PHOSPHATE_DISSOLVED,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_PHOSPHATE_TOTAL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_PHOSPHORUS,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_PHOSPHORUS_DISOLVED,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_PHOSPHORUS_DISOLVED_ORGANIC,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_PHOSPHORUS_DISOLVED_INORGANIC,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_PHOSPHORUS_PARTICULATE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_PHOSPHORUS_PARTICULATE_ORGANIC,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_PHOSPHORUS_PARTICULATE_INORGANIC,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_PHOSPHORUS_SUSPENDED,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_PHOSPHORUS_SUSPENDED_ORGANIC,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_PHOSPHORUS_SUSPENDED_INORGANIC,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_PHOSPHORUS_TOTAL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_PHOSPHORUS_TOTAL_ORGANIC,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_PHOSPHORUS_TOTAL_INORGANIC,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_SEDIMENT,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_SEDIMENT_BED,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_SEDIMENT_DISOLVED,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        NUT_SEDIMENT_SUSPENDED,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Sediment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        SED_CONCENTRATION,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Wave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WAV_DIRECTION,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WAV_HEIGHT,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WAV_PERIOD,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_ABSORBANCE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_ALBIDO,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_BACTERIA,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_CONDUCTIVITY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_DENSITY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_DEPTH,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_DIR,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_DISCHARGE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_DISOLVED_OXYGEN,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_EVAPORATION,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_FLOW,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_FLUORESCENCE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_GAGE_HEIGHT,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_HARDNESS,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_HEIGHT,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_LEVEL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_PAR,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_PH,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_PRESSURE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_QUANTITY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_RETENTION_TIME,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_SALINITY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_SPD,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_TEMP,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_TRACER,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_TRANSPARENCY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_TURBIDITY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_VELOCITY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_VELOCITY_U,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_VELOCITY_V,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_VELOCITY_W,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_WIDTH,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        WTR_OTHER,</t>
   </si>
 </sst>
 </file>
@@ -4544,7 +5214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4598,6 +5268,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4914,9 +5587,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{407D1833-63F5-4230-AD16-32E9E48F56BB}">
   <dimension ref="A1:J285"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A255" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C276" sqref="C276"/>
+      <selection pane="bottomLeft" activeCell="H296" sqref="H296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -10620,6 +11293,364 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B891FCC8-6932-42EA-B0A0-1A3A06F7421B}">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>373</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="B2" s="1">
+        <f>1/1000</f>
+        <v>1E-3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B933,2,TRUE)</f>
+        <v>Tidal Height</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>839</v>
+      </c>
+      <c r="B3">
+        <v>0.01</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B934,2,TRUE)</f>
+        <v>Tidal Height</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B935,2,TRUE)</f>
+        <v>Significant waveheight</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1339</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f>VLOOKUP(C5,'MASTER KEY'!$A$2:$B936,2,TRUE)</f>
+        <v>Peak wave period</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1338</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B937,2,TRUE)</f>
+        <v>Mean wave period</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1343</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B938,2,TRUE)</f>
+        <v>Peak wave direction</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1338</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B939,2,TRUE)</f>
+        <v>Mean wave period</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f>VLOOKUP(C9,'MASTER KEY'!$A$2:$B939,2,TRUE)</f>
+        <v>Depth</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B10">
+        <v>1E-3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1373</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f>VLOOKUP(C10,'MASTER KEY'!$A$2:$B940,2,TRUE)</f>
+        <v>Current velocity</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f>VLOOKUP(C11,'MASTER KEY'!$A$2:$B941,2,TRUE)</f>
+        <v>Current direction</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1399</v>
+      </c>
+      <c r="B12">
+        <v>1E-3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1373</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f>VLOOKUP(C12,'MASTER KEY'!$A$2:$B942,2,TRUE)</f>
+        <v>Current velocity</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f>VLOOKUP(C13,'MASTER KEY'!$A$2:$B943,2,TRUE)</f>
+        <v>Current direction</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f>VLOOKUP(C14,'MASTER KEY'!$A$2:$B944,2,TRUE)</f>
+        <v>HEADING</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>939</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f>VLOOKUP(C15,'MASTER KEY'!$A$2:$B945,2,TRUE)</f>
+        <v>Pitch</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f>VLOOKUP(C16,'MASTER KEY'!$A$2:$B946,2,TRUE)</f>
+        <v>ROLL</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f>VLOOKUP(C17,'MASTER KEY'!$A$2:$B947,2,TRUE)</f>
+        <v>Temperature</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>494</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <f>VLOOKUP(C18,'MASTER KEY'!$A$2:$B948,2,TRUE)</f>
+        <v>Tidal Height</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1343</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <f>VLOOKUP(C19,'MASTER KEY'!$A$2:$B949,2,TRUE)</f>
+        <v>Peak wave direction</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1345</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <f>VLOOKUP(C20,'MASTER KEY'!$A$2:$B950,2,TRUE)</f>
+        <v>Mean wave direction</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D21" s="1" t="e">
+        <f>VLOOKUP(C21,'MASTER KEY'!$A$2:$B951,2,TRUE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D22" s="1" t="e">
+        <f>VLOOKUP(C22,'MASTER KEY'!$A$2:$B952,2,TRUE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>1419</v>
+      </c>
+      <c r="D23" s="1" t="e">
+        <f>VLOOKUP(C23,'MASTER KEY'!$A$2:$B953,2,TRUE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D24" s="1" t="e">
+        <f>VLOOKUP(C24,'MASTER KEY'!$A$2:$B954,2,TRUE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62FB3BD-BFAE-4A57-9EA4-1FE2FC61EC11}">
   <dimension ref="A1:D54"/>
   <sheetViews>
@@ -11448,7 +12479,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F92A6A-D5C0-43D4-A5FF-410FD3BDDAB2}">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -11720,7 +12751,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82049BCF-AB42-45E7-B0B9-F1876ACDD291}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -12023,7 +13054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B95F86-EBEF-4D20-B901-BEE7601EB736}">
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -12228,7 +13259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC805144-0550-45A7-AE1E-79020EDA04F0}">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -12397,7 +13428,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B5E73C-E323-4B74-9F14-922929B990A3}">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -12532,7 +13563,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14A182F4-44FD-43F6-93A9-99BB7F63199E}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -12651,7 +13682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B6692B-9920-4E77-9D5B-6B101F30D414}">
   <dimension ref="A3:A5"/>
   <sheetViews>
@@ -12680,6 +13711,1204 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90053AC-E970-C241-A8E9-106E6E17DECD}">
+  <dimension ref="A1:A236"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>1451</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>1463</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>1474</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>1482</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>1486</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>1491</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>1613</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>1629</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>1631</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>1639</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>1648</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3327CA4D-663D-443F-80DC-1A1E539BD38E}">
   <dimension ref="A1:F270"/>
   <sheetViews>
@@ -18664,7 +20893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E5E19A-8269-4B75-9F84-B2CE294BEEE9}">
   <dimension ref="A1:E105"/>
   <sheetViews>
@@ -20593,7 +22822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56AD1D0B-ECF7-4309-8F1E-D29C7C0B24A7}">
   <dimension ref="A1:G73"/>
   <sheetViews>
@@ -21751,7 +23980,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F3350C-7CCF-4B4A-9A9A-12B7BE46DA49}">
   <dimension ref="A1:D23"/>
   <sheetViews>
@@ -22115,7 +24344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00F53C71-6126-496F-BF12-2421C1B2ABC6}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -22760,7 +24989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCC28208-034A-46AB-8361-1B4BBD0AB7D3}">
   <dimension ref="A1:D23"/>
   <sheetViews>
@@ -23124,7 +25353,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618D0C58-8C8E-440E-A497-ABAD71259CF4}">
   <dimension ref="A1:D35"/>
   <sheetViews>
@@ -23672,362 +25901,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B891FCC8-6932-42EA-B0A0-1A3A06F7421B}">
-  <dimension ref="A1:D24"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>373</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>496</v>
-      </c>
-      <c r="B2" s="1">
-        <f>1/1000</f>
-        <v>1E-3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B933,2,TRUE)</f>
-        <v>Tidal Height</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>839</v>
-      </c>
-      <c r="B3">
-        <v>0.01</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B934,2,TRUE)</f>
-        <v>Tidal Height</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>1379</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1317</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B935,2,TRUE)</f>
-        <v>Significant waveheight</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
-        <v>1380</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>1339</v>
-      </c>
-      <c r="D5" s="1" t="str">
-        <f>VLOOKUP(C5,'MASTER KEY'!$A$2:$B936,2,TRUE)</f>
-        <v>Peak wave period</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
-        <v>1381</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>1338</v>
-      </c>
-      <c r="D6" s="1" t="str">
-        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B937,2,TRUE)</f>
-        <v>Mean wave period</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
-        <v>1382</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>1343</v>
-      </c>
-      <c r="D7" s="1" t="str">
-        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B938,2,TRUE)</f>
-        <v>Peak wave direction</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
-        <v>1418</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>1338</v>
-      </c>
-      <c r="D8" s="1" t="str">
-        <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B939,2,TRUE)</f>
-        <v>Mean wave period</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D9" s="1" t="str">
-        <f>VLOOKUP(C9,'MASTER KEY'!$A$2:$B939,2,TRUE)</f>
-        <v>Depth</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>1397</v>
-      </c>
-      <c r="B10">
-        <v>1E-3</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>1373</v>
-      </c>
-      <c r="D10" s="1" t="str">
-        <f>VLOOKUP(C10,'MASTER KEY'!$A$2:$B940,2,TRUE)</f>
-        <v>Current velocity</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>1398</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>1402</v>
-      </c>
-      <c r="D11" s="1" t="str">
-        <f>VLOOKUP(C11,'MASTER KEY'!$A$2:$B941,2,TRUE)</f>
-        <v>Current direction</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>1399</v>
-      </c>
-      <c r="B12">
-        <v>1E-3</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>1373</v>
-      </c>
-      <c r="D12" s="1" t="str">
-        <f>VLOOKUP(C12,'MASTER KEY'!$A$2:$B942,2,TRUE)</f>
-        <v>Current velocity</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>1382</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>1402</v>
-      </c>
-      <c r="D13" s="1" t="str">
-        <f>VLOOKUP(C13,'MASTER KEY'!$A$2:$B943,2,TRUE)</f>
-        <v>Current direction</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>1405</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>934</v>
-      </c>
-      <c r="D14" s="1" t="str">
-        <f>VLOOKUP(C14,'MASTER KEY'!$A$2:$B944,2,TRUE)</f>
-        <v>HEADING</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>939</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>940</v>
-      </c>
-      <c r="D15" s="1" t="str">
-        <f>VLOOKUP(C15,'MASTER KEY'!$A$2:$B945,2,TRUE)</f>
-        <v>Pitch</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>1406</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>946</v>
-      </c>
-      <c r="D16" s="1" t="str">
-        <f>VLOOKUP(C16,'MASTER KEY'!$A$2:$B946,2,TRUE)</f>
-        <v>ROLL</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="D17" s="1" t="str">
-        <f>VLOOKUP(C17,'MASTER KEY'!$A$2:$B947,2,TRUE)</f>
-        <v>Temperature</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>1407</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="D18" s="1" t="str">
-        <f>VLOOKUP(C18,'MASTER KEY'!$A$2:$B948,2,TRUE)</f>
-        <v>Tidal Height</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>1408</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>1343</v>
-      </c>
-      <c r="D19" s="1" t="str">
-        <f>VLOOKUP(C19,'MASTER KEY'!$A$2:$B949,2,TRUE)</f>
-        <v>Peak wave direction</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>1409</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>1345</v>
-      </c>
-      <c r="D20" s="1" t="str">
-        <f>VLOOKUP(C20,'MASTER KEY'!$A$2:$B950,2,TRUE)</f>
-        <v>Mean wave direction</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
-        <v>1326</v>
-      </c>
-      <c r="D21" s="1" t="e">
-        <f>VLOOKUP(C21,'MASTER KEY'!$A$2:$B951,2,TRUE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
-        <v>1410</v>
-      </c>
-      <c r="D22" s="1" t="e">
-        <f>VLOOKUP(C22,'MASTER KEY'!$A$2:$B952,2,TRUE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>1419</v>
-      </c>
-      <c r="D23" s="1" t="e">
-        <f>VLOOKUP(C23,'MASTER KEY'!$A$2:$B953,2,TRUE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
-        <v>1420</v>
-      </c>
-      <c r="D24" s="1" t="e">
-        <f>VLOOKUP(C24,'MASTER KEY'!$A$2:$B954,2,TRUE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated key and scripts
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -1,43 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00101765\AED Dropbox\AED_Cockburn_db\CSIEM\Data\Sherry\csiem-data\data-governance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\csiem-data\data-governance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D06A06-9BF7-4B44-81D9-C4F4E2F7CA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B6E0C2-F745-48E2-B60C-3DEC7CB9AD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="5430" windowWidth="35190" windowHeight="15450" tabRatio="841" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="841" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER KEY" sheetId="1" r:id="rId1"/>
-    <sheet name="SentientHubs" sheetId="18" r:id="rId2"/>
-    <sheet name="Model_TFV" sheetId="5" r:id="rId3"/>
-    <sheet name="THEME5MET" sheetId="19" r:id="rId4"/>
-    <sheet name="MAFRL" sheetId="8" r:id="rId5"/>
-    <sheet name="IMOSBGC" sheetId="9" r:id="rId6"/>
-    <sheet name="IMOSPROFILE" sheetId="10" r:id="rId7"/>
-    <sheet name="DWER" sheetId="2" r:id="rId8"/>
-    <sheet name="DWERMOORING" sheetId="11" r:id="rId9"/>
-    <sheet name="BOM" sheetId="3" r:id="rId10"/>
-    <sheet name="DOT" sheetId="4" r:id="rId11"/>
-    <sheet name="THEME5" sheetId="7" r:id="rId12"/>
-    <sheet name="WWMSP5" sheetId="16" r:id="rId13"/>
-    <sheet name="WWMSP2" sheetId="20" r:id="rId14"/>
-    <sheet name="JPPLAWAC" sheetId="12" r:id="rId15"/>
-    <sheet name="UWA" sheetId="15" r:id="rId16"/>
-    <sheet name="BMTBNA" sheetId="17" r:id="rId17"/>
-    <sheet name="FPA_BMT" sheetId="14" r:id="rId18"/>
-    <sheet name="WC_BMT" sheetId="13" r:id="rId19"/>
-    <sheet name="Information" sheetId="6" r:id="rId20"/>
+    <sheet name="THEME2LIGHT" sheetId="21" r:id="rId2"/>
+    <sheet name="SentientHubs" sheetId="18" r:id="rId3"/>
+    <sheet name="Model_TFV" sheetId="5" r:id="rId4"/>
+    <sheet name="THEME5MET" sheetId="19" r:id="rId5"/>
+    <sheet name="MAFRL" sheetId="8" r:id="rId6"/>
+    <sheet name="IMOSBGC" sheetId="9" r:id="rId7"/>
+    <sheet name="IMOSPROFILE" sheetId="10" r:id="rId8"/>
+    <sheet name="DWER" sheetId="2" r:id="rId9"/>
+    <sheet name="DWERMOORING" sheetId="11" r:id="rId10"/>
+    <sheet name="BOM" sheetId="3" r:id="rId11"/>
+    <sheet name="DOT" sheetId="4" r:id="rId12"/>
+    <sheet name="THEME5" sheetId="7" r:id="rId13"/>
+    <sheet name="WWMSP5" sheetId="16" r:id="rId14"/>
+    <sheet name="WWMSP2" sheetId="20" r:id="rId15"/>
+    <sheet name="JPPLAWAC" sheetId="12" r:id="rId16"/>
+    <sheet name="UWA" sheetId="15" r:id="rId17"/>
+    <sheet name="BMTBNA" sheetId="17" r:id="rId18"/>
+    <sheet name="FPA_BMT" sheetId="14" r:id="rId19"/>
+    <sheet name="WC_BMT" sheetId="13" r:id="rId20"/>
+    <sheet name="Information" sheetId="6" r:id="rId21"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'MASTER KEY'!$A$1:$J$318</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -774,7 +775,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4151" uniqueCount="1786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4207" uniqueCount="1791">
   <si>
     <t>Units</t>
   </si>
@@ -6220,6 +6221,42 @@
   </si>
   <si>
     <t>assuming this 'PAR STD' = PAR standard?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Internal temperature (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C)</t>
+    </r>
+  </si>
+  <si>
+    <t>var00319</t>
+  </si>
+  <si>
+    <t>Total M Par day</t>
+  </si>
+  <si>
+    <t>mol/m2/day</t>
+  </si>
+  <si>
+    <t>Ignore</t>
   </si>
 </sst>
 </file>
@@ -6828,11 +6865,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J318"/>
+  <dimension ref="A1:J319"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A286" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A297" sqref="A297"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A273" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H300" sqref="H300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13064,6 +13101,20 @@
         <v>1784</v>
       </c>
     </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A319" s="30" t="s">
+        <v>1787</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>1788</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>1789</v>
+      </c>
+      <c r="E319" s="1" t="s">
+        <v>1784</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J318" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -13074,6 +13125,370 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>845</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B931,2,TRUE)</f>
+        <v>Air Temperature</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>846</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B932,2,TRUE)</f>
+        <v>Temperature</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>847</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B933,2,TRUE)</f>
+        <v>Turbidity</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>354</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f>VLOOKUP(C5,'MASTER KEY'!$A$2:$B934,2,TRUE)</f>
+        <v>Salinity</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>848</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B935,2,TRUE)</f>
+        <v>Oxygen</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>849</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B936,2,TRUE)</f>
+        <v>O2 Saturation</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>850</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B937,2,TRUE)</f>
+        <v>pH</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>851</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f>VLOOKUP(C9,'MASTER KEY'!$A$2:$B938,2,TRUE)</f>
+        <v>Depth</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>852</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f>VLOOKUP(C10,'MASTER KEY'!$A$2:$B939,2,TRUE)</f>
+        <v>Tilt</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>853</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f>VLOOKUP(C11,'MASTER KEY'!$A$2:$B940,2,TRUE)</f>
+        <v>WL - 410</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>854</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f>VLOOKUP(C12,'MASTER KEY'!$A$2:$B941,2,TRUE)</f>
+        <v>WL - 440</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>855</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f>VLOOKUP(C13,'MASTER KEY'!$A$2:$B942,2,TRUE)</f>
+        <v>WL - 490</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>856</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f>VLOOKUP(C14,'MASTER KEY'!$A$2:$B943,2,TRUE)</f>
+        <v>WL - 510</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>857</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f>VLOOKUP(C15,'MASTER KEY'!$A$2:$B944,2,TRUE)</f>
+        <v>WL - 550</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>858</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f>VLOOKUP(C16,'MASTER KEY'!$A$2:$B945,2,TRUE)</f>
+        <v>WL - 590</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>859</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f>VLOOKUP(C17,'MASTER KEY'!$A$2:$B946,2,TRUE)</f>
+        <v>WL - 635</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>860</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <f>VLOOKUP(C18,'MASTER KEY'!$A$2:$B947,2,TRUE)</f>
+        <v>WL - 660</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>861</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <f>VLOOKUP(C19,'MASTER KEY'!$A$2:$B948,2,TRUE)</f>
+        <v>WL - 700</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>862</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="D20" s="1" t="str">
+        <f>VLOOKUP(C20,'MASTER KEY'!$A$2:$B949,2,TRUE)</f>
+        <v>PAR</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>863</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="D21" s="1" t="str">
+        <f>VLOOKUP(C21,'MASTER KEY'!$A$2:$B950,2,TRUE)</f>
+        <v>PAR</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>864</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D22" s="1" t="str">
+        <f>VLOOKUP(C22,'MASTER KEY'!$A$2:$B951,2,TRUE)</f>
+        <v>Conductivity</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>865</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D23" s="1" t="str">
+        <f>VLOOKUP(C23,'MASTER KEY'!$A$2:$B952,2,TRUE)</f>
+        <v>O2 Saturation</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D35"/>
   <sheetViews>
@@ -13624,7 +14039,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
@@ -14006,7 +14421,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D54"/>
   <sheetViews>
@@ -14835,7 +15250,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -15107,7 +15522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBC0BB9-8F45-4117-8EDC-41406E638950}">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -15511,7 +15926,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -15814,11 +16229,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -16037,7 +16452,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -16206,7 +16621,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -16341,7 +16756,400 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD7D7559-1643-4FF9-B8E5-4B46BD5C53B5}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D2" t="str">
+        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B928,2,TRUE)</f>
+        <v>Temperature</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>901</v>
+      </c>
+      <c r="D3" t="str">
+        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B929,2,TRUE)</f>
+        <v>Tilt</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1790</v>
+      </c>
+      <c r="D4" t="e">
+        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B930,2,TRUE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>1722</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="D5" t="str">
+        <f>VLOOKUP(C5,'MASTER KEY'!$A$2:$B931,2,TRUE)</f>
+        <v>PAR</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>1743</v>
+      </c>
+      <c r="D6" t="str">
+        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B933,2,TRUE)</f>
+        <v>WL - 398µW</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>1744</v>
+      </c>
+      <c r="D7" t="str">
+        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B934,2,TRUE)</f>
+        <v>WL - 448µW</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>1745</v>
+      </c>
+      <c r="D8" t="str">
+        <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B935,2,TRUE)</f>
+        <v>WL - 470µW</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>1746</v>
+      </c>
+      <c r="D9" t="str">
+        <f>VLOOKUP(C9,'MASTER KEY'!$A$2:$B936,2,TRUE)</f>
+        <v>WL - 524µW</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>1727</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>1747</v>
+      </c>
+      <c r="D10" t="str">
+        <f>VLOOKUP(C10,'MASTER KEY'!$A$2:$B937,2,TRUE)</f>
+        <v>WL - 554µW</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>1728</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>1748</v>
+      </c>
+      <c r="D11" t="str">
+        <f>VLOOKUP(C11,'MASTER KEY'!$A$2:$B938,2,TRUE)</f>
+        <v>WL - 590µW</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>1729</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>1749</v>
+      </c>
+      <c r="D12" t="str">
+        <f>VLOOKUP(C12,'MASTER KEY'!$A$2:$B939,2,TRUE)</f>
+        <v>WL - 628µW</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>1730</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>1750</v>
+      </c>
+      <c r="D13" t="str">
+        <f>VLOOKUP(C13,'MASTER KEY'!$A$2:$B940,2,TRUE)</f>
+        <v>WL - 656µW</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>1751</v>
+      </c>
+      <c r="D14" t="str">
+        <f>VLOOKUP(C14,'MASTER KEY'!$A$2:$B941,2,TRUE)</f>
+        <v>WL - 699µW</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>1770</v>
+      </c>
+      <c r="D15" t="str">
+        <f>VLOOKUP(C15,'MASTER KEY'!$A$2:$B942,2,TRUE)</f>
+        <v>WL - 398µmol</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>1733</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>1771</v>
+      </c>
+      <c r="D16" t="str">
+        <f>VLOOKUP(C16,'MASTER KEY'!$A$2:$B943,2,TRUE)</f>
+        <v>WL - 448µmol</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>1734</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>1772</v>
+      </c>
+      <c r="D17" t="str">
+        <f>VLOOKUP(C17,'MASTER KEY'!$A$2:$B944,2,TRUE)</f>
+        <v>WL - 470µmol</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D18" t="str">
+        <f>VLOOKUP(C18,'MASTER KEY'!$A$2:$B945,2,TRUE)</f>
+        <v>WL - 524µmol</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>1736</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>1774</v>
+      </c>
+      <c r="D19" t="str">
+        <f>VLOOKUP(C19,'MASTER KEY'!$A$2:$B946,2,TRUE)</f>
+        <v>WL - 554µmol</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>1737</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>1775</v>
+      </c>
+      <c r="D20" t="str">
+        <f>VLOOKUP(C20,'MASTER KEY'!$A$2:$B947,2,TRUE)</f>
+        <v>WL - 590µmol</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>1776</v>
+      </c>
+      <c r="D21" t="str">
+        <f>VLOOKUP(C21,'MASTER KEY'!$A$2:$B948,2,TRUE)</f>
+        <v>WL - 628µmol</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>1739</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>1777</v>
+      </c>
+      <c r="D22" t="str">
+        <f>VLOOKUP(C22,'MASTER KEY'!$A$2:$B949,2,TRUE)</f>
+        <v>WL - 656µmol</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>1740</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>1778</v>
+      </c>
+      <c r="D23" t="str">
+        <f>VLOOKUP(C23,'MASTER KEY'!$A$2:$B950,2,TRUE)</f>
+        <v>WL - 699µmol</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>1780</v>
+      </c>
+      <c r="D24" t="str">
+        <f>VLOOKUP(C24,'MASTER KEY'!$A$2:$B951,2,TRUE)</f>
+        <v>Total Par day</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>1787</v>
+      </c>
+      <c r="D25" t="str">
+        <f>VLOOKUP(C25,'MASTER KEY'!$A$2:$B952,2,TRUE)</f>
+        <v>Total M Par day</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -16460,7 +17268,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A3:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>837</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A236"/>
   <sheetViews>
@@ -17658,35 +18494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A3:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="52.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>837</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F284"/>
   <sheetViews>
@@ -23954,12 +24762,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5261A16-8B5D-4B5D-ADA5-57BB15B52747}">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24269,10 +25077,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E105"/>
   <sheetViews>
@@ -26201,7 +27010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G73"/>
   <sheetViews>
@@ -27359,7 +28168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
@@ -27723,7 +28532,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
@@ -28366,368 +29175,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>845</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B931,2,TRUE)</f>
-        <v>Air Temperature</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>846</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B932,2,TRUE)</f>
-        <v>Temperature</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>847</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B933,2,TRUE)</f>
-        <v>Turbidity</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>354</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D5" s="1" t="str">
-        <f>VLOOKUP(C5,'MASTER KEY'!$A$2:$B934,2,TRUE)</f>
-        <v>Salinity</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>848</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D6" s="1" t="str">
-        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B935,2,TRUE)</f>
-        <v>Oxygen</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>849</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="D7" s="1" t="str">
-        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B936,2,TRUE)</f>
-        <v>O2 Saturation</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>850</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="D8" s="1" t="str">
-        <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B937,2,TRUE)</f>
-        <v>pH</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>851</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D9" s="1" t="str">
-        <f>VLOOKUP(C9,'MASTER KEY'!$A$2:$B938,2,TRUE)</f>
-        <v>Depth</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>852</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>901</v>
-      </c>
-      <c r="D10" s="1" t="str">
-        <f>VLOOKUP(C10,'MASTER KEY'!$A$2:$B939,2,TRUE)</f>
-        <v>Tilt</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>853</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>902</v>
-      </c>
-      <c r="D11" s="1" t="str">
-        <f>VLOOKUP(C11,'MASTER KEY'!$A$2:$B940,2,TRUE)</f>
-        <v>WL - 410</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>854</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>903</v>
-      </c>
-      <c r="D12" s="1" t="str">
-        <f>VLOOKUP(C12,'MASTER KEY'!$A$2:$B941,2,TRUE)</f>
-        <v>WL - 440</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>855</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>904</v>
-      </c>
-      <c r="D13" s="1" t="str">
-        <f>VLOOKUP(C13,'MASTER KEY'!$A$2:$B942,2,TRUE)</f>
-        <v>WL - 490</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>856</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>905</v>
-      </c>
-      <c r="D14" s="1" t="str">
-        <f>VLOOKUP(C14,'MASTER KEY'!$A$2:$B943,2,TRUE)</f>
-        <v>WL - 510</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>857</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>906</v>
-      </c>
-      <c r="D15" s="1" t="str">
-        <f>VLOOKUP(C15,'MASTER KEY'!$A$2:$B944,2,TRUE)</f>
-        <v>WL - 550</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>858</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>907</v>
-      </c>
-      <c r="D16" s="1" t="str">
-        <f>VLOOKUP(C16,'MASTER KEY'!$A$2:$B945,2,TRUE)</f>
-        <v>WL - 590</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>859</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>908</v>
-      </c>
-      <c r="D17" s="1" t="str">
-        <f>VLOOKUP(C17,'MASTER KEY'!$A$2:$B946,2,TRUE)</f>
-        <v>WL - 635</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>860</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>909</v>
-      </c>
-      <c r="D18" s="1" t="str">
-        <f>VLOOKUP(C18,'MASTER KEY'!$A$2:$B947,2,TRUE)</f>
-        <v>WL - 660</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>861</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>910</v>
-      </c>
-      <c r="D19" s="1" t="str">
-        <f>VLOOKUP(C19,'MASTER KEY'!$A$2:$B948,2,TRUE)</f>
-        <v>WL - 700</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>862</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>898</v>
-      </c>
-      <c r="D20" s="1" t="str">
-        <f>VLOOKUP(C20,'MASTER KEY'!$A$2:$B949,2,TRUE)</f>
-        <v>PAR</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>863</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>898</v>
-      </c>
-      <c r="D21" s="1" t="str">
-        <f>VLOOKUP(C21,'MASTER KEY'!$A$2:$B950,2,TRUE)</f>
-        <v>PAR</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>864</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="D22" s="1" t="str">
-        <f>VLOOKUP(C22,'MASTER KEY'!$A$2:$B951,2,TRUE)</f>
-        <v>Conductivity</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>865</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="D23" s="1" t="str">
-        <f>VLOOKUP(C23,'MASTER KEY'!$A$2:$B952,2,TRUE)</f>
-        <v>O2 Saturation</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update WWM variables in variable_key
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\csiem-data\data-governance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\csiem-data\data-governance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B6E0C2-F745-48E2-B60C-3DEC7CB9AD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="841" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="841" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER KEY" sheetId="1" r:id="rId1"/>
@@ -26,19 +25,23 @@
     <sheet name="BOM" sheetId="3" r:id="rId11"/>
     <sheet name="DOT" sheetId="4" r:id="rId12"/>
     <sheet name="THEME5" sheetId="7" r:id="rId13"/>
-    <sheet name="WWMSP5" sheetId="16" r:id="rId14"/>
-    <sheet name="WWMSP2" sheetId="20" r:id="rId15"/>
-    <sheet name="JPPLAWAC" sheetId="12" r:id="rId16"/>
-    <sheet name="UWA" sheetId="15" r:id="rId17"/>
-    <sheet name="BMTBNA" sheetId="17" r:id="rId18"/>
-    <sheet name="FPA_BMT" sheetId="14" r:id="rId19"/>
-    <sheet name="WC_BMT" sheetId="13" r:id="rId20"/>
-    <sheet name="Information" sheetId="6" r:id="rId21"/>
+    <sheet name="WWM" sheetId="22" r:id="rId14"/>
+    <sheet name="WWMSP5" sheetId="16" r:id="rId15"/>
+    <sheet name="WWMSP2" sheetId="20" r:id="rId16"/>
+    <sheet name="JPPLAWAC" sheetId="12" r:id="rId17"/>
+    <sheet name="UWA" sheetId="15" r:id="rId18"/>
+    <sheet name="BMTBNA" sheetId="17" r:id="rId19"/>
+    <sheet name="FPA_BMT" sheetId="14" r:id="rId20"/>
+    <sheet name="WC_BMT" sheetId="13" r:id="rId21"/>
+    <sheet name="Information" sheetId="6" r:id="rId22"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId23"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'MASTER KEY'!$A$1:$J$318</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,12 +62,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Peisheng Huang</author>
   </authors>
   <commentList>
-    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -88,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B24" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -112,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B46" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="B46" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -136,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B69" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="B69" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -160,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B78" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="B78" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -184,7 +187,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B87" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="B87" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -208,7 +211,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B89" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="B89" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -232,7 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B90" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="B90" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -256,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B92" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="B92" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -280,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B93" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="B93" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -304,7 +307,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B103" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="B103" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -328,7 +331,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C130" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="C130" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -352,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D130" authorId="0" shapeId="0" xr:uid="{6292DC12-5EE5-42A1-9F81-DF16A7AF48DF}">
+    <comment ref="D130" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -376,7 +379,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C153" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="C153" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -400,7 +403,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B181" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="B181" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -424,7 +427,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B184" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="B184" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -448,7 +451,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B201" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="B201" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -472,7 +475,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B205" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="B205" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -496,7 +499,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B211" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="B211" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -520,7 +523,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B213" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="B213" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -544,7 +547,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B215" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="B215" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -568,7 +571,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B217" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
+    <comment ref="B217" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -592,7 +595,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B268" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+    <comment ref="B268" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -616,7 +619,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B272" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
+    <comment ref="B272" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -640,7 +643,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C287" authorId="0" shapeId="0" xr:uid="{A74E28BE-96D5-4ACF-B30F-D0AFB8E69778}">
+    <comment ref="C287" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -664,7 +667,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D287" authorId="0" shapeId="0" xr:uid="{6BD8EECE-B305-4CAE-BC9C-970FB38528C1}">
+    <comment ref="D287" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -688,7 +691,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E287" authorId="0" shapeId="0" xr:uid="{01E1734E-5A27-4C51-8374-25F9A2B941E0}">
+    <comment ref="E287" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -717,12 +720,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Peisheng Huang</author>
   </authors>
   <commentList>
-    <comment ref="C272" authorId="0" shapeId="0" xr:uid="{F58B7081-2000-4075-A493-0BDDA661698B}">
+    <comment ref="C272" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -746,7 +749,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E272" authorId="0" shapeId="0" xr:uid="{DC8D6C02-CC39-45AF-91CA-8D1A427F00C6}">
+    <comment ref="E272" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -775,7 +778,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4207" uniqueCount="1791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4219" uniqueCount="1796">
   <si>
     <t>Units</t>
   </si>
@@ -6258,11 +6261,26 @@
   <si>
     <t>Ignore</t>
   </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>wave direction</t>
+  </si>
+  <si>
+    <t>TPP</t>
+  </si>
+  <si>
+    <t>wave period</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6568,6 +6586,2442 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="MASTER KEY"/>
+      <sheetName val="SentientHubs"/>
+      <sheetName val="Model_TFV"/>
+      <sheetName val="THEME5MET"/>
+      <sheetName val="MAFRL"/>
+      <sheetName val="IMOSBGC"/>
+      <sheetName val="IMOSPROFILE"/>
+      <sheetName val="DWER"/>
+      <sheetName val="DWERMOORING"/>
+      <sheetName val="BOM"/>
+      <sheetName val="WWM"/>
+      <sheetName val="DOT"/>
+      <sheetName val="THEME5"/>
+      <sheetName val="WWMSP5"/>
+      <sheetName val="JPPLAWAC"/>
+      <sheetName val="UWA"/>
+      <sheetName val="BMTBNA"/>
+      <sheetName val="FPA_BMT"/>
+      <sheetName val="WC_BMT"/>
+      <sheetName val="Information"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>var00001</v>
+          </cell>
+          <cell r="B2" t="str">
+            <v>E coli</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>var00002</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>Enterococci</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>var00003</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>TN:TP</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>var00004</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>Organic Nitrogen</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>var00005</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v>Organic Phosphorus</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>var00006</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v>Salinity</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>var00007</v>
+          </cell>
+          <cell r="B8" t="str">
+            <v>Temperature</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>var00008</v>
+          </cell>
+          <cell r="B9" t="str">
+            <v>Depth</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>var00009</v>
+          </cell>
+          <cell r="B10" t="str">
+            <v>Total Nitrogen</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>var00010</v>
+          </cell>
+          <cell r="B11" t="str">
+            <v>Total Phosphorus</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>var00011</v>
+          </cell>
+          <cell r="B12" t="str">
+            <v>Total Organic Carbon</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>var00012</v>
+          </cell>
+          <cell r="B13" t="str">
+            <v>Total Suspended Solids</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>var00013</v>
+          </cell>
+          <cell r="B14" t="str">
+            <v>Turbidity</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>var00014</v>
+          </cell>
+          <cell r="B15" t="str">
+            <v>Chlorophyll-a</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>var00015</v>
+          </cell>
+          <cell r="B16" t="str">
+            <v>Ruppia Biomass</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>var00016</v>
+          </cell>
+          <cell r="B17" t="str">
+            <v>Suspended Solids #1</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>var00017</v>
+          </cell>
+          <cell r="B18" t="str">
+            <v>Sediment Mass (SS1)</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>var00018</v>
+          </cell>
+          <cell r="B19" t="str">
+            <v>Suspended Solids #2</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>var00019</v>
+          </cell>
+          <cell r="B20" t="str">
+            <v>Sediment Mass (SS2)</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>var00020</v>
+          </cell>
+          <cell r="B21" t="str">
+            <v>Suspended Solids #3</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>var00021</v>
+          </cell>
+          <cell r="B22" t="str">
+            <v>Sediment Mass (SS3)</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>var00022</v>
+          </cell>
+          <cell r="B23" t="str">
+            <v>Water Age</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24" t="str">
+            <v>var00023</v>
+          </cell>
+          <cell r="B24" t="str">
+            <v>Oxygen</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25" t="str">
+            <v>var00024</v>
+          </cell>
+          <cell r="B25" t="str">
+            <v>Reactive Silica</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26" t="str">
+            <v>var00025</v>
+          </cell>
+          <cell r="B26" t="str">
+            <v>Ammonium</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27" t="str">
+            <v>var00026</v>
+          </cell>
+          <cell r="B27" t="str">
+            <v>Nitrate</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28" t="str">
+            <v>var00027</v>
+          </cell>
+          <cell r="B28" t="str">
+            <v>Filterable Reactive Phosphate</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29" t="str">
+            <v>var00028</v>
+          </cell>
+          <cell r="B29" t="str">
+            <v>Adsorped Phosphate</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30" t="str">
+            <v>var00029</v>
+          </cell>
+          <cell r="B30" t="str">
+            <v>Dissolved Organic Carbon</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31" t="str">
+            <v>var00030</v>
+          </cell>
+          <cell r="B31" t="str">
+            <v>Dissolved Organic Carbon (refractory)</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32" t="str">
+            <v>var00031</v>
+          </cell>
+          <cell r="B32" t="str">
+            <v>Particulate Organic Carbon</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33" t="str">
+            <v>var00032</v>
+          </cell>
+          <cell r="B33" t="str">
+            <v>Dissolved Organic Nitrogen</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34" t="str">
+            <v>var00033</v>
+          </cell>
+          <cell r="B34" t="str">
+            <v>Particulate Organic Nitrogen</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35" t="str">
+            <v>var00034</v>
+          </cell>
+          <cell r="B35" t="str">
+            <v>Dissolved Organic Nitrogen (refractory)</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36" t="str">
+            <v>var00035</v>
+          </cell>
+          <cell r="B36" t="str">
+            <v>Dissolved Organic Phosphorus</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37" t="str">
+            <v>var00036</v>
+          </cell>
+          <cell r="B37" t="str">
+            <v>Particulate Organic Phosphorus</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38" t="str">
+            <v>var00037</v>
+          </cell>
+          <cell r="B38" t="str">
+            <v>Dissolved Organic Phosphorus (refractory)</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39" t="str">
+            <v>var00038</v>
+          </cell>
+          <cell r="B39" t="str">
+            <v>Phytoplankton Biomass (greens)</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40" t="str">
+            <v>var00039</v>
+          </cell>
+          <cell r="B40" t="str">
+            <v>Phytoplankton Biomass (crypt)</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41" t="str">
+            <v>var00040</v>
+          </cell>
+          <cell r="B41" t="str">
+            <v>Phytoplankton Biomass (diatom)</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42" t="str">
+            <v>var00041</v>
+          </cell>
+          <cell r="B42" t="str">
+            <v>Phytoplankton Biomass (dino)</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43" t="str">
+            <v>var00042</v>
+          </cell>
+          <cell r="B43" t="str">
+            <v>Filamentous Algae (floating)</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44" t="str">
+            <v>var00043</v>
+          </cell>
+          <cell r="B44" t="str">
+            <v>Filamentous Algae Nitrogen (floating)</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45" t="str">
+            <v>var00044</v>
+          </cell>
+          <cell r="B45" t="str">
+            <v>Filamentous Algae Phosphorus (floating)</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46" t="str">
+            <v>var00045</v>
+          </cell>
+          <cell r="B46" t="str">
+            <v>Filamentous Algae Biomass (total)</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47" t="str">
+            <v>var00046</v>
+          </cell>
+          <cell r="B47" t="str">
+            <v>Filamentous Algae Biomass (total)</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48" t="str">
+            <v>var00047</v>
+          </cell>
+          <cell r="B48" t="str">
+            <v>Filamentous Algae Biomass (total)</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49" t="str">
+            <v>var00048</v>
+          </cell>
+          <cell r="B49" t="str">
+            <v>O2 Dissolved Sediment Flux</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50" t="str">
+            <v>var00049</v>
+          </cell>
+          <cell r="B50" t="str">
+            <v>DIC Dissolved Sediment Flux</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51" t="str">
+            <v>var00050</v>
+          </cell>
+          <cell r="B51" t="str">
+            <v>NH4 Dissolved Sediment Flux</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52" t="str">
+            <v>var00051</v>
+          </cell>
+          <cell r="B52" t="str">
+            <v>NO3 Dissolved Sediment Flux</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53" t="str">
+            <v>var00052</v>
+          </cell>
+          <cell r="B53" t="str">
+            <v>FRP Dissolved Sediment Flux</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54" t="str">
+            <v>var00053</v>
+          </cell>
+          <cell r="B54" t="str">
+            <v>POC Dissolved Sediment Flux</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55" t="str">
+            <v>var00054</v>
+          </cell>
+          <cell r="B55" t="str">
+            <v>DOC Dissolved Sediment Flux</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56" t="str">
+            <v>var00055</v>
+          </cell>
+          <cell r="B56" t="str">
+            <v>PON Dissolved Sediment Flux</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="A57" t="str">
+            <v>var00056</v>
+          </cell>
+          <cell r="B57" t="str">
+            <v>DON Dissolved Sediment Flux</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="A58" t="str">
+            <v>var00057</v>
+          </cell>
+          <cell r="B58" t="str">
+            <v>POP Dissolved Sediment Flux</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59" t="str">
+            <v>var00058</v>
+          </cell>
+          <cell r="B59" t="str">
+            <v>DOP Dissolved Sediment Flux</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60" t="str">
+            <v>var00059</v>
+          </cell>
+          <cell r="B60" t="str">
+            <v>Photosynthetically Active Radiation</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61" t="str">
+            <v>var00060</v>
+          </cell>
+          <cell r="B61" t="str">
+            <v>Ruppia Gross Primary Productivity</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62" t="str">
+            <v>var00061</v>
+          </cell>
+          <cell r="B62" t="str">
+            <v>Ruppia Net Primary Productivity</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63" t="str">
+            <v>var00062</v>
+          </cell>
+          <cell r="B63" t="str">
+            <v>Ruppia Biomass</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64" t="str">
+            <v>var00063</v>
+          </cell>
+          <cell r="B64" t="str">
+            <v>Ruppia Leaf Area Index</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65" t="str">
+            <v>var00064</v>
+          </cell>
+          <cell r="B65" t="str">
+            <v>Ruppia Biomass (above-ground)</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66" t="str">
+            <v>var00065</v>
+          </cell>
+          <cell r="B66" t="str">
+            <v>Ruppia Biomass (below-ground)</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67" t="str">
+            <v>var00066</v>
+          </cell>
+          <cell r="B67" t="str">
+            <v>Ruppia Root Depth</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68" t="str">
+            <v>var00067</v>
+          </cell>
+          <cell r="B68" t="str">
+            <v>Ruppia O2 Injection Rate</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="A69" t="str">
+            <v>var00068</v>
+          </cell>
+          <cell r="B69" t="str">
+            <v>Sedimentation Velocity (SS1)</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="A70" t="str">
+            <v>var00069</v>
+          </cell>
+          <cell r="B70" t="str">
+            <v>Sedimentation Rate (SS1)</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="A71" t="str">
+            <v>var00070</v>
+          </cell>
+          <cell r="B71" t="str">
+            <v>Sedimentation Velocity (SS2)</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="A72" t="str">
+            <v>var00071</v>
+          </cell>
+          <cell r="B72" t="str">
+            <v>Sedimentation Rate (SS2)</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73" t="str">
+            <v>var00072</v>
+          </cell>
+          <cell r="B73" t="str">
+            <v>Sedimentation Velocity (SS3)</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74" t="str">
+            <v>var00073</v>
+          </cell>
+          <cell r="B74" t="str">
+            <v>Sedimentation Rate (SS3)</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75" t="str">
+            <v>var00074</v>
+          </cell>
+          <cell r="B75" t="str">
+            <v>Sediment Mass</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76" t="str">
+            <v>var00075</v>
+          </cell>
+          <cell r="B76" t="str">
+            <v>Critical Shear Stress</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77" t="str">
+            <v>var00076</v>
+          </cell>
+          <cell r="B77" t="str">
+            <v>Resuspension Rate</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="A78" t="str">
+            <v>var00077</v>
+          </cell>
+          <cell r="B78" t="str">
+            <v>Sediment Fraction (SS1)</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="A79" t="str">
+            <v>var00078</v>
+          </cell>
+          <cell r="B79" t="str">
+            <v>Sediment Fraction (SS2)</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="A80" t="str">
+            <v>var00079</v>
+          </cell>
+          <cell r="B80" t="str">
+            <v>Sediment Fraction (SS3)</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="A81" t="str">
+            <v>var00080</v>
+          </cell>
+          <cell r="B81" t="str">
+            <v>Sedimentation Rate (SS)</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="A82" t="str">
+            <v>var00081</v>
+          </cell>
+          <cell r="B82" t="str">
+            <v>SS Net SWI Flux</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="A83" t="str">
+            <v>var00082</v>
+          </cell>
+          <cell r="B83" t="str">
+            <v>Change in SWI Position</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84" t="str">
+            <v>var00083</v>
+          </cell>
+          <cell r="B84" t="str">
+            <v>Resuspension Rate (SS)</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="A85" t="str">
+            <v>var00084</v>
+          </cell>
+          <cell r="B85" t="str">
+            <v>Bottom Shear Stress</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="A86" t="str">
+            <v>var00085</v>
+          </cell>
+          <cell r="B86" t="str">
+            <v>O2 Saturation</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="A87" t="str">
+            <v>var00086</v>
+          </cell>
+          <cell r="B87" t="str">
+            <v>O2 Dissolved Sediment Flux</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="A88" t="str">
+            <v>var00087</v>
+          </cell>
+          <cell r="B88" t="str">
+            <v>O2 Atmospheric Flux</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="A89" t="str">
+            <v>var00088</v>
+          </cell>
+          <cell r="B89" t="str">
+            <v>O2 Dissolved Sediment Exchange Rate</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="A90" t="str">
+            <v>var00089</v>
+          </cell>
+          <cell r="B90" t="str">
+            <v>O2 Atmospheric Exchange Rate</v>
+          </cell>
+        </row>
+        <row r="91">
+          <cell r="A91" t="str">
+            <v>var00090</v>
+          </cell>
+          <cell r="B91" t="str">
+            <v>Si Dissolved Sediment Flux</v>
+          </cell>
+        </row>
+        <row r="92">
+          <cell r="A92" t="str">
+            <v>var00091</v>
+          </cell>
+          <cell r="B92" t="str">
+            <v>NH4 Dissolved Sediment Flux</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="A93" t="str">
+            <v>var00092</v>
+          </cell>
+          <cell r="B93" t="str">
+            <v>NO3 Dissolved Sediment Flux</v>
+          </cell>
+        </row>
+        <row r="94">
+          <cell r="A94" t="str">
+            <v>var00093</v>
+          </cell>
+          <cell r="B94" t="str">
+            <v>Nitrification Rate</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="A95" t="str">
+            <v>var00094</v>
+          </cell>
+          <cell r="B95" t="str">
+            <v>Denitrification Rate</v>
+          </cell>
+        </row>
+        <row r="96">
+          <cell r="A96" t="str">
+            <v>var00095</v>
+          </cell>
+          <cell r="B96" t="str">
+            <v>Annamox Rate</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="A97" t="str">
+            <v>var00096</v>
+          </cell>
+          <cell r="B97" t="str">
+            <v>DNRA Rate</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="A98" t="str">
+            <v>var00097</v>
+          </cell>
+          <cell r="B98" t="str">
+            <v>DIN Atmospheric Deposition Flux</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="A99" t="str">
+            <v>var00098</v>
+          </cell>
+          <cell r="B99" t="str">
+            <v>PIP Sedimentation Rate</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="A100" t="str">
+            <v>var00099</v>
+          </cell>
+          <cell r="B100" t="str">
+            <v>PIP Resuspension Rate</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="A101" t="str">
+            <v>var00100</v>
+          </cell>
+          <cell r="B101" t="str">
+            <v>PIP Net SWI Flux</v>
+          </cell>
+        </row>
+        <row r="102">
+          <cell r="A102" t="str">
+            <v>var00101</v>
+          </cell>
+          <cell r="B102" t="str">
+            <v>FRP Sorption Rate</v>
+          </cell>
+        </row>
+        <row r="103">
+          <cell r="A103" t="str">
+            <v>var00102</v>
+          </cell>
+          <cell r="B103" t="str">
+            <v>FRP Dissolved Sediment Flux</v>
+          </cell>
+        </row>
+        <row r="104">
+          <cell r="A104" t="str">
+            <v>var00103</v>
+          </cell>
+          <cell r="B104" t="str">
+            <v>DIP Atmospheric Deposition Flux</v>
+          </cell>
+        </row>
+        <row r="105">
+          <cell r="A105" t="str">
+            <v>var00104</v>
+          </cell>
+          <cell r="B105" t="str">
+            <v>POC Sedimentation Rate</v>
+          </cell>
+        </row>
+        <row r="106">
+          <cell r="A106" t="str">
+            <v>var00105</v>
+          </cell>
+          <cell r="B106" t="str">
+            <v>PON Sedimentation Rate</v>
+          </cell>
+        </row>
+        <row r="107">
+          <cell r="A107" t="str">
+            <v>var00106</v>
+          </cell>
+          <cell r="B107" t="str">
+            <v>POP Sedimentation Rate</v>
+          </cell>
+        </row>
+        <row r="108">
+          <cell r="A108" t="str">
+            <v>var00107</v>
+          </cell>
+          <cell r="B108" t="str">
+            <v>Sediment OM Fraction</v>
+          </cell>
+        </row>
+        <row r="109">
+          <cell r="A109" t="str">
+            <v>var00108</v>
+          </cell>
+          <cell r="B109" t="str">
+            <v>Chromophoric DOM</v>
+          </cell>
+        </row>
+        <row r="110">
+          <cell r="A110" t="str">
+            <v>var00109</v>
+          </cell>
+          <cell r="B110" t="str">
+            <v>Sediment Total Organic Carbon</v>
+          </cell>
+        </row>
+        <row r="111">
+          <cell r="A111" t="str">
+            <v>var00110</v>
+          </cell>
+          <cell r="B111" t="str">
+            <v>Sediment Total Organic Nitrogen</v>
+          </cell>
+        </row>
+        <row r="112">
+          <cell r="A112" t="str">
+            <v>var00111</v>
+          </cell>
+          <cell r="B112" t="str">
+            <v>Sediment Total Organic Phosphorus</v>
+          </cell>
+        </row>
+        <row r="113">
+          <cell r="A113" t="str">
+            <v>var00112</v>
+          </cell>
+          <cell r="B113" t="str">
+            <v>POC Net SWI Flux</v>
+          </cell>
+        </row>
+        <row r="114">
+          <cell r="A114" t="str">
+            <v>var00113</v>
+          </cell>
+          <cell r="B114" t="str">
+            <v>DOC Net SWI Flux</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="A115" t="str">
+            <v>var00114</v>
+          </cell>
+          <cell r="B115" t="str">
+            <v>PON Net SWI Flux</v>
+          </cell>
+        </row>
+        <row r="116">
+          <cell r="A116" t="str">
+            <v>var00115</v>
+          </cell>
+          <cell r="B116" t="str">
+            <v>DON Net SWI Flux</v>
+          </cell>
+        </row>
+        <row r="117">
+          <cell r="A117" t="str">
+            <v>var00116</v>
+          </cell>
+          <cell r="B117" t="str">
+            <v>POP Net SWI Flux</v>
+          </cell>
+        </row>
+        <row r="118">
+          <cell r="A118" t="str">
+            <v>var00117</v>
+          </cell>
+          <cell r="B118" t="str">
+            <v>DOP Net SWI Flux</v>
+          </cell>
+        </row>
+        <row r="119">
+          <cell r="A119" t="str">
+            <v>var00118</v>
+          </cell>
+          <cell r="B119" t="str">
+            <v>POC Resuspension Rate</v>
+          </cell>
+        </row>
+        <row r="120">
+          <cell r="A120" t="str">
+            <v>var00119</v>
+          </cell>
+          <cell r="B120" t="str">
+            <v>PON Resuspension Rate</v>
+          </cell>
+        </row>
+        <row r="121">
+          <cell r="A121" t="str">
+            <v>var00120</v>
+          </cell>
+          <cell r="B121" t="str">
+            <v>POP Resuspension Rate</v>
+          </cell>
+        </row>
+        <row r="122">
+          <cell r="A122" t="str">
+            <v>var00121</v>
+          </cell>
+          <cell r="B122" t="str">
+            <v>POC Hydrolysis Rate</v>
+          </cell>
+        </row>
+        <row r="123">
+          <cell r="A123" t="str">
+            <v>var00122</v>
+          </cell>
+          <cell r="B123" t="str">
+            <v>PON Hydrolysis Rate</v>
+          </cell>
+        </row>
+        <row r="124">
+          <cell r="A124" t="str">
+            <v>var00123</v>
+          </cell>
+          <cell r="B124" t="str">
+            <v>POP Hydrolysis Rate</v>
+          </cell>
+        </row>
+        <row r="125">
+          <cell r="A125" t="str">
+            <v>var00124</v>
+          </cell>
+          <cell r="B125" t="str">
+            <v>DOC Mineralisation Rate</v>
+          </cell>
+        </row>
+        <row r="126">
+          <cell r="A126" t="str">
+            <v>var00125</v>
+          </cell>
+          <cell r="B126" t="str">
+            <v>DON Mineralisation Rate</v>
+          </cell>
+        </row>
+        <row r="127">
+          <cell r="A127" t="str">
+            <v>var00126</v>
+          </cell>
+          <cell r="B127" t="str">
+            <v>DOP Mineralisation Rate</v>
+          </cell>
+        </row>
+        <row r="128">
+          <cell r="A128" t="str">
+            <v>var00127</v>
+          </cell>
+          <cell r="B128" t="str">
+            <v>DOC Mineralisation Rate (anaerobic)</v>
+          </cell>
+        </row>
+        <row r="129">
+          <cell r="A129" t="str">
+            <v>var00128</v>
+          </cell>
+          <cell r="B129" t="str">
+            <v>DOC Mineralisation Rate (denitrification)</v>
+          </cell>
+        </row>
+        <row r="130">
+          <cell r="A130" t="str">
+            <v>var00129</v>
+          </cell>
+          <cell r="B130" t="str">
+            <v>Wind Direction</v>
+          </cell>
+        </row>
+        <row r="131">
+          <cell r="A131" t="str">
+            <v>var00130</v>
+          </cell>
+          <cell r="B131" t="str">
+            <v>Wind Speed</v>
+          </cell>
+        </row>
+        <row r="132">
+          <cell r="A132" t="str">
+            <v>var00131</v>
+          </cell>
+          <cell r="B132" t="str">
+            <v>Chlorophyll-b</v>
+          </cell>
+        </row>
+        <row r="133">
+          <cell r="A133" t="str">
+            <v>var00132</v>
+          </cell>
+          <cell r="B133" t="str">
+            <v>Chlorophyll-c</v>
+          </cell>
+        </row>
+        <row r="134">
+          <cell r="A134" t="str">
+            <v>var00133</v>
+          </cell>
+          <cell r="B134" t="str">
+            <v>Cloud Cover</v>
+          </cell>
+        </row>
+        <row r="135">
+          <cell r="A135" t="str">
+            <v>var00134</v>
+          </cell>
+          <cell r="B135" t="str">
+            <v>Conductivity</v>
+          </cell>
+        </row>
+        <row r="136">
+          <cell r="A136" t="str">
+            <v>var00135</v>
+          </cell>
+          <cell r="B136" t="str">
+            <v>Flow Status</v>
+          </cell>
+        </row>
+        <row r="137">
+          <cell r="A137" t="str">
+            <v>var00136</v>
+          </cell>
+          <cell r="B137" t="str">
+            <v>Total TKN</v>
+          </cell>
+        </row>
+        <row r="138">
+          <cell r="A138" t="str">
+            <v>var00137</v>
+          </cell>
+          <cell r="B138" t="str">
+            <v>pH</v>
+          </cell>
+        </row>
+        <row r="139">
+          <cell r="A139" t="str">
+            <v>var00138</v>
+          </cell>
+          <cell r="B139" t="str">
+            <v>Phaeophytin a</v>
+          </cell>
+        </row>
+        <row r="140">
+          <cell r="A140" t="str">
+            <v>var00139</v>
+          </cell>
+          <cell r="B140" t="str">
+            <v>Total Alkalinity</v>
+          </cell>
+        </row>
+        <row r="141">
+          <cell r="A141" t="str">
+            <v>var00140</v>
+          </cell>
+          <cell r="B141" t="str">
+            <v>Secchi depth</v>
+          </cell>
+        </row>
+        <row r="142">
+          <cell r="A142" t="str">
+            <v>var00141</v>
+          </cell>
+          <cell r="B142" t="str">
+            <v>Tide status</v>
+          </cell>
+        </row>
+        <row r="143">
+          <cell r="A143" t="str">
+            <v>var00142</v>
+          </cell>
+          <cell r="B143" t="str">
+            <v>Max Discharge</v>
+          </cell>
+        </row>
+        <row r="144">
+          <cell r="A144" t="str">
+            <v>var00143</v>
+          </cell>
+          <cell r="B144" t="str">
+            <v>Mean Discharge</v>
+          </cell>
+        </row>
+        <row r="145">
+          <cell r="A145" t="str">
+            <v>var00144</v>
+          </cell>
+          <cell r="B145" t="str">
+            <v>Min Discharge</v>
+          </cell>
+        </row>
+        <row r="146">
+          <cell r="A146" t="str">
+            <v>var00145</v>
+          </cell>
+          <cell r="B146" t="str">
+            <v>Discharge</v>
+          </cell>
+        </row>
+        <row r="147">
+          <cell r="A147" t="str">
+            <v>var00146</v>
+          </cell>
+          <cell r="B147" t="str">
+            <v>Max Stage Height CTF</v>
+          </cell>
+        </row>
+        <row r="148">
+          <cell r="A148" t="str">
+            <v>var00147</v>
+          </cell>
+          <cell r="B148" t="str">
+            <v>Mean Stage Height CTF</v>
+          </cell>
+        </row>
+        <row r="149">
+          <cell r="A149" t="str">
+            <v>var00148</v>
+          </cell>
+          <cell r="B149" t="str">
+            <v>Min Stage Height CTF</v>
+          </cell>
+        </row>
+        <row r="150">
+          <cell r="A150" t="str">
+            <v>var00149</v>
+          </cell>
+          <cell r="B150" t="str">
+            <v>Max Stage Height</v>
+          </cell>
+        </row>
+        <row r="151">
+          <cell r="A151" t="str">
+            <v>var00150</v>
+          </cell>
+          <cell r="B151" t="str">
+            <v>Mean Stage Height</v>
+          </cell>
+        </row>
+        <row r="152">
+          <cell r="A152" t="str">
+            <v>var00151</v>
+          </cell>
+          <cell r="B152" t="str">
+            <v>Min Stage Height</v>
+          </cell>
+        </row>
+        <row r="153">
+          <cell r="A153" t="str">
+            <v>var00152</v>
+          </cell>
+          <cell r="B153" t="str">
+            <v>Precipitation</v>
+          </cell>
+        </row>
+        <row r="154">
+          <cell r="A154" t="str">
+            <v>var00153</v>
+          </cell>
+          <cell r="B154" t="str">
+            <v>Air Temperature</v>
+          </cell>
+        </row>
+        <row r="155">
+          <cell r="A155" t="str">
+            <v>var00154</v>
+          </cell>
+          <cell r="B155" t="str">
+            <v>Wet Bulb Air Temperature</v>
+          </cell>
+        </row>
+        <row r="156">
+          <cell r="A156" t="str">
+            <v>var00155</v>
+          </cell>
+          <cell r="B156" t="str">
+            <v>Dew Point Temperature</v>
+          </cell>
+        </row>
+        <row r="157">
+          <cell r="A157" t="str">
+            <v>var00156</v>
+          </cell>
+          <cell r="B157" t="str">
+            <v>Relative Humidity</v>
+          </cell>
+        </row>
+        <row r="158">
+          <cell r="A158" t="str">
+            <v>var00157</v>
+          </cell>
+          <cell r="B158" t="str">
+            <v>Max Wind Speed</v>
+          </cell>
+        </row>
+        <row r="159">
+          <cell r="A159" t="str">
+            <v>var00158</v>
+          </cell>
+          <cell r="B159" t="str">
+            <v>Cloud amount of first group in eighths</v>
+          </cell>
+        </row>
+        <row r="160">
+          <cell r="A160" t="str">
+            <v>var00159</v>
+          </cell>
+          <cell r="B160" t="str">
+            <v>Cloud height of first group</v>
+          </cell>
+        </row>
+        <row r="161">
+          <cell r="A161" t="str">
+            <v>var00160</v>
+          </cell>
+          <cell r="B161" t="str">
+            <v>Cloud amount of second group in eighths</v>
+          </cell>
+        </row>
+        <row r="162">
+          <cell r="A162" t="str">
+            <v>var00161</v>
+          </cell>
+          <cell r="B162" t="str">
+            <v>Cloud height of second group</v>
+          </cell>
+        </row>
+        <row r="163">
+          <cell r="A163" t="str">
+            <v>var00162</v>
+          </cell>
+          <cell r="B163" t="str">
+            <v>Cloud amount of third group in eighths</v>
+          </cell>
+        </row>
+        <row r="164">
+          <cell r="A164" t="str">
+            <v>var00163</v>
+          </cell>
+          <cell r="B164" t="str">
+            <v>Cloud height of third group</v>
+          </cell>
+        </row>
+        <row r="165">
+          <cell r="A165" t="str">
+            <v>var00164</v>
+          </cell>
+          <cell r="B165" t="str">
+            <v>Cloud amount of fourth group in eighths</v>
+          </cell>
+        </row>
+        <row r="166">
+          <cell r="A166" t="str">
+            <v>var00165</v>
+          </cell>
+          <cell r="B166" t="str">
+            <v>Cloud height of fourth group</v>
+          </cell>
+        </row>
+        <row r="167">
+          <cell r="A167" t="str">
+            <v>var00166</v>
+          </cell>
+          <cell r="B167" t="str">
+            <v>Ceilometer cloud amount of first group</v>
+          </cell>
+        </row>
+        <row r="168">
+          <cell r="A168" t="str">
+            <v>var00167</v>
+          </cell>
+          <cell r="B168" t="str">
+            <v>Ceilometer cloud height of first group</v>
+          </cell>
+        </row>
+        <row r="169">
+          <cell r="A169" t="str">
+            <v>var00168</v>
+          </cell>
+          <cell r="B169" t="str">
+            <v>Ceilometer cloud amount of second group</v>
+          </cell>
+        </row>
+        <row r="170">
+          <cell r="A170" t="str">
+            <v>var00169</v>
+          </cell>
+          <cell r="B170" t="str">
+            <v>Ceilometer cloud height of second group</v>
+          </cell>
+        </row>
+        <row r="171">
+          <cell r="A171" t="str">
+            <v>var00170</v>
+          </cell>
+          <cell r="B171" t="str">
+            <v>Ceilometer cloud amount of third group</v>
+          </cell>
+        </row>
+        <row r="172">
+          <cell r="A172" t="str">
+            <v>var00171</v>
+          </cell>
+          <cell r="B172" t="str">
+            <v>Ceilometer cloud height of third group</v>
+          </cell>
+        </row>
+        <row r="173">
+          <cell r="A173" t="str">
+            <v>var00172</v>
+          </cell>
+          <cell r="B173" t="str">
+            <v>Ceilometer sky clear flag</v>
+          </cell>
+        </row>
+        <row r="174">
+          <cell r="A174" t="str">
+            <v>var00173</v>
+          </cell>
+          <cell r="B174" t="str">
+            <v>Horizontal visibility</v>
+          </cell>
+        </row>
+        <row r="175">
+          <cell r="A175" t="str">
+            <v>var00174</v>
+          </cell>
+          <cell r="B175" t="str">
+            <v>AWS visibility</v>
+          </cell>
+        </row>
+        <row r="176">
+          <cell r="A176" t="str">
+            <v>var00175</v>
+          </cell>
+          <cell r="B176" t="str">
+            <v>Present weather in code</v>
+          </cell>
+        </row>
+        <row r="177">
+          <cell r="A177" t="str">
+            <v>var00176</v>
+          </cell>
+          <cell r="B177" t="str">
+            <v>Mean sea level pressure</v>
+          </cell>
+        </row>
+        <row r="178">
+          <cell r="A178" t="str">
+            <v>var00177</v>
+          </cell>
+          <cell r="B178" t="str">
+            <v>Station level pressure</v>
+          </cell>
+        </row>
+        <row r="179">
+          <cell r="A179" t="str">
+            <v>var00178</v>
+          </cell>
+          <cell r="B179" t="str">
+            <v>Chlorophyll sample volume</v>
+          </cell>
+        </row>
+        <row r="180">
+          <cell r="A180" t="str">
+            <v>var00179</v>
+          </cell>
+          <cell r="B180" t="str">
+            <v>Bottom Depth</v>
+          </cell>
+        </row>
+        <row r="181">
+          <cell r="A181" t="str">
+            <v>var00180</v>
+          </cell>
+          <cell r="B181" t="str">
+            <v>Tidal Height</v>
+          </cell>
+        </row>
+        <row r="182">
+          <cell r="A182" t="str">
+            <v>var00181</v>
+          </cell>
+          <cell r="B182" t="str">
+            <v>PAR</v>
+          </cell>
+        </row>
+        <row r="183">
+          <cell r="A183" t="str">
+            <v>var00182</v>
+          </cell>
+          <cell r="B183" t="str">
+            <v>Tilt</v>
+          </cell>
+        </row>
+        <row r="184">
+          <cell r="A184" t="str">
+            <v>var00183</v>
+          </cell>
+          <cell r="B184" t="str">
+            <v>WL - 410</v>
+          </cell>
+        </row>
+        <row r="185">
+          <cell r="A185" t="str">
+            <v>var00184</v>
+          </cell>
+          <cell r="B185" t="str">
+            <v>WL - 440</v>
+          </cell>
+        </row>
+        <row r="186">
+          <cell r="A186" t="str">
+            <v>var00185</v>
+          </cell>
+          <cell r="B186" t="str">
+            <v>WL - 490</v>
+          </cell>
+        </row>
+        <row r="187">
+          <cell r="A187" t="str">
+            <v>var00186</v>
+          </cell>
+          <cell r="B187" t="str">
+            <v>WL - 510</v>
+          </cell>
+        </row>
+        <row r="188">
+          <cell r="A188" t="str">
+            <v>var00187</v>
+          </cell>
+          <cell r="B188" t="str">
+            <v>WL - 550</v>
+          </cell>
+        </row>
+        <row r="189">
+          <cell r="A189" t="str">
+            <v>var00188</v>
+          </cell>
+          <cell r="B189" t="str">
+            <v>WL - 590</v>
+          </cell>
+        </row>
+        <row r="190">
+          <cell r="A190" t="str">
+            <v>var00189</v>
+          </cell>
+          <cell r="B190" t="str">
+            <v>WL - 635</v>
+          </cell>
+        </row>
+        <row r="191">
+          <cell r="A191" t="str">
+            <v>var00190</v>
+          </cell>
+          <cell r="B191" t="str">
+            <v>WL - 660</v>
+          </cell>
+        </row>
+        <row r="192">
+          <cell r="A192" t="str">
+            <v>var00191</v>
+          </cell>
+          <cell r="B192" t="str">
+            <v>WL - 700</v>
+          </cell>
+        </row>
+        <row r="193">
+          <cell r="A193" t="str">
+            <v>var00192</v>
+          </cell>
+          <cell r="B193" t="str">
+            <v>ACCELERATIONX</v>
+          </cell>
+        </row>
+        <row r="194">
+          <cell r="A194" t="str">
+            <v>var00193</v>
+          </cell>
+          <cell r="B194" t="str">
+            <v>ACCELERATIONY</v>
+          </cell>
+        </row>
+        <row r="195">
+          <cell r="A195" t="str">
+            <v>var00194</v>
+          </cell>
+          <cell r="B195" t="str">
+            <v>ACCELERATIONZ</v>
+          </cell>
+        </row>
+        <row r="196">
+          <cell r="A196" t="str">
+            <v>var00195</v>
+          </cell>
+          <cell r="B196" t="str">
+            <v>AMPLITUDE1</v>
+          </cell>
+        </row>
+        <row r="197">
+          <cell r="A197" t="str">
+            <v>var00196</v>
+          </cell>
+          <cell r="B197" t="str">
+            <v>AMPLITUDE2</v>
+          </cell>
+        </row>
+        <row r="198">
+          <cell r="A198" t="str">
+            <v>var00197</v>
+          </cell>
+          <cell r="B198" t="str">
+            <v>AMPLITUDE3</v>
+          </cell>
+        </row>
+        <row r="199">
+          <cell r="A199" t="str">
+            <v>var00198</v>
+          </cell>
+          <cell r="B199" t="str">
+            <v>CELL</v>
+          </cell>
+        </row>
+        <row r="200">
+          <cell r="A200" t="str">
+            <v>var00199</v>
+          </cell>
+          <cell r="B200" t="str">
+            <v>DENSITY ANOMALY</v>
+          </cell>
+        </row>
+        <row r="201">
+          <cell r="A201" t="str">
+            <v>var00201</v>
+          </cell>
+          <cell r="B201" t="str">
+            <v>HEADING</v>
+          </cell>
+        </row>
+        <row r="202">
+          <cell r="A202" t="str">
+            <v>var00202</v>
+          </cell>
+          <cell r="B202" t="str">
+            <v>LOWER_UCUR</v>
+          </cell>
+        </row>
+        <row r="203">
+          <cell r="A203" t="str">
+            <v>var00203</v>
+          </cell>
+          <cell r="B203" t="str">
+            <v>LOWER_VCUR</v>
+          </cell>
+        </row>
+        <row r="204">
+          <cell r="A204" t="str">
+            <v>var00204</v>
+          </cell>
+          <cell r="B204" t="str">
+            <v>MIDDLE_UCUR</v>
+          </cell>
+        </row>
+        <row r="205">
+          <cell r="A205" t="str">
+            <v>var00205</v>
+          </cell>
+          <cell r="B205" t="str">
+            <v>MIDDLE_VCUR</v>
+          </cell>
+        </row>
+        <row r="206">
+          <cell r="A206" t="str">
+            <v>var00206</v>
+          </cell>
+          <cell r="B206" t="str">
+            <v>Pitch</v>
+          </cell>
+        </row>
+        <row r="207">
+          <cell r="A207" t="str">
+            <v>var00207</v>
+          </cell>
+          <cell r="B207" t="str">
+            <v>PRESSURE</v>
+          </cell>
+        </row>
+        <row r="208">
+          <cell r="A208" t="str">
+            <v>var00208</v>
+          </cell>
+          <cell r="B208" t="str">
+            <v>PRESSURE_SENSOR_DEPTH</v>
+          </cell>
+        </row>
+        <row r="209">
+          <cell r="A209" t="str">
+            <v>var00209</v>
+          </cell>
+          <cell r="B209" t="str">
+            <v>ROLL</v>
+          </cell>
+        </row>
+        <row r="210">
+          <cell r="A210" t="str">
+            <v>var00210</v>
+          </cell>
+          <cell r="B210" t="str">
+            <v>SPEED_OF_SOUND</v>
+          </cell>
+        </row>
+        <row r="211">
+          <cell r="A211" t="str">
+            <v>var00211</v>
+          </cell>
+          <cell r="B211" t="str">
+            <v>UCUR (eastward velocity)</v>
+          </cell>
+        </row>
+        <row r="212">
+          <cell r="A212" t="str">
+            <v>var00212</v>
+          </cell>
+          <cell r="B212" t="str">
+            <v>UPPER_UCUR</v>
+          </cell>
+        </row>
+        <row r="213">
+          <cell r="A213" t="str">
+            <v>var00213</v>
+          </cell>
+          <cell r="B213" t="str">
+            <v>UPPER_VCUR</v>
+          </cell>
+        </row>
+        <row r="214">
+          <cell r="A214" t="str">
+            <v>var00214</v>
+          </cell>
+          <cell r="B214" t="str">
+            <v>VCUR (northward velocity)</v>
+          </cell>
+        </row>
+        <row r="215">
+          <cell r="A215" t="str">
+            <v>var00215</v>
+          </cell>
+          <cell r="B215" t="str">
+            <v>WCUR</v>
+          </cell>
+        </row>
+        <row r="216">
+          <cell r="A216" t="str">
+            <v>var00216</v>
+          </cell>
+          <cell r="B216" t="str">
+            <v>light attenuation coefficient</v>
+          </cell>
+        </row>
+        <row r="217">
+          <cell r="A217" t="str">
+            <v>var00217</v>
+          </cell>
+          <cell r="B217" t="str">
+            <v>cell</v>
+          </cell>
+        </row>
+        <row r="218">
+          <cell r="A218" t="str">
+            <v>var00218</v>
+          </cell>
+          <cell r="B218" t="str">
+            <v>density</v>
+          </cell>
+        </row>
+        <row r="219">
+          <cell r="A219" t="str">
+            <v>var00219</v>
+          </cell>
+          <cell r="B219" t="str">
+            <v>fluorescence</v>
+          </cell>
+        </row>
+        <row r="220">
+          <cell r="A220" t="str">
+            <v>var00220</v>
+          </cell>
+          <cell r="B220" t="str">
+            <v>Prochlorococcus</v>
+          </cell>
+        </row>
+        <row r="221">
+          <cell r="A221" t="str">
+            <v>var00221</v>
+          </cell>
+          <cell r="B221" t="str">
+            <v>Synechococcus</v>
+          </cell>
+        </row>
+        <row r="222">
+          <cell r="A222" t="str">
+            <v>var00222</v>
+          </cell>
+          <cell r="B222" t="str">
+            <v>Picoeukaryotes</v>
+          </cell>
+        </row>
+        <row r="223">
+          <cell r="A223" t="str">
+            <v>var00223</v>
+          </cell>
+          <cell r="B223" t="str">
+            <v>Allo</v>
+          </cell>
+        </row>
+        <row r="224">
+          <cell r="A224" t="str">
+            <v>var00224</v>
+          </cell>
+          <cell r="B224" t="str">
+            <v>AlphaBetaCar</v>
+          </cell>
+        </row>
+        <row r="225">
+          <cell r="A225" t="str">
+            <v>var00225</v>
+          </cell>
+          <cell r="B225" t="str">
+            <v>Anth</v>
+          </cell>
+        </row>
+        <row r="226">
+          <cell r="A226" t="str">
+            <v>var00226</v>
+          </cell>
+          <cell r="B226" t="str">
+            <v>Asta</v>
+          </cell>
+        </row>
+        <row r="227">
+          <cell r="A227" t="str">
+            <v>var00227</v>
+          </cell>
+          <cell r="B227" t="str">
+            <v>BetaBetaCar</v>
+          </cell>
+        </row>
+        <row r="228">
+          <cell r="A228" t="str">
+            <v>var00228</v>
+          </cell>
+          <cell r="B228" t="str">
+            <v>BetaEpiCar</v>
+          </cell>
+        </row>
+        <row r="229">
+          <cell r="A229" t="str">
+            <v>var00229</v>
+          </cell>
+          <cell r="B229" t="str">
+            <v>Butfuco</v>
+          </cell>
+        </row>
+        <row r="230">
+          <cell r="A230" t="str">
+            <v>var00230</v>
+          </cell>
+          <cell r="B230" t="str">
+            <v>Cantha</v>
+          </cell>
+        </row>
+        <row r="231">
+          <cell r="A231" t="str">
+            <v>var00231</v>
+          </cell>
+          <cell r="B231" t="str">
+            <v>CphlA</v>
+          </cell>
+        </row>
+        <row r="232">
+          <cell r="A232" t="str">
+            <v>var00232</v>
+          </cell>
+          <cell r="B232" t="str">
+            <v>CphlB</v>
+          </cell>
+        </row>
+        <row r="233">
+          <cell r="A233" t="str">
+            <v>var00233</v>
+          </cell>
+          <cell r="B233" t="str">
+            <v>CphlC1</v>
+          </cell>
+        </row>
+        <row r="234">
+          <cell r="A234" t="str">
+            <v>var00234</v>
+          </cell>
+          <cell r="B234" t="str">
+            <v>CphlC2</v>
+          </cell>
+        </row>
+        <row r="235">
+          <cell r="A235" t="str">
+            <v>var00235</v>
+          </cell>
+          <cell r="B235" t="str">
+            <v>CphlC3</v>
+          </cell>
+        </row>
+        <row r="236">
+          <cell r="A236" t="str">
+            <v>var00236</v>
+          </cell>
+          <cell r="B236" t="str">
+            <v>CphlC1C2</v>
+          </cell>
+        </row>
+        <row r="237">
+          <cell r="A237" t="str">
+            <v>var00237</v>
+          </cell>
+          <cell r="B237" t="str">
+            <v>CphlideA</v>
+          </cell>
+        </row>
+        <row r="238">
+          <cell r="A238" t="str">
+            <v>var00238</v>
+          </cell>
+          <cell r="B238" t="str">
+            <v>Diadchr</v>
+          </cell>
+        </row>
+        <row r="239">
+          <cell r="A239" t="str">
+            <v>var00239</v>
+          </cell>
+          <cell r="B239" t="str">
+            <v>Diadino</v>
+          </cell>
+        </row>
+        <row r="240">
+          <cell r="A240" t="str">
+            <v>var00240</v>
+          </cell>
+          <cell r="B240" t="str">
+            <v>Diato</v>
+          </cell>
+        </row>
+        <row r="241">
+          <cell r="A241" t="str">
+            <v>var00241</v>
+          </cell>
+          <cell r="B241" t="str">
+            <v>Dino</v>
+          </cell>
+        </row>
+        <row r="242">
+          <cell r="A242" t="str">
+            <v>var00242</v>
+          </cell>
+          <cell r="B242" t="str">
+            <v>DvCphlA+CphlA</v>
+          </cell>
+        </row>
+        <row r="243">
+          <cell r="A243" t="str">
+            <v>var00243</v>
+          </cell>
+          <cell r="B243" t="str">
+            <v>DvCphlA</v>
+          </cell>
+        </row>
+        <row r="244">
+          <cell r="A244" t="str">
+            <v>var00244</v>
+          </cell>
+          <cell r="B244" t="str">
+            <v>DvCphlB+CphlB</v>
+          </cell>
+        </row>
+        <row r="245">
+          <cell r="A245" t="str">
+            <v>var00245</v>
+          </cell>
+          <cell r="B245" t="str">
+            <v>DvCphlB</v>
+          </cell>
+        </row>
+        <row r="246">
+          <cell r="A246" t="str">
+            <v>var00246</v>
+          </cell>
+          <cell r="B246" t="str">
+            <v>Echin</v>
+          </cell>
+        </row>
+        <row r="247">
+          <cell r="A247" t="str">
+            <v>var00247</v>
+          </cell>
+          <cell r="B247" t="str">
+            <v>Fuco</v>
+          </cell>
+        </row>
+        <row r="248">
+          <cell r="A248" t="str">
+            <v>var00248</v>
+          </cell>
+          <cell r="B248" t="str">
+            <v>Gyro</v>
+          </cell>
+        </row>
+        <row r="249">
+          <cell r="A249" t="str">
+            <v>var00249</v>
+          </cell>
+          <cell r="B249" t="str">
+            <v>Hexfuco</v>
+          </cell>
+        </row>
+        <row r="250">
+          <cell r="A250" t="str">
+            <v>var00250</v>
+          </cell>
+          <cell r="B250" t="str">
+            <v>Ketohexfuco</v>
+          </cell>
+        </row>
+        <row r="251">
+          <cell r="A251" t="str">
+            <v>var00251</v>
+          </cell>
+          <cell r="B251" t="str">
+            <v>Lut</v>
+          </cell>
+        </row>
+        <row r="252">
+          <cell r="A252" t="str">
+            <v>var00252</v>
+          </cell>
+          <cell r="B252" t="str">
+            <v>Lyco</v>
+          </cell>
+        </row>
+        <row r="253">
+          <cell r="A253" t="str">
+            <v>var00253</v>
+          </cell>
+          <cell r="B253" t="str">
+            <v>MgDvp</v>
+          </cell>
+        </row>
+        <row r="254">
+          <cell r="A254" t="str">
+            <v>var00254</v>
+          </cell>
+          <cell r="B254" t="str">
+            <v>Neo</v>
+          </cell>
+        </row>
+        <row r="255">
+          <cell r="A255" t="str">
+            <v>var00255</v>
+          </cell>
+          <cell r="B255" t="str">
+            <v>Perid</v>
+          </cell>
+        </row>
+        <row r="256">
+          <cell r="A256" t="str">
+            <v>var00256</v>
+          </cell>
+          <cell r="B256" t="str">
+            <v>PhideA</v>
+          </cell>
+        </row>
+        <row r="257">
+          <cell r="A257" t="str">
+            <v>var00257</v>
+          </cell>
+          <cell r="B257" t="str">
+            <v>PhytinA</v>
+          </cell>
+        </row>
+        <row r="258">
+          <cell r="A258" t="str">
+            <v>var00258</v>
+          </cell>
+          <cell r="B258" t="str">
+            <v>PhytinB</v>
+          </cell>
+        </row>
+        <row r="259">
+          <cell r="A259" t="str">
+            <v>var00259</v>
+          </cell>
+          <cell r="B259" t="str">
+            <v>Pras</v>
+          </cell>
+        </row>
+        <row r="260">
+          <cell r="A260" t="str">
+            <v>var00260</v>
+          </cell>
+          <cell r="B260" t="str">
+            <v>PyrophideA</v>
+          </cell>
+        </row>
+        <row r="261">
+          <cell r="A261" t="str">
+            <v>var00261</v>
+          </cell>
+          <cell r="B261" t="str">
+            <v>PyrophytinA</v>
+          </cell>
+        </row>
+        <row r="262">
+          <cell r="A262" t="str">
+            <v>var00262</v>
+          </cell>
+          <cell r="B262" t="str">
+            <v>Viola</v>
+          </cell>
+        </row>
+        <row r="263">
+          <cell r="A263" t="str">
+            <v>var00263</v>
+          </cell>
+          <cell r="B263" t="str">
+            <v>Zea</v>
+          </cell>
+        </row>
+        <row r="264">
+          <cell r="A264" t="str">
+            <v>var00264</v>
+          </cell>
+          <cell r="B264" t="str">
+            <v>Nitrite</v>
+          </cell>
+        </row>
+        <row r="265">
+          <cell r="A265" t="str">
+            <v>var00265</v>
+          </cell>
+          <cell r="B265" t="str">
+            <v>TSSorganic</v>
+          </cell>
+        </row>
+        <row r="266">
+          <cell r="A266" t="str">
+            <v>var00266</v>
+          </cell>
+          <cell r="B266" t="str">
+            <v>TSSinorganic</v>
+          </cell>
+        </row>
+        <row r="267">
+          <cell r="A267" t="str">
+            <v>var00267</v>
+          </cell>
+          <cell r="B267" t="str">
+            <v>DIC</v>
+          </cell>
+        </row>
+        <row r="268">
+          <cell r="A268" t="str">
+            <v>var00268</v>
+          </cell>
+          <cell r="B268" t="str">
+            <v>Pressure head</v>
+          </cell>
+        </row>
+        <row r="269">
+          <cell r="A269" t="str">
+            <v>var00269</v>
+          </cell>
+          <cell r="B269" t="str">
+            <v>velocity x component of current</v>
+          </cell>
+        </row>
+        <row r="270">
+          <cell r="A270" t="str">
+            <v>var00270</v>
+          </cell>
+          <cell r="B270" t="str">
+            <v>velocity y component of current</v>
+          </cell>
+        </row>
+        <row r="271">
+          <cell r="A271" t="str">
+            <v>var00271</v>
+          </cell>
+          <cell r="B271" t="str">
+            <v>Significant waveheight</v>
+          </cell>
+        </row>
+        <row r="272">
+          <cell r="A272" t="str">
+            <v>var00272</v>
+          </cell>
+          <cell r="B272" t="str">
+            <v>Mean 1/3 waveheight</v>
+          </cell>
+        </row>
+        <row r="273">
+          <cell r="A273" t="str">
+            <v>var00273</v>
+          </cell>
+          <cell r="B273" t="str">
+            <v>Mean 1/10 waveheight</v>
+          </cell>
+        </row>
+        <row r="274">
+          <cell r="A274" t="str">
+            <v>var00274</v>
+          </cell>
+          <cell r="B274" t="str">
+            <v>Maximum waveheight</v>
+          </cell>
+        </row>
+        <row r="275">
+          <cell r="A275" t="str">
+            <v>var00275</v>
+          </cell>
+          <cell r="B275" t="str">
+            <v>Mean wave height</v>
+          </cell>
+        </row>
+        <row r="276">
+          <cell r="A276" t="str">
+            <v>var00276</v>
+          </cell>
+          <cell r="B276" t="str">
+            <v>Mean wave period</v>
+          </cell>
+        </row>
+        <row r="277">
+          <cell r="A277" t="str">
+            <v>var00277</v>
+          </cell>
+          <cell r="B277" t="str">
+            <v>Peak wave period</v>
+          </cell>
+        </row>
+        <row r="278">
+          <cell r="A278" t="str">
+            <v>var00278</v>
+          </cell>
+          <cell r="B278" t="str">
+            <v>Mean 1/3 period</v>
+          </cell>
+        </row>
+        <row r="279">
+          <cell r="A279" t="str">
+            <v>var00279</v>
+          </cell>
+          <cell r="B279" t="str">
+            <v>Mean 1/10 period</v>
+          </cell>
+        </row>
+        <row r="280">
+          <cell r="A280" t="str">
+            <v>var00280</v>
+          </cell>
+          <cell r="B280" t="str">
+            <v>Maximum wave period</v>
+          </cell>
+        </row>
+        <row r="281">
+          <cell r="A281" t="str">
+            <v>var00281</v>
+          </cell>
+          <cell r="B281" t="str">
+            <v>Peak wave direction</v>
+          </cell>
+        </row>
+        <row r="282">
+          <cell r="A282" t="str">
+            <v>var00282</v>
+          </cell>
+          <cell r="B282" t="str">
+            <v>Directional spread</v>
+          </cell>
+        </row>
+        <row r="283">
+          <cell r="A283" t="str">
+            <v>var00283</v>
+          </cell>
+          <cell r="B283" t="str">
+            <v>Mean wave direction</v>
+          </cell>
+        </row>
+        <row r="284">
+          <cell r="A284" t="str">
+            <v>var00284</v>
+          </cell>
+          <cell r="B284" t="str">
+            <v>Current velocity</v>
+          </cell>
+        </row>
+        <row r="285">
+          <cell r="A285" t="str">
+            <v>var00285</v>
+          </cell>
+          <cell r="B285" t="str">
+            <v>Current direction</v>
+          </cell>
+        </row>
+        <row r="286">
+          <cell r="A286" t="str">
+            <v>var00286</v>
+          </cell>
+          <cell r="B286" t="str">
+            <v>Min Wind Speed</v>
+          </cell>
+        </row>
+        <row r="287">
+          <cell r="A287" t="str">
+            <v>var00287</v>
+          </cell>
+          <cell r="B287" t="str">
+            <v>Wind Direction STD</v>
+          </cell>
+        </row>
+        <row r="288">
+          <cell r="A288" t="str">
+            <v>var00288</v>
+          </cell>
+          <cell r="B288" t="str">
+            <v>max station level pressure</v>
+          </cell>
+        </row>
+        <row r="289">
+          <cell r="A289" t="str">
+            <v>var00289</v>
+          </cell>
+          <cell r="B289" t="str">
+            <v>min station level pressure</v>
+          </cell>
+        </row>
+        <row r="290">
+          <cell r="A290" t="str">
+            <v>var00290</v>
+          </cell>
+          <cell r="B290" t="str">
+            <v>station level pressure std</v>
+          </cell>
+        </row>
+        <row r="291">
+          <cell r="A291" t="str">
+            <v>var00291</v>
+          </cell>
+          <cell r="B291" t="str">
+            <v>mean solar radiation</v>
+          </cell>
+        </row>
+        <row r="292">
+          <cell r="A292" t="str">
+            <v>var00292</v>
+          </cell>
+          <cell r="B292" t="str">
+            <v>min solar radiation</v>
+          </cell>
+        </row>
+        <row r="293">
+          <cell r="A293" t="str">
+            <v>var00293</v>
+          </cell>
+          <cell r="B293" t="str">
+            <v>max solar radiation</v>
+          </cell>
+        </row>
+        <row r="294">
+          <cell r="A294" t="str">
+            <v>var00294</v>
+          </cell>
+          <cell r="B294" t="str">
+            <v>solar radiation std</v>
+          </cell>
+        </row>
+        <row r="295">
+          <cell r="A295" t="str">
+            <v>var00295</v>
+          </cell>
+          <cell r="B295" t="str">
+            <v>max PAR</v>
+          </cell>
+        </row>
+        <row r="296">
+          <cell r="A296" t="str">
+            <v>var00296</v>
+          </cell>
+          <cell r="B296" t="str">
+            <v>min PAR</v>
+          </cell>
+        </row>
+        <row r="297">
+          <cell r="A297" t="str">
+            <v>var00297</v>
+          </cell>
+          <cell r="B297" t="str">
+            <v>PAR STD</v>
+          </cell>
+        </row>
+        <row r="298">
+          <cell r="A298" t="str">
+            <v>var00298</v>
+          </cell>
+          <cell r="B298" t="str">
+            <v>Total Par</v>
+          </cell>
+        </row>
+        <row r="299">
+          <cell r="A299" t="str">
+            <v>var00299</v>
+          </cell>
+          <cell r="B299" t="str">
+            <v>Total Solar</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6864,10 +9318,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J319"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A273" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H300" sqref="H300"/>
     </sheetView>
@@ -13116,7 +15570,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J318" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J318"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -13125,7 +15579,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13489,7 +15943,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14040,7 +16494,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14422,7 +16876,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15251,7 +17705,113 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D2" t="str">
+        <f>VLOOKUP(C2,'[1]MASTER KEY'!$A$2:$B930,2,TRUE)</f>
+        <v>Significant waveheight</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>1343</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1339</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15522,8 +18082,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBC0BB9-8F45-4117-8EDC-41406E638950}">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15926,8 +18486,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16229,8 +18789,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16452,8 +19012,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16621,143 +19181,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1374</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="D2" t="str">
-        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B928,2,TRUE)</f>
-        <v>Tidal Height</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>839</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>898</v>
-      </c>
-      <c r="D3" t="str">
-        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B929,2,TRUE)</f>
-        <v>PAR</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1309</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1315</v>
-      </c>
-      <c r="D4" t="str">
-        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B930,2,TRUE)</f>
-        <v>velocity x component of current</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1310</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>1316</v>
-      </c>
-      <c r="D5" t="str">
-        <f>VLOOKUP(C5,'MASTER KEY'!$A$2:$B931,2,TRUE)</f>
-        <v>velocity y component of current</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>715</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D6" t="str">
-        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B932,2,TRUE)</f>
-        <v>Temperature</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>714</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D7" t="str">
-        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B933,2,TRUE)</f>
-        <v>Salinity</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1375</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>1373</v>
-      </c>
-      <c r="D8" t="str">
-        <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B934,2,TRUE)</f>
-        <v>Current velocity</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD7D7559-1643-4FF9-B8E5-4B46BD5C53B5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17150,7 +19575,142 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D2" t="str">
+        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B928,2,TRUE)</f>
+        <v>Tidal Height</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>839</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="D3" t="str">
+        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B929,2,TRUE)</f>
+        <v>PAR</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1315</v>
+      </c>
+      <c r="D4" t="str">
+        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B930,2,TRUE)</f>
+        <v>velocity x component of current</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1316</v>
+      </c>
+      <c r="D5" t="str">
+        <f>VLOOKUP(C5,'MASTER KEY'!$A$2:$B931,2,TRUE)</f>
+        <v>velocity y component of current</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>715</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D6" t="str">
+        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B932,2,TRUE)</f>
+        <v>Temperature</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>714</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" t="str">
+        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B933,2,TRUE)</f>
+        <v>Salinity</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1373</v>
+      </c>
+      <c r="D8" t="str">
+        <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B934,2,TRUE)</f>
+        <v>Current velocity</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17268,8 +19828,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17297,7 +19857,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A236"/>
   <sheetViews>
     <sheetView topLeftCell="A109" workbookViewId="0">
@@ -18495,7 +21055,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F284"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24763,7 +27323,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5261A16-8B5D-4B5D-ADA5-57BB15B52747}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25082,7 +27642,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27011,7 +29571,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView topLeftCell="A23" workbookViewId="0">
@@ -28169,7 +30729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28533,7 +31093,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Updated imports for Theme2, WCWA & FPA
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\csiem-data\data-governance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDD4773-BA47-40AE-B986-8B71A1278767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DB061B-FA64-4F76-8D11-6D9728D935BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" tabRatio="841" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" firstSheet="1" activeTab="1" xr2:uid="{F9B0BAF6-804F-4CC2-AC1B-42D25A858702}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{F9B0BAF6-804F-4CC2-AC1B-42D25A858702}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="6" r:id="rId1"/>
@@ -388,7 +387,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4850" uniqueCount="2010">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4873" uniqueCount="2016">
   <si>
     <t>Model Variable Conversion</t>
   </si>
@@ -6538,6 +6537,24 @@
   </si>
   <si>
     <t>trh_gtc34_c40</t>
+  </si>
+  <si>
+    <t>Posidonia Sinuosa Total Biomass</t>
+  </si>
+  <si>
+    <t>posidonia_sinuosa_total_biomass</t>
+  </si>
+  <si>
+    <t>µmol C/m2</t>
+  </si>
+  <si>
+    <t>Posidonia Sinuosa Dry Weight</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>posidonia_sinuosa_dry_weight</t>
   </si>
 </sst>
 </file>
@@ -7282,10 +7299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A3:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -7311,10 +7325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3637D217-629A-4AA1-BFB1-326590517B91}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D13"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -7527,10 +7538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D25"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -7932,10 +7940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D25"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -8333,10 +8338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:XFD65"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -10263,10 +10265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -11422,10 +11421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -11787,10 +11783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
   <cols>
@@ -12450,10 +12443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D23"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -12824,10 +12814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D35"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
   <cols>
@@ -13382,10 +13369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D24"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -13773,14 +13757,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:L341"/>
+  <dimension ref="A1:L343"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F341" sqref="F341"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="1">
-      <selection activeCell="F319" sqref="F319"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
@@ -21749,6 +21729,55 @@
         <v>20</v>
       </c>
     </row>
+    <row r="342" spans="1:11" ht="14.4">
+      <c r="A342" s="1" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B342" t="s">
+        <v>2010</v>
+      </c>
+      <c r="C342" s="1" t="s">
+        <v>1897</v>
+      </c>
+      <c r="E342" s="10" t="s">
+        <v>1907</v>
+      </c>
+      <c r="F342" t="s">
+        <v>2011</v>
+      </c>
+      <c r="H342" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K342" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="343" spans="1:11" ht="14.4">
+      <c r="A343" s="1" t="s">
+        <v>1973</v>
+      </c>
+      <c r="B343" t="s">
+        <v>2013</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>2014</v>
+      </c>
+      <c r="D343" s="1" t="s">
+        <v>2014</v>
+      </c>
+      <c r="E343" s="1" t="s">
+        <v>2014</v>
+      </c>
+      <c r="F343" t="s">
+        <v>2015</v>
+      </c>
+      <c r="H343" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K343" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:L318" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="10">
@@ -21771,10 +21800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
@@ -21880,10 +21906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -22184,10 +22207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -22414,10 +22434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D10"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -22587,10 +22604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -22732,10 +22746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
@@ -22852,10 +22863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A236"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
@@ -24052,7 +24060,6 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
@@ -24064,10 +24071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0CBB6E-1B94-4464-948D-3552DECBF22E}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -24141,13 +24145,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F304"/>
+  <dimension ref="A1:F306"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B306" sqref="B306"/>
-    </sheetView>
-    <sheetView topLeftCell="A271" workbookViewId="1">
+    <sheetView topLeftCell="A271" workbookViewId="0">
       <selection activeCell="A304" sqref="A304:XFD304"/>
     </sheetView>
   </sheetViews>
@@ -30984,13 +30984,13 @@
         <v>Posidonia Sinuosa Above Ground Biomass</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>1897</v>
+        <v>2012</v>
       </c>
       <c r="D302" t="s">
         <v>1910</v>
       </c>
       <c r="E302" s="1" t="s">
-        <v>1897</v>
+        <v>2012</v>
       </c>
       <c r="F302">
         <v>1</v>
@@ -31005,13 +31005,13 @@
         <v>Posidonia Sinuosa Below Ground Biomass</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>1897</v>
+        <v>2012</v>
       </c>
       <c r="D303" t="s">
         <v>1911</v>
       </c>
       <c r="E303" s="1" t="s">
-        <v>1897</v>
+        <v>2012</v>
       </c>
       <c r="F303">
         <v>1</v>
@@ -31035,6 +31035,48 @@
         <v>92</v>
       </c>
       <c r="F304">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6">
+      <c r="A305" s="1" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B305" t="str">
+        <f>VLOOKUP(A305,'MASTER KEY'!$A$2:$B1274,2,FALSE)</f>
+        <v>Posidonia Sinuosa Total Biomass</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>2012</v>
+      </c>
+      <c r="D305" t="s">
+        <v>2011</v>
+      </c>
+      <c r="E305" s="1" t="s">
+        <v>2012</v>
+      </c>
+      <c r="F305">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6">
+      <c r="A306" s="1" t="s">
+        <v>1973</v>
+      </c>
+      <c r="B306" t="str">
+        <f>VLOOKUP(A306,'MASTER KEY'!$A$2:$B1275,2,FALSE)</f>
+        <v>Posidonia Sinuosa Dry Weight</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>2014</v>
+      </c>
+      <c r="D306" t="s">
+        <v>2015</v>
+      </c>
+      <c r="E306" s="1" t="s">
+        <v>2014</v>
+      </c>
+      <c r="F306">
         <v>1</v>
       </c>
     </row>
@@ -31051,9 +31093,6 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -32078,9 +32117,6 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -32956,10 +32992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -33287,10 +33320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D17"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -33564,6 +33594,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010003AB3CEE24CC9549A4C2A281013CE3FF" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c392439da3f348303a75f5d18241249a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef9f29e7-1a1c-412a-b28d-c6b5d10182ce" xmlns:ns3="3bc65d7e-f616-49fd-b09c-31cb8a0f9f35" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="791e796a73d52f1825a418e61b158f36" ns2:_="" ns3:_="">
     <xsd:import namespace="ef9f29e7-1a1c-412a-b28d-c6b5d10182ce"/>
@@ -33774,16 +33813,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4FF3EBF-E249-4974-B438-7AE6C30398AF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{002762F3-4309-419D-97A6-51D1B85C85F3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33800,12 +33838,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4FF3EBF-E249-4974-B438-7AE6C30398AF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated mapping code and imports
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\csiem-data\data-governance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DB061B-FA64-4F76-8D11-6D9728D935BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DC2857-0950-47D5-B140-E08DE7C383C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{F9B0BAF6-804F-4CC2-AC1B-42D25A858702}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="1" xr2:uid="{F9B0BAF6-804F-4CC2-AC1B-42D25A858702}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="6" r:id="rId1"/>
@@ -387,7 +387,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4873" uniqueCount="2016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4881" uniqueCount="2018">
   <si>
     <t>Model Variable Conversion</t>
   </si>
@@ -6555,6 +6555,12 @@
   </si>
   <si>
     <t>posidonia_sinuosa_dry_weight</t>
+  </si>
+  <si>
+    <t>Picoplankton Fraction</t>
+  </si>
+  <si>
+    <t>picop_brewin2012in</t>
   </si>
 </sst>
 </file>
@@ -7301,9 +7307,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="52.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:1">
@@ -7327,12 +7333,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -7540,10 +7546,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7942,11 +7948,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="38" customFormat="1">
@@ -8340,10 +8346,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -10267,9 +10273,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11423,9 +11429,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -11785,12 +11791,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="9.109375" style="1"/>
-    <col min="4" max="4" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="36.7109375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -12445,10 +12451,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -12816,13 +12822,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="53" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="3" max="3" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -13268,7 +13274,7 @@
         <v>Station Level Pressure</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="14.4">
+    <row r="30" spans="1:4" ht="15">
       <c r="A30" t="s">
         <v>1616</v>
       </c>
@@ -13283,7 +13289,7 @@
         <v>Water Surface Height</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="14.4">
+    <row r="31" spans="1:4" ht="15">
       <c r="A31" t="s">
         <v>1617</v>
       </c>
@@ -13298,7 +13304,7 @@
         <v>Temperature</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="14.4">
+    <row r="32" spans="1:4" ht="15">
       <c r="A32" t="s">
         <v>597</v>
       </c>
@@ -13313,7 +13319,7 @@
         <v>Air Temperature</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="14.4">
+    <row r="33" spans="1:4" ht="15">
       <c r="A33" t="s">
         <v>1618</v>
       </c>
@@ -13328,7 +13334,7 @@
         <v>Station Level Pressure</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="14.4">
+    <row r="34" spans="1:4" ht="15">
       <c r="A34" t="s">
         <v>497</v>
       </c>
@@ -13343,7 +13349,7 @@
         <v>Wind Direction</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="14.4">
+    <row r="35" spans="1:4" ht="15">
       <c r="A35" t="s">
         <v>506</v>
       </c>
@@ -13371,9 +13377,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
   </cols>
@@ -13757,30 +13763,30 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:L343"/>
+  <dimension ref="A1:L344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView tabSelected="1" topLeftCell="I299" workbookViewId="0">
+      <selection activeCell="L345" sqref="L345"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="60" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="32" customFormat="1" ht="24.9" customHeight="1">
+    <row r="1" spans="1:12" s="32" customFormat="1" ht="24.95" customHeight="1">
       <c r="A1" s="32" t="s">
         <v>2</v>
       </c>
@@ -21056,7 +21062,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="315" spans="1:11" ht="14.4">
+    <row r="315" spans="1:11" ht="15">
       <c r="A315" s="23" t="s">
         <v>1899</v>
       </c>
@@ -21073,7 +21079,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="316" spans="1:11" ht="14.4">
+    <row r="316" spans="1:11" ht="15">
       <c r="A316" s="23" t="s">
         <v>1900</v>
       </c>
@@ -21090,7 +21096,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="317" spans="1:11" ht="14.4">
+    <row r="317" spans="1:11" ht="15">
       <c r="A317" s="23" t="s">
         <v>1901</v>
       </c>
@@ -21110,7 +21116,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="318" spans="1:11" ht="14.4">
+    <row r="318" spans="1:11" ht="15">
       <c r="A318" s="23" t="s">
         <v>1906</v>
       </c>
@@ -21729,7 +21735,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="342" spans="1:11" ht="14.4">
+    <row r="342" spans="1:11" ht="15">
       <c r="A342" s="1" t="s">
         <v>1972</v>
       </c>
@@ -21752,9 +21758,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="343" spans="1:11" ht="14.4">
+    <row r="343" spans="1:11" ht="15">
       <c r="A343" s="1" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="B343" t="s">
         <v>2013</v>
@@ -21776,6 +21782,32 @@
       </c>
       <c r="K343" s="1" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="344" spans="1:11">
+      <c r="A344" s="1" t="s">
+        <v>1973</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>2016</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D344" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="E344" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="F344" s="1" t="s">
+        <v>2017</v>
+      </c>
+      <c r="H344" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K344" s="1" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -21802,7 +21834,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
@@ -21908,10 +21940,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -22209,10 +22241,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -22436,10 +22468,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -22564,7 +22596,7 @@
         <v>Mean Wave Period</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.2">
+    <row r="9" spans="1:5" ht="17.25">
       <c r="A9" s="14" t="s">
         <v>1667</v>
       </c>
@@ -22579,7 +22611,7 @@
         <v>Peak Wave Direction</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16.2">
+    <row r="10" spans="1:5" ht="17.25">
       <c r="A10" s="15" t="s">
         <v>1668</v>
       </c>
@@ -22606,9 +22638,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -22748,7 +22780,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
@@ -22865,7 +22897,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
   </cols>
@@ -24061,7 +24093,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24073,10 +24105,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -24151,14 +24183,14 @@
       <selection activeCell="A304" sqref="A304:XFD304"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -31065,7 +31097,7 @@
       </c>
       <c r="B306" t="str">
         <f>VLOOKUP(A306,'MASTER KEY'!$A$2:$B1275,2,FALSE)</f>
-        <v>Posidonia Sinuosa Dry Weight</v>
+        <v>Picoplankton Fraction</v>
       </c>
       <c r="C306" s="1" t="s">
         <v>2014</v>
@@ -31096,12 +31128,12 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -32120,10 +32152,10 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -32994,10 +33026,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -33322,10 +33354,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -33594,15 +33626,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010003AB3CEE24CC9549A4C2A281013CE3FF" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c392439da3f348303a75f5d18241249a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef9f29e7-1a1c-412a-b28d-c6b5d10182ce" xmlns:ns3="3bc65d7e-f616-49fd-b09c-31cb8a0f9f35" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="791e796a73d52f1825a418e61b158f36" ns2:_="" ns3:_="">
     <xsd:import namespace="ef9f29e7-1a1c-412a-b28d-c6b5d10182ce"/>
@@ -33813,15 +33836,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4FF3EBF-E249-4974-B438-7AE6C30398AF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{002762F3-4309-419D-97A6-51D1B85C85F3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33838,4 +33862,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4FF3EBF-E249-4974-B438-7AE6C30398AF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
reupdated varkey excel, csv2matlab csv2parquet appear to be working but havent ran it all the way, takes a long time, IMOS bgc also works now
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loxte\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loxte\AppData\Local\Temp\scp18756\GIS_DATA\csiem-data-hub\git\data-governance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038A0A39-1C09-4433-8FEE-08626439F8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84897D77-D540-4F03-BD23-4F8A3DB23D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4893" uniqueCount="2036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4984" uniqueCount="2052">
   <si>
     <t>//</t>
   </si>
@@ -6296,6 +6296,54 @@
   </si>
   <si>
     <t>Spectral Radiative Flux (WL - 700W)</t>
+  </si>
+  <si>
+    <t>Part. sz (W'worth) - Clay &lt;4um (%)</t>
+  </si>
+  <si>
+    <t>Part. sz (W'worth) - Silt v fine silt &gt;4 - &lt;8um (%)</t>
+  </si>
+  <si>
+    <t>Part. sz (W''worth) - Silt fine silt &gt;8 - &lt;16um (%)</t>
+  </si>
+  <si>
+    <t>Part. sz (W''worth) - Silt medium &gt;16 - &lt;31um (%)</t>
+  </si>
+  <si>
+    <t>Part. sz (W''worth) - Silt coarse &gt;31 - &lt;63um (%)</t>
+  </si>
+  <si>
+    <t>Part. sz (W''worth) - Silt  &gt;4 - &lt;63um (%)</t>
+  </si>
+  <si>
+    <t>Part. sz (W'worth) - Sand v fine &gt;63 - &lt;=125um (%)</t>
+  </si>
+  <si>
+    <t>Part. sz (W'worth) - Sand fine &gt;125 - &lt;=250um (%)</t>
+  </si>
+  <si>
+    <t>Part. sz (W'worth) - Sand med &gt;250 - &lt;=500um (%)</t>
+  </si>
+  <si>
+    <t>Part. sz (W'worth) - Sand coarse &gt;500um-&lt;=1mm (%)</t>
+  </si>
+  <si>
+    <t>var00364</t>
+  </si>
+  <si>
+    <t>Part. sz (W'worth) - Sand v coarse &gt;1 - &lt;=2mm (%)</t>
+  </si>
+  <si>
+    <t>var00365</t>
+  </si>
+  <si>
+    <t>Part. sz (W''worth) - Sand &gt;63 - &lt;2000um (%)</t>
+  </si>
+  <si>
+    <t>var00366</t>
+  </si>
+  <si>
+    <t>Part. sz (W'worth) - Gravel &gt;2mm (%)</t>
   </si>
 </sst>
 </file>
@@ -13409,10 +13457,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L344"/>
+  <dimension ref="A1:L357"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="B186" sqref="B186"/>
+    <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -21453,6 +21501,305 @@
       </c>
       <c r="K344" s="2" t="s">
         <v>1459</v>
+      </c>
+    </row>
+    <row r="345" spans="1:11">
+      <c r="A345" s="6" t="s">
+        <v>972</v>
+      </c>
+      <c r="B345" s="6" t="s">
+        <v>2036</v>
+      </c>
+      <c r="C345" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D345" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E345" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="H345" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="K345" s="6" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="346" spans="1:11">
+      <c r="A346" s="6" t="s">
+        <v>974</v>
+      </c>
+      <c r="B346" s="6" t="s">
+        <v>2037</v>
+      </c>
+      <c r="C346" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D346" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E346" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="H346" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="K346" s="6" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="347" spans="1:11">
+      <c r="A347" s="6" t="s">
+        <v>976</v>
+      </c>
+      <c r="B347" s="6" t="s">
+        <v>2038</v>
+      </c>
+      <c r="C347" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D347" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E347" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="H347" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="K347" s="6" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="348" spans="1:11">
+      <c r="A348" s="6" t="s">
+        <v>978</v>
+      </c>
+      <c r="B348" s="6" t="s">
+        <v>2039</v>
+      </c>
+      <c r="C348" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D348" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E348" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="H348" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="K348" s="6" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="349" spans="1:11">
+      <c r="A349" s="6" t="s">
+        <v>980</v>
+      </c>
+      <c r="B349" s="6" t="s">
+        <v>2040</v>
+      </c>
+      <c r="C349" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D349" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E349" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="H349" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="K349" s="6" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="350" spans="1:11">
+      <c r="A350" s="6" t="s">
+        <v>982</v>
+      </c>
+      <c r="B350" s="6" t="s">
+        <v>2041</v>
+      </c>
+      <c r="C350" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D350" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E350" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="H350" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="K350" s="6" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="351" spans="1:11">
+      <c r="A351" s="6" t="s">
+        <v>984</v>
+      </c>
+      <c r="B351" s="6" t="s">
+        <v>2042</v>
+      </c>
+      <c r="C351" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D351" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E351" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="H351" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="K351" s="6" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="352" spans="1:11">
+      <c r="A352" s="6" t="s">
+        <v>986</v>
+      </c>
+      <c r="B352" s="6" t="s">
+        <v>2043</v>
+      </c>
+      <c r="C352" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D352" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E352" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="H352" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="K352" s="6" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="353" spans="1:11">
+      <c r="A353" s="6" t="s">
+        <v>988</v>
+      </c>
+      <c r="B353" s="6" t="s">
+        <v>2044</v>
+      </c>
+      <c r="C353" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D353" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E353" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="H353" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="K353" s="6" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="354" spans="1:11">
+      <c r="A354" s="6" t="s">
+        <v>990</v>
+      </c>
+      <c r="B354" s="6" t="s">
+        <v>2045</v>
+      </c>
+      <c r="C354" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D354" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E354" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="H354" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="K354" s="6" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="355" spans="1:11">
+      <c r="A355" s="6" t="s">
+        <v>2046</v>
+      </c>
+      <c r="B355" s="6" t="s">
+        <v>2047</v>
+      </c>
+      <c r="C355" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D355" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E355" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="H355" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="K355" s="6" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="356" spans="1:11">
+      <c r="A356" s="6" t="s">
+        <v>2048</v>
+      </c>
+      <c r="B356" s="6" t="s">
+        <v>2049</v>
+      </c>
+      <c r="C356" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D356" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E356" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="H356" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="K356" s="6" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="357" spans="1:11">
+      <c r="A357" s="6" t="s">
+        <v>2050</v>
+      </c>
+      <c r="B357" s="6" t="s">
+        <v>2051</v>
+      </c>
+      <c r="C357" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D357" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E357" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="H357" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="K357" s="6" t="s">
+        <v>1318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BMT SWAN data import code added
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loxte\Downloads\Wednesday excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loxte\Downloads\8_4_24Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD00053A-C0ED-4A3C-96D1-60A69CB80D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF146D48-23CE-4A4C-87D0-5D86E447F4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -25,24 +25,25 @@
     <sheet name="WWMSP5" sheetId="10" r:id="rId10"/>
     <sheet name="WWMSP3SGREST" sheetId="29" r:id="rId11"/>
     <sheet name="WWMSP5Waves" sheetId="30" r:id="rId12"/>
-    <sheet name="WWMSP3SEDPSD" sheetId="28" r:id="rId13"/>
-    <sheet name="THEME3CTD" sheetId="11" r:id="rId14"/>
-    <sheet name="WWMSP2" sheetId="12" r:id="rId15"/>
-    <sheet name="THEME2LIGHT" sheetId="13" r:id="rId16"/>
-    <sheet name="MAFRL" sheetId="14" r:id="rId17"/>
-    <sheet name="IMOSBGC" sheetId="15" r:id="rId18"/>
-    <sheet name="IMOSPROFILE" sheetId="16" r:id="rId19"/>
-    <sheet name="DWER" sheetId="17" r:id="rId20"/>
-    <sheet name="DWERMOORING" sheetId="18" r:id="rId21"/>
-    <sheet name="BOM" sheetId="19" r:id="rId22"/>
-    <sheet name="DOT" sheetId="20" r:id="rId23"/>
-    <sheet name="WWM" sheetId="21" r:id="rId24"/>
-    <sheet name="JPPLAWAC" sheetId="22" r:id="rId25"/>
-    <sheet name="UWA" sheetId="23" r:id="rId26"/>
-    <sheet name="BMTBNA" sheetId="24" r:id="rId27"/>
-    <sheet name="FPA_BMT" sheetId="25" r:id="rId28"/>
-    <sheet name="WC_BMT" sheetId="26" r:id="rId29"/>
-    <sheet name="SentientHubs" sheetId="27" r:id="rId30"/>
+    <sheet name="BMT-SWAN" sheetId="31" r:id="rId13"/>
+    <sheet name="WWMSP3SEDPSD" sheetId="28" r:id="rId14"/>
+    <sheet name="THEME3CTD" sheetId="11" r:id="rId15"/>
+    <sheet name="WWMSP2" sheetId="12" r:id="rId16"/>
+    <sheet name="THEME2LIGHT" sheetId="13" r:id="rId17"/>
+    <sheet name="MAFRL" sheetId="14" r:id="rId18"/>
+    <sheet name="IMOSBGC" sheetId="15" r:id="rId19"/>
+    <sheet name="IMOSPROFILE" sheetId="16" r:id="rId20"/>
+    <sheet name="DWER" sheetId="17" r:id="rId21"/>
+    <sheet name="DWERMOORING" sheetId="18" r:id="rId22"/>
+    <sheet name="BOM" sheetId="19" r:id="rId23"/>
+    <sheet name="DOT" sheetId="20" r:id="rId24"/>
+    <sheet name="WWM" sheetId="21" r:id="rId25"/>
+    <sheet name="JPPLAWAC" sheetId="22" r:id="rId26"/>
+    <sheet name="UWA" sheetId="23" r:id="rId27"/>
+    <sheet name="BMTBNA" sheetId="24" r:id="rId28"/>
+    <sheet name="FPA_BMT" sheetId="25" r:id="rId29"/>
+    <sheet name="WC_BMT" sheetId="26" r:id="rId30"/>
+    <sheet name="SentientHubs" sheetId="27" r:id="rId31"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">'MASTER KEY'!$A$1:$L$319</definedName>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5091" uniqueCount="2060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5102" uniqueCount="2062">
   <si>
     <t>//</t>
   </si>
@@ -6371,6 +6372,12 @@
   </si>
   <si>
     <t>COMEBACK TO</t>
+  </si>
+  <si>
+    <t>DIR</t>
+  </si>
+  <si>
+    <t>TPER</t>
   </si>
 </sst>
 </file>
@@ -7643,8 +7650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2CA83D-4699-4CCB-99EF-A91382D8DEB3}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="A1:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7717,6 +7724,83 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F35DC7-0D53-4798-9745-A37E709CB4BD}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2060</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="D2" t="str">
+        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B1219,2,TRUE)</f>
+        <v>Peak Wave Direction</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="D3" t="str">
+        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B1219,2,TRUE)</f>
+        <v>Significant Wave Height</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>2061</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="D4" t="str">
+        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B1219,2,TRUE)</f>
+        <v>Peak Wave Period</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E23F14F-096E-466F-8721-D24D64E4AB52}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -7963,7 +8047,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -8179,7 +8263,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -8586,7 +8670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -8989,7 +9073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -10921,7 +11005,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -12074,372 +12158,6 @@
       </c>
       <c r="D73" t="e">
         <f>VLOOKUP(C73,'MASTER KEY'!$A$2:$B994,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:D23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A2" t="s">
-        <v>501</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="D2" t="str">
-        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B923,2,FALSE)</f>
-        <v>PRESSURE</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A3" t="s">
-        <v>503</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>504</v>
-      </c>
-      <c r="D3" t="e">
-        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B924,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A4" t="s">
-        <v>233</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D4" t="str">
-        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B925,2,FALSE)</f>
-        <v>Temperature</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A5" t="s">
-        <v>505</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>504</v>
-      </c>
-      <c r="D5" t="e">
-        <f>VLOOKUP(C5,'MASTER KEY'!$A$2:$B926,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A6" t="s">
-        <v>506</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D6" t="str">
-        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B927,2,FALSE)</f>
-        <v>Salinity</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A7" t="s">
-        <v>507</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>504</v>
-      </c>
-      <c r="D7" t="e">
-        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B928,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A8" t="s">
-        <v>508</v>
-      </c>
-      <c r="B8" s="14">
-        <f>32/1000</f>
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="D8" t="str">
-        <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B929,2,FALSE)</f>
-        <v>Dissolved Oxygen</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A9" t="s">
-        <v>509</v>
-      </c>
-      <c r="B9" s="4">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>504</v>
-      </c>
-      <c r="D9" t="e">
-        <f>VLOOKUP(C9,'MASTER KEY'!$A$2:$B930,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A10" t="s">
-        <v>510</v>
-      </c>
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="D10" t="str">
-        <f>VLOOKUP(C10,'MASTER KEY'!$A$2:$B931,2,FALSE)</f>
-        <v>Turbidity</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A11" t="s">
-        <v>511</v>
-      </c>
-      <c r="B11" s="4">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>504</v>
-      </c>
-      <c r="D11" t="e">
-        <f>VLOOKUP(C11,'MASTER KEY'!$A$2:$B932,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A12" t="s">
-        <v>512</v>
-      </c>
-      <c r="B12" s="4">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>504</v>
-      </c>
-      <c r="D12" t="e">
-        <f>VLOOKUP(C12,'MASTER KEY'!$A$2:$B933,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A13" t="s">
-        <v>513</v>
-      </c>
-      <c r="B13" s="4">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>504</v>
-      </c>
-      <c r="D13" t="e">
-        <f>VLOOKUP(C13,'MASTER KEY'!$A$2:$B934,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A14" t="s">
-        <v>514</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>504</v>
-      </c>
-      <c r="D14" t="e">
-        <f>VLOOKUP(C14,'MASTER KEY'!$A$2:$B935,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A15" t="s">
-        <v>515</v>
-      </c>
-      <c r="B15" s="4">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>504</v>
-      </c>
-      <c r="D15" t="e">
-        <f>VLOOKUP(C15,'MASTER KEY'!$A$2:$B936,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A16" t="s">
-        <v>516</v>
-      </c>
-      <c r="B16" s="4">
-        <v>1</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="D16" t="str">
-        <f>VLOOKUP(C16,'MASTER KEY'!$A$2:$B937,2,FALSE)</f>
-        <v>Chlorophyll-a</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A17" t="s">
-        <v>517</v>
-      </c>
-      <c r="B17" s="4">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>504</v>
-      </c>
-      <c r="D17" t="e">
-        <f>VLOOKUP(C17,'MASTER KEY'!$A$2:$B938,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A18" t="s">
-        <v>518</v>
-      </c>
-      <c r="B18" s="4">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D18" t="str">
-        <f>VLOOKUP(C18,'MASTER KEY'!$A$2:$B939,2,FALSE)</f>
-        <v>Specific Conductivity</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A19" t="s">
-        <v>519</v>
-      </c>
-      <c r="B19" s="4">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>504</v>
-      </c>
-      <c r="D19" t="e">
-        <f>VLOOKUP(C19,'MASTER KEY'!$A$2:$B940,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A20" t="s">
-        <v>520</v>
-      </c>
-      <c r="B20" s="4">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="D20" t="e">
-        <f>VLOOKUP(C20,'MASTER KEY'!$A$2:$B941,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A21" t="s">
-        <v>521</v>
-      </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>504</v>
-      </c>
-      <c r="D21" t="e">
-        <f>VLOOKUP(C21,'MASTER KEY'!$A$2:$B942,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A22" t="s">
-        <v>522</v>
-      </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="D22" t="str">
-        <f>VLOOKUP(C22,'MASTER KEY'!$A$2:$B943,2,FALSE)</f>
-        <v>Density</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A23" t="s">
-        <v>524</v>
-      </c>
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>504</v>
-      </c>
-      <c r="D23" t="e">
-        <f>VLOOKUP(C23,'MASTER KEY'!$A$2:$B944,2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -20885,6 +20603,372 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A2" t="s">
+        <v>501</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="D2" t="str">
+        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B923,2,FALSE)</f>
+        <v>PRESSURE</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A3" t="s">
+        <v>503</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>504</v>
+      </c>
+      <c r="D3" t="e">
+        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B924,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" t="str">
+        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B925,2,FALSE)</f>
+        <v>Temperature</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A5" t="s">
+        <v>505</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>504</v>
+      </c>
+      <c r="D5" t="e">
+        <f>VLOOKUP(C5,'MASTER KEY'!$A$2:$B926,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A6" t="s">
+        <v>506</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D6" t="str">
+        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B927,2,FALSE)</f>
+        <v>Salinity</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A7" t="s">
+        <v>507</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>504</v>
+      </c>
+      <c r="D7" t="e">
+        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B928,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A8" t="s">
+        <v>508</v>
+      </c>
+      <c r="B8" s="14">
+        <f>32/1000</f>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D8" t="str">
+        <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B929,2,FALSE)</f>
+        <v>Dissolved Oxygen</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>504</v>
+      </c>
+      <c r="D9" t="e">
+        <f>VLOOKUP(C9,'MASTER KEY'!$A$2:$B930,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A10" t="s">
+        <v>510</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="D10" t="str">
+        <f>VLOOKUP(C10,'MASTER KEY'!$A$2:$B931,2,FALSE)</f>
+        <v>Turbidity</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A11" t="s">
+        <v>511</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>504</v>
+      </c>
+      <c r="D11" t="e">
+        <f>VLOOKUP(C11,'MASTER KEY'!$A$2:$B932,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A12" t="s">
+        <v>512</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>504</v>
+      </c>
+      <c r="D12" t="e">
+        <f>VLOOKUP(C12,'MASTER KEY'!$A$2:$B933,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A13" t="s">
+        <v>513</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>504</v>
+      </c>
+      <c r="D13" t="e">
+        <f>VLOOKUP(C13,'MASTER KEY'!$A$2:$B934,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A14" t="s">
+        <v>514</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>504</v>
+      </c>
+      <c r="D14" t="e">
+        <f>VLOOKUP(C14,'MASTER KEY'!$A$2:$B935,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A15" t="s">
+        <v>515</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>504</v>
+      </c>
+      <c r="D15" t="e">
+        <f>VLOOKUP(C15,'MASTER KEY'!$A$2:$B936,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A16" t="s">
+        <v>516</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="D16" t="str">
+        <f>VLOOKUP(C16,'MASTER KEY'!$A$2:$B937,2,FALSE)</f>
+        <v>Chlorophyll-a</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A17" t="s">
+        <v>517</v>
+      </c>
+      <c r="B17" s="4">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>504</v>
+      </c>
+      <c r="D17" t="e">
+        <f>VLOOKUP(C17,'MASTER KEY'!$A$2:$B938,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A18" t="s">
+        <v>518</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="D18" t="str">
+        <f>VLOOKUP(C18,'MASTER KEY'!$A$2:$B939,2,FALSE)</f>
+        <v>Specific Conductivity</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A19" t="s">
+        <v>519</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>504</v>
+      </c>
+      <c r="D19" t="e">
+        <f>VLOOKUP(C19,'MASTER KEY'!$A$2:$B940,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A20" t="s">
+        <v>520</v>
+      </c>
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="D20" t="e">
+        <f>VLOOKUP(C20,'MASTER KEY'!$A$2:$B941,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A21" t="s">
+        <v>521</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>504</v>
+      </c>
+      <c r="D21" t="e">
+        <f>VLOOKUP(C21,'MASTER KEY'!$A$2:$B942,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A22" t="s">
+        <v>522</v>
+      </c>
+      <c r="B22" s="4">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="D22" t="str">
+        <f>VLOOKUP(C22,'MASTER KEY'!$A$2:$B943,2,FALSE)</f>
+        <v>Density</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A23" t="s">
+        <v>524</v>
+      </c>
+      <c r="B23" s="4">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>504</v>
+      </c>
+      <c r="D23" t="e">
+        <f>VLOOKUP(C23,'MASTER KEY'!$A$2:$B944,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -21546,7 +21630,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -21924,7 +22008,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -22483,7 +22567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -22875,7 +22959,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -22989,7 +23073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -23295,7 +23379,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -23527,7 +23611,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -23702,7 +23786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -23842,132 +23926,6 @@
       </c>
       <c r="D8" t="str">
         <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B926,2,FALSE)</f>
-        <v>Current Velocity</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D2" t="str">
-        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B920,2,FALSE)</f>
-        <v>Water Surface Height</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A3" t="s">
-        <v>229</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D3" t="str">
-        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B921,2,FALSE)</f>
-        <v>Current Velocity (x component)</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A4" t="s">
-        <v>231</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D4" t="str">
-        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B922,2,FALSE)</f>
-        <v>Current Velocity (y component)</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A5" t="s">
-        <v>233</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D5" t="str">
-        <f>VLOOKUP(C5,'MASTER KEY'!$A$2:$B923,2,FALSE)</f>
-        <v>Temperature</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A6" t="s">
-        <v>235</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D6" t="str">
-        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B924,2,FALSE)</f>
-        <v>Salinity</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1">
-      <c r="A7" t="s">
-        <v>237</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D7" t="str">
-        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B925,2,FALSE)</f>
         <v>Current Velocity</v>
       </c>
     </row>
@@ -24043,6 +24001,132 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D2" t="str">
+        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B920,2,FALSE)</f>
+        <v>Water Surface Height</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" t="str">
+        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B921,2,FALSE)</f>
+        <v>Current Velocity (x component)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D4" t="str">
+        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B922,2,FALSE)</f>
+        <v>Current Velocity (y component)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D5" t="str">
+        <f>VLOOKUP(C5,'MASTER KEY'!$A$2:$B923,2,FALSE)</f>
+        <v>Temperature</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A6" t="s">
+        <v>235</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D6" t="str">
+        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B924,2,FALSE)</f>
+        <v>Salinity</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A7" t="s">
+        <v>237</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D7" t="str">
+        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B925,2,FALSE)</f>
+        <v>Current Velocity</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>

</xml_diff>

<commit_message>
Fixed up WRF properly, now its finished
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loxte\Downloads\19-04-2024 WAMSI WORK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loxte\Downloads\22_04_2024 wamsi work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570A11EC-C3D1-4DD7-8273-61340CC4ADB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BB23D8-FBF6-4BAC-917E-8CF0046B1061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2772" windowWidth="17280" windowHeight="8880" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5219" uniqueCount="2088">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5236" uniqueCount="2094">
   <si>
     <t>//</t>
   </si>
@@ -6456,6 +6456,24 @@
   </si>
   <si>
     <t>maximum cloud cover</t>
+  </si>
+  <si>
+    <t>var00383</t>
+  </si>
+  <si>
+    <t>Precipitation Rate</t>
+  </si>
+  <si>
+    <t>precipitation_rate</t>
+  </si>
+  <si>
+    <t>var00384</t>
+  </si>
+  <si>
+    <t>Air Pressure</t>
+  </si>
+  <si>
+    <t>RAINNCRATE</t>
   </si>
 </sst>
 </file>
@@ -6601,7 +6619,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6661,6 +6679,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6748,7 +6772,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6916,7 +6940,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12293,11 +12321,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L367"/>
+  <dimension ref="A1:L369"/>
   <sheetViews>
     <sheetView zoomScale="66" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A343" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F372" sqref="F372"/>
+      <pane ySplit="1" topLeftCell="A352" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A369" sqref="A369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20902,39 +20930,39 @@
         <v>2053</v>
       </c>
     </row>
-    <row r="366" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A366" s="55" t="s">
+    <row r="366" spans="1:12" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A366" s="59" t="s">
         <v>2078</v>
       </c>
-      <c r="B366" s="59" t="s">
+      <c r="B366" s="60" t="s">
         <v>2087</v>
       </c>
-      <c r="C366" s="55" t="s">
+      <c r="C366" s="59" t="s">
         <v>1104</v>
       </c>
-      <c r="D366" s="55" t="s">
+      <c r="D366" s="59" t="s">
         <v>1104</v>
       </c>
-      <c r="E366" s="55" t="s">
+      <c r="E366" s="59" t="s">
         <v>2053</v>
       </c>
-      <c r="F366" s="55" t="s">
+      <c r="F366" s="59" t="s">
         <v>2053</v>
       </c>
-      <c r="G366" s="55" t="s">
+      <c r="G366" s="59" t="s">
         <v>2053</v>
       </c>
-      <c r="H366" s="55" t="s">
+      <c r="H366" s="59" t="s">
         <v>2053</v>
       </c>
-      <c r="I366" s="55" t="s">
+      <c r="I366" s="59" t="s">
         <v>2053</v>
       </c>
-      <c r="J366" s="55"/>
-      <c r="K366" s="55" t="s">
+      <c r="J366" s="59"/>
+      <c r="K366" s="59" t="s">
         <v>2053</v>
       </c>
-      <c r="L366" s="55" t="s">
+      <c r="L366" s="59" t="s">
         <v>2053</v>
       </c>
     </row>
@@ -20972,6 +21000,55 @@
       </c>
       <c r="L367" s="55" t="s">
         <v>2053</v>
+      </c>
+    </row>
+    <row r="368" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A368" s="2" t="s">
+        <v>2088</v>
+      </c>
+      <c r="B368" s="2" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C368" s="17" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E368" s="2" t="s">
+        <v>1164</v>
+      </c>
+      <c r="F368" s="2" t="s">
+        <v>2090</v>
+      </c>
+      <c r="G368" s="2" t="s">
+        <v>1793</v>
+      </c>
+      <c r="H368" s="2" t="s">
+        <v>1794</v>
+      </c>
+      <c r="I368" s="44" t="s">
+        <v>1180</v>
+      </c>
+      <c r="K368" s="2" t="s">
+        <v>1732</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A369" s="6" t="s">
+        <v>2091</v>
+      </c>
+      <c r="B369" s="6" t="s">
+        <v>2092</v>
+      </c>
+      <c r="C369" s="6" t="s">
+        <v>1851</v>
+      </c>
+      <c r="D369" s="6" t="s">
+        <v>1851</v>
+      </c>
+      <c r="E369" s="6" t="s">
+        <v>1851</v>
+      </c>
+      <c r="F369" s="6" t="s">
+        <v>1850</v>
       </c>
     </row>
   </sheetData>
@@ -25708,14 +25785,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
     <col min="4" max="4" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -25741,15 +25819,14 @@
         <v>2056</v>
       </c>
       <c r="B2">
-        <f>1/100</f>
-        <v>0.01</v>
-      </c>
-      <c r="C2" s="57" t="s">
-        <v>382</v>
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2091</v>
       </c>
       <c r="D2" t="str">
         <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B1221,2,TRUE)</f>
-        <v>Station Level Pressure</v>
+        <v>Air Pressure</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -25787,7 +25864,8 @@
         <v>2059</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <f>1/1000</f>
+        <v>1E-3</v>
       </c>
       <c r="C5" s="57" t="s">
         <v>330</v>
@@ -25799,186 +25877,202 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2060</v>
+        <v>2093</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>333</v>
+        <v>2088</v>
       </c>
       <c r="D6" t="str">
-        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B1225,2,TRUE)</f>
-        <v>Air Temperature</v>
+        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B1224,2,TRUE)</f>
+        <v>Precipitation Rate</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>2060</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>333</v>
+      </c>
+      <c r="D7" t="str">
+        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B1225,2,TRUE)</f>
+        <v>Air Temperature</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>2061</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>2072</v>
       </c>
-      <c r="D7" t="str">
-        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B1226,2,TRUE)</f>
+      <c r="D8" t="str">
+        <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B1226,2,TRUE)</f>
         <v>Specific humidity at 2m height</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A8" s="54" t="s">
+    <row r="9" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A9" s="54" t="s">
         <v>2062</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>2073</v>
       </c>
-      <c r="D8" t="str">
-        <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B1227,2,TRUE)</f>
+      <c r="D9" t="str">
+        <f>VLOOKUP(C9,'MASTER KEY'!$A$2:$B1227,2,TRUE)</f>
         <v>Sensible heat flux</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
-        <v>2063</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>2074</v>
-      </c>
-      <c r="D9" t="str">
-        <f>VLOOKUP(C9,'MASTER KEY'!$A$2:$B1228,2,TRUE)</f>
-        <v xml:space="preserve">Latent heat flux </v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
+        <v>2063</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>2074</v>
+      </c>
+      <c r="D10" t="str">
+        <f>VLOOKUP(C10,'MASTER KEY'!$A$2:$B1228,2,TRUE)</f>
+        <v xml:space="preserve">Latent heat flux </v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
         <v>2064</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>2075</v>
       </c>
-      <c r="D10" t="str">
-        <f>VLOOKUP(C10,'MASTER KEY'!$A$2:$B1229,2,TRUE)</f>
+      <c r="D11" t="str">
+        <f>VLOOKUP(C11,'MASTER KEY'!$A$2:$B1229,2,TRUE)</f>
         <v>sea surface temperature</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>2065</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="58" t="s">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="58" t="s">
         <v>339</v>
       </c>
-      <c r="D11" t="str">
-        <f>VLOOKUP(C11,'MASTER KEY'!$A$2:$B1230,2,TRUE)</f>
+      <c r="D12" t="str">
+        <f>VLOOKUP(C12,'MASTER KEY'!$A$2:$B1230,2,TRUE)</f>
         <v>Relative Humidity</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>2066</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>2076</v>
-      </c>
-      <c r="D12" t="str">
-        <f>VLOOKUP(C12,'MASTER KEY'!$A$2:$B1231,2,TRUE)</f>
-        <v>eastern wind speed at 10 m height</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="D13" t="str">
-        <f>VLOOKUP(C13,'MASTER KEY'!$A$2:$B1232,2,TRUE)</f>
-        <v>northern wind speed at 10 m height</v>
+        <f>VLOOKUP(C13,'MASTER KEY'!$A$2:$B1231,2,TRUE)</f>
+        <v>eastern wind speed at 10 m height</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="58" t="s">
-        <v>268</v>
+      <c r="C14" s="6" t="s">
+        <v>2077</v>
       </c>
       <c r="D14" t="str">
-        <f>VLOOKUP(C14,'MASTER KEY'!$A$2:$B1233,2,TRUE)</f>
-        <v>Wind Speed</v>
+        <f>VLOOKUP(C14,'MASTER KEY'!$A$2:$B1232,2,TRUE)</f>
+        <v>northern wind speed at 10 m height</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" s="58" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D15" t="str">
-        <f>VLOOKUP(C15,'MASTER KEY'!$A$2:$B1234,2,TRUE)</f>
-        <v>Wind Direction</v>
+        <f>VLOOKUP(C15,'MASTER KEY'!$A$2:$B1233,2,TRUE)</f>
+        <v>Wind Speed</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>2078</v>
+      <c r="C16" s="58" t="s">
+        <v>270</v>
       </c>
       <c r="D16" t="str">
-        <f>VLOOKUP(C16,'MASTER KEY'!$A$2:$B1235,2,TRUE)</f>
-        <v>maximum cloud cover</v>
+        <f>VLOOKUP(C16,'MASTER KEY'!$A$2:$B1234,2,TRUE)</f>
+        <v>Wind Direction</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>2070</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="D17" t="str">
+        <f>VLOOKUP(C17,'MASTER KEY'!$A$2:$B1235,2,TRUE)</f>
+        <v>Cloud Cover</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>2071</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>2079</v>
       </c>
-      <c r="D17" t="str">
-        <f>VLOOKUP(C17,'MASTER KEY'!$A$2:$B1236,2,TRUE)</f>
+      <c r="D18" t="str">
+        <f>VLOOKUP(C18,'MASTER KEY'!$A$2:$B1236,2,TRUE)</f>
         <v>RAINV</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added code to import BOM BARRA data
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loxte\Downloads\22_04_2024 wamsi work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BB23D8-FBF6-4BAC-917E-8CF0046B1061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F786E5F0-CC3F-46BF-B84B-C5E67F045F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,34 +16,35 @@
     <sheet name="Information" sheetId="1" r:id="rId1"/>
     <sheet name="MASTER KEY" sheetId="2" r:id="rId2"/>
     <sheet name="IMOSSRS" sheetId="3" r:id="rId3"/>
-    <sheet name="WWMSP1.1-WRF" sheetId="4" r:id="rId4"/>
-    <sheet name="THEME2.2" sheetId="5" r:id="rId5"/>
-    <sheet name="Model_TFV" sheetId="6" r:id="rId6"/>
-    <sheet name="FPA-MQMP" sheetId="7" r:id="rId7"/>
-    <sheet name="THEME5" sheetId="8" r:id="rId8"/>
-    <sheet name="THEME5MET" sheetId="9" r:id="rId9"/>
-    <sheet name="WWMSP5" sheetId="10" r:id="rId10"/>
-    <sheet name="WWMSP3SGREST" sheetId="29" r:id="rId11"/>
-    <sheet name="WWMSP5Waves" sheetId="30" r:id="rId12"/>
-    <sheet name="BMT-SWAN" sheetId="31" r:id="rId13"/>
-    <sheet name="WWMSP3SEDPSD" sheetId="28" r:id="rId14"/>
-    <sheet name="THEME3CTD" sheetId="11" r:id="rId15"/>
-    <sheet name="WWMSP2" sheetId="12" r:id="rId16"/>
-    <sheet name="THEME2LIGHT" sheetId="13" r:id="rId17"/>
-    <sheet name="MAFRL" sheetId="14" r:id="rId18"/>
-    <sheet name="IMOSBGC" sheetId="15" r:id="rId19"/>
-    <sheet name="IMOSPROFILE" sheetId="16" r:id="rId20"/>
-    <sheet name="DWER" sheetId="17" r:id="rId21"/>
-    <sheet name="DWERMOORING" sheetId="18" r:id="rId22"/>
-    <sheet name="BOM" sheetId="19" r:id="rId23"/>
-    <sheet name="DOT" sheetId="20" r:id="rId24"/>
-    <sheet name="WWM" sheetId="21" r:id="rId25"/>
-    <sheet name="JPPLAWAC" sheetId="22" r:id="rId26"/>
-    <sheet name="UWA" sheetId="23" r:id="rId27"/>
-    <sheet name="BMTBNA" sheetId="24" r:id="rId28"/>
-    <sheet name="FPA_BMT" sheetId="25" r:id="rId29"/>
-    <sheet name="WC_BMT" sheetId="26" r:id="rId30"/>
-    <sheet name="SentientHubs" sheetId="27" r:id="rId31"/>
+    <sheet name="BOM-BARRA" sheetId="32" r:id="rId4"/>
+    <sheet name="WWMSP1.1-WRF" sheetId="4" r:id="rId5"/>
+    <sheet name="THEME2.2" sheetId="5" r:id="rId6"/>
+    <sheet name="Model_TFV" sheetId="6" r:id="rId7"/>
+    <sheet name="FPA-MQMP" sheetId="7" r:id="rId8"/>
+    <sheet name="THEME5" sheetId="8" r:id="rId9"/>
+    <sheet name="THEME5MET" sheetId="9" r:id="rId10"/>
+    <sheet name="WWMSP5" sheetId="10" r:id="rId11"/>
+    <sheet name="WWMSP3SGREST" sheetId="29" r:id="rId12"/>
+    <sheet name="WWMSP5Waves" sheetId="30" r:id="rId13"/>
+    <sheet name="BMT-SWAN" sheetId="31" r:id="rId14"/>
+    <sheet name="WWMSP3SEDPSD" sheetId="28" r:id="rId15"/>
+    <sheet name="THEME3CTD" sheetId="11" r:id="rId16"/>
+    <sheet name="WWMSP2" sheetId="12" r:id="rId17"/>
+    <sheet name="THEME2LIGHT" sheetId="13" r:id="rId18"/>
+    <sheet name="MAFRL" sheetId="14" r:id="rId19"/>
+    <sheet name="IMOSBGC" sheetId="15" r:id="rId20"/>
+    <sheet name="IMOSPROFILE" sheetId="16" r:id="rId21"/>
+    <sheet name="DWER" sheetId="17" r:id="rId22"/>
+    <sheet name="DWERMOORING" sheetId="18" r:id="rId23"/>
+    <sheet name="BOM" sheetId="19" r:id="rId24"/>
+    <sheet name="DOT" sheetId="20" r:id="rId25"/>
+    <sheet name="WWM" sheetId="21" r:id="rId26"/>
+    <sheet name="JPPLAWAC" sheetId="22" r:id="rId27"/>
+    <sheet name="UWA" sheetId="23" r:id="rId28"/>
+    <sheet name="BMTBNA" sheetId="24" r:id="rId29"/>
+    <sheet name="FPA_BMT" sheetId="25" r:id="rId30"/>
+    <sheet name="WC_BMT" sheetId="26" r:id="rId31"/>
+    <sheet name="SentientHubs" sheetId="27" r:id="rId32"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">'MASTER KEY'!$A$1:$L$319</definedName>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5236" uniqueCount="2094">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5287" uniqueCount="2105">
   <si>
     <t>//</t>
   </si>
@@ -6474,6 +6475,39 @@
   </si>
   <si>
     <t>RAINNCRATE</t>
+  </si>
+  <si>
+    <t>uwnd10m</t>
+  </si>
+  <si>
+    <t>vwnd10m</t>
+  </si>
+  <si>
+    <t>mslp</t>
+  </si>
+  <si>
+    <t>lwsfcdown</t>
+  </si>
+  <si>
+    <t>swsfcdown</t>
+  </si>
+  <si>
+    <t>temp_scrn</t>
+  </si>
+  <si>
+    <t>precip_rate</t>
+  </si>
+  <si>
+    <t>relhum</t>
+  </si>
+  <si>
+    <t>var00385</t>
+  </si>
+  <si>
+    <t>var00386</t>
+  </si>
+  <si>
+    <t>var00387</t>
   </si>
 </sst>
 </file>
@@ -6619,7 +6653,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6685,6 +6719,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6772,7 +6812,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6945,6 +6985,7 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="13" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7279,6 +7320,341 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>844</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D2" t="str">
+        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B916,2,FALSE)</f>
+        <v>Wind Speed</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>845</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D3" t="str">
+        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B917,2,FALSE)</f>
+        <v>Wind Direction</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>846</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>847</v>
+      </c>
+      <c r="D4" t="str">
+        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B918,2,FALSE)</f>
+        <v>Wind Direction (std)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>848</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D5" t="str">
+        <f>VLOOKUP(C5,'MASTER KEY'!$A$2:$B919,2,FALSE)</f>
+        <v>Wind Speed (max)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>849</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>850</v>
+      </c>
+      <c r="D6" t="str">
+        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B920,2,FALSE)</f>
+        <v>Wind Speed (min)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>851</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D7" t="str">
+        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B921,2,FALSE)</f>
+        <v>Station Level Pressure</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>852</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>853</v>
+      </c>
+      <c r="D8" t="str">
+        <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B922,2,FALSE)</f>
+        <v>Station Level Pressure (max)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>854</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>855</v>
+      </c>
+      <c r="D9" t="str">
+        <f>VLOOKUP(C9,'MASTER KEY'!$A$2:$B923,2,FALSE)</f>
+        <v>Station Level Pressure (min)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>856</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>857</v>
+      </c>
+      <c r="D10" t="str">
+        <f>VLOOKUP(C10,'MASTER KEY'!$A$2:$B924,2,FALSE)</f>
+        <v>Station Level Pressure (std)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>858</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>859</v>
+      </c>
+      <c r="D11" t="str">
+        <f>VLOOKUP(C11,'MASTER KEY'!$A$2:$B925,2,FALSE)</f>
+        <v>Surface Solar Irradiance</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>860</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>861</v>
+      </c>
+      <c r="D12" t="str">
+        <f>VLOOKUP(C12,'MASTER KEY'!$A$2:$B926,2,FALSE)</f>
+        <v>Surface Solar Irradiance (max)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>862</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>863</v>
+      </c>
+      <c r="D13" t="str">
+        <f>VLOOKUP(C13,'MASTER KEY'!$A$2:$B927,2,FALSE)</f>
+        <v>Surface Solar Irradiance (min)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>864</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>865</v>
+      </c>
+      <c r="D14" t="str">
+        <f>VLOOKUP(C14,'MASTER KEY'!$A$2:$B928,2,FALSE)</f>
+        <v>Surface Solar Irradiance (std)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>866</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D15" t="str">
+        <f>VLOOKUP(C15,'MASTER KEY'!$A$2:$B929,2,FALSE)</f>
+        <v>Surface Photosynthetically Active Photon Flux</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>867</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>868</v>
+      </c>
+      <c r="D16" t="str">
+        <f>VLOOKUP(C16,'MASTER KEY'!$A$2:$B930,2,FALSE)</f>
+        <v>Surface Photosynthetically Active Photon Flux (max)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>869</v>
+      </c>
+      <c r="B17" s="4">
+        <v>1</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>870</v>
+      </c>
+      <c r="D17" t="str">
+        <f>VLOOKUP(C17,'MASTER KEY'!$A$2:$B931,2,FALSE)</f>
+        <v>Surface Photosynthetically Active Photon Flux (min)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>871</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>275</v>
+      </c>
+      <c r="D18" t="str">
+        <f>VLOOKUP(C18,'MASTER KEY'!$A$2:$B932,2,FALSE)</f>
+        <v>Surface Photosynthetically Active Photon Flux (std)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>872</v>
+      </c>
+      <c r="B19" s="4">
+        <f>4*24</f>
+        <v>96</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>873</v>
+      </c>
+      <c r="D19" t="str">
+        <f>VLOOKUP(C19,'MASTER KEY'!$A$2:$B933,2,FALSE)</f>
+        <v>Daily Solar Irradiance</v>
+      </c>
+      <c r="E19" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>875</v>
+      </c>
+      <c r="B20" s="4">
+        <f>4*24</f>
+        <v>96</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D20" t="str">
+        <f>VLOOKUP(C20,'MASTER KEY'!$A$2:$B934,2,FALSE)</f>
+        <v>Daily Surface Photosynthetically Active Photon Flux</v>
+      </c>
+      <c r="E20" t="s">
+        <v>874</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -7563,7 +7939,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD20BAA-AE37-4608-B486-3BB6A38AE87B}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -7796,7 +8172,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2CA83D-4699-4CCB-99EF-A91382D8DEB3}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -7873,7 +8249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F35DC7-0D53-4798-9745-A37E709CB4BD}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -7950,7 +8326,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E23F14F-096E-466F-8721-D24D64E4AB52}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -8197,7 +8573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -8413,7 +8789,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -8820,7 +9196,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -9223,7 +9599,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -11155,1177 +11531,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:G73"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>525</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="D2" t="str">
-        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B916,2,FALSE)</f>
-        <v>Secchi Depth</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>526</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D3" t="str">
-        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B917,2,FALSE)</f>
-        <v>Salinity</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>527</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>504</v>
-      </c>
-      <c r="D4" t="e">
-        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B918,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>528</v>
-      </c>
-      <c r="B5" s="25">
-        <v>1.2000000048E-2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="D5" t="str">
-        <f>VLOOKUP(C5,'MASTER KEY'!$A$2:$B919,2,FALSE)</f>
-        <v>Dissolved Inorganic Carbon</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>530</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>504</v>
-      </c>
-      <c r="D6" t="e">
-        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B920,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>531</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="D7" t="str">
-        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B921,2,FALSE)</f>
-        <v>Total Alkalinity</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>532</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>504</v>
-      </c>
-      <c r="D8" t="e">
-        <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B922,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>533</v>
-      </c>
-      <c r="B9" s="14">
-        <f>32/1000</f>
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="D9" t="str">
-        <f>VLOOKUP(C9,'MASTER KEY'!$A$2:$B923,2,FALSE)</f>
-        <v>Dissolved Oxygen</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>534</v>
-      </c>
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>504</v>
-      </c>
-      <c r="D10" t="e">
-        <f>VLOOKUP(C10,'MASTER KEY'!$A$2:$B924,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>535</v>
-      </c>
-      <c r="B11" s="26">
-        <v>1.4E-2</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="D11" t="str">
-        <f>VLOOKUP(C11,'MASTER KEY'!$A$2:$B925,2,FALSE)</f>
-        <v>Ammonium</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>536</v>
-      </c>
-      <c r="B12" s="4">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>504</v>
-      </c>
-      <c r="D12" t="e">
-        <f>VLOOKUP(C12,'MASTER KEY'!$A$2:$B926,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>537</v>
-      </c>
-      <c r="B13" s="26">
-        <v>1.4E-2</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="D13" t="str">
-        <f>VLOOKUP(C13,'MASTER KEY'!$A$2:$B927,2,FALSE)</f>
-        <v>Nitrate</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>538</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>504</v>
-      </c>
-      <c r="D14" t="e">
-        <f>VLOOKUP(C14,'MASTER KEY'!$A$2:$B928,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>539</v>
-      </c>
-      <c r="B15" s="26">
-        <v>1.4E-2</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="D15" t="str">
-        <f>VLOOKUP(C15,'MASTER KEY'!$A$2:$B929,2,FALSE)</f>
-        <v>Nitrite</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>541</v>
-      </c>
-      <c r="B16" s="4">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>504</v>
-      </c>
-      <c r="D16" t="e">
-        <f>VLOOKUP(C16,'MASTER KEY'!$A$2:$B930,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>542</v>
-      </c>
-      <c r="B17" s="14">
-        <v>3.1E-2</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="D17" t="str">
-        <f>VLOOKUP(C17,'MASTER KEY'!$A$2:$B931,2,FALSE)</f>
-        <v>Filterable Reactive Phosphate</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>543</v>
-      </c>
-      <c r="B18" s="4">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>504</v>
-      </c>
-      <c r="D18" t="e">
-        <f>VLOOKUP(C18,'MASTER KEY'!$A$2:$B932,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>544</v>
-      </c>
-      <c r="B19" s="14">
-        <v>2.81E-2</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="D19" t="str">
-        <f>VLOOKUP(C19,'MASTER KEY'!$A$2:$B933,2,FALSE)</f>
-        <v>Reactive Silica</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>545</v>
-      </c>
-      <c r="B20" s="4">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>504</v>
-      </c>
-      <c r="D20" t="e">
-        <f>VLOOKUP(C20,'MASTER KEY'!$A$2:$B934,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>546</v>
-      </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="D21" t="str">
-        <f>VLOOKUP(C21,'MASTER KEY'!$A$2:$B935,2,FALSE)</f>
-        <v>TSSorganic</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>548</v>
-      </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="D22" t="str">
-        <f>VLOOKUP(C22,'MASTER KEY'!$A$2:$B936,2,FALSE)</f>
-        <v>TSSinorganic</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>550</v>
-      </c>
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="D23" t="str">
-        <f>VLOOKUP(C23,'MASTER KEY'!$A$2:$B937,2,FALSE)</f>
-        <v>Total Suspended Solids</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>551</v>
-      </c>
-      <c r="B24" s="4">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>504</v>
-      </c>
-      <c r="D24" t="e">
-        <f>VLOOKUP(C24,'MASTER KEY'!$A$2:$B938,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>552</v>
-      </c>
-      <c r="B25" s="4">
-        <v>1</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="D25" t="str">
-        <f>VLOOKUP(C25,'MASTER KEY'!$A$2:$B939,2,FALSE)</f>
-        <v>Prochlorococcus</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>554</v>
-      </c>
-      <c r="B26" s="4">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>504</v>
-      </c>
-      <c r="D26" t="e">
-        <f>VLOOKUP(C26,'MASTER KEY'!$A$2:$B940,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>555</v>
-      </c>
-      <c r="B27" s="4">
-        <v>1</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="D27" t="str">
-        <f>VLOOKUP(C27,'MASTER KEY'!$A$2:$B941,2,FALSE)</f>
-        <v>Synechococcus</v>
-      </c>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>557</v>
-      </c>
-      <c r="B28" s="4">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>504</v>
-      </c>
-      <c r="D28" t="e">
-        <f>VLOOKUP(C28,'MASTER KEY'!$A$2:$B942,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>558</v>
-      </c>
-      <c r="B29" s="4">
-        <v>1</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>559</v>
-      </c>
-      <c r="D29" t="str">
-        <f>VLOOKUP(C29,'MASTER KEY'!$A$2:$B943,2,FALSE)</f>
-        <v>Picoeukaryotes</v>
-      </c>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>560</v>
-      </c>
-      <c r="B30" s="4">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>504</v>
-      </c>
-      <c r="D30" t="e">
-        <f>VLOOKUP(C30,'MASTER KEY'!$A$2:$B944,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>561</v>
-      </c>
-      <c r="B31" s="4">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>562</v>
-      </c>
-      <c r="D31" t="str">
-        <f>VLOOKUP(C31,'MASTER KEY'!$A$2:$B945,2,FALSE)</f>
-        <v>Allo</v>
-      </c>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>563</v>
-      </c>
-      <c r="B32" s="4">
-        <v>1</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="D32" t="str">
-        <f>VLOOKUP(C32,'MASTER KEY'!$A$2:$B946,2,FALSE)</f>
-        <v>AlphaBetaCar</v>
-      </c>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>565</v>
-      </c>
-      <c r="B33" s="4">
-        <v>1</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="D33" t="str">
-        <f>VLOOKUP(C33,'MASTER KEY'!$A$2:$B947,2,FALSE)</f>
-        <v>Anth</v>
-      </c>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>567</v>
-      </c>
-      <c r="B34" s="4">
-        <v>1</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>568</v>
-      </c>
-      <c r="D34" t="str">
-        <f>VLOOKUP(C34,'MASTER KEY'!$A$2:$B948,2,FALSE)</f>
-        <v>Asta</v>
-      </c>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>569</v>
-      </c>
-      <c r="B35" s="4">
-        <v>1</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="D35" t="str">
-        <f>VLOOKUP(C35,'MASTER KEY'!$A$2:$B949,2,FALSE)</f>
-        <v>BetaBetaCar</v>
-      </c>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>571</v>
-      </c>
-      <c r="B36" s="4">
-        <v>1</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>572</v>
-      </c>
-      <c r="D36" t="str">
-        <f>VLOOKUP(C36,'MASTER KEY'!$A$2:$B950,2,FALSE)</f>
-        <v>BetaEpiCar</v>
-      </c>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>573</v>
-      </c>
-      <c r="B37" s="4">
-        <v>1</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>574</v>
-      </c>
-      <c r="D37" t="str">
-        <f>VLOOKUP(C37,'MASTER KEY'!$A$2:$B951,2,FALSE)</f>
-        <v>Butfuco</v>
-      </c>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>575</v>
-      </c>
-      <c r="B38" s="4">
-        <v>1</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>576</v>
-      </c>
-      <c r="D38" t="str">
-        <f>VLOOKUP(C38,'MASTER KEY'!$A$2:$B952,2,FALSE)</f>
-        <v>Cantha</v>
-      </c>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>577</v>
-      </c>
-      <c r="B39" s="4">
-        <v>1</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="D39" t="str">
-        <f>VLOOKUP(C39,'MASTER KEY'!$A$2:$B953,2,FALSE)</f>
-        <v>CphlA</v>
-      </c>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>579</v>
-      </c>
-      <c r="B40" s="4">
-        <v>1</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>580</v>
-      </c>
-      <c r="D40" t="str">
-        <f>VLOOKUP(C40,'MASTER KEY'!$A$2:$B954,2,FALSE)</f>
-        <v>CphlB</v>
-      </c>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>581</v>
-      </c>
-      <c r="B41" s="4">
-        <v>1</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="D41" t="str">
-        <f>VLOOKUP(C41,'MASTER KEY'!$A$2:$B955,2,FALSE)</f>
-        <v>CphlC1</v>
-      </c>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>583</v>
-      </c>
-      <c r="B42" s="4">
-        <v>1</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>584</v>
-      </c>
-      <c r="D42" t="str">
-        <f>VLOOKUP(C42,'MASTER KEY'!$A$2:$B956,2,FALSE)</f>
-        <v>CphlC2</v>
-      </c>
-      <c r="G42" s="2"/>
-    </row>
-    <row r="43" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>585</v>
-      </c>
-      <c r="B43" s="4">
-        <v>1</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>586</v>
-      </c>
-      <c r="D43" t="str">
-        <f>VLOOKUP(C43,'MASTER KEY'!$A$2:$B957,2,FALSE)</f>
-        <v>CphlC3</v>
-      </c>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>587</v>
-      </c>
-      <c r="B44" s="4">
-        <v>1</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="D44" t="str">
-        <f>VLOOKUP(C44,'MASTER KEY'!$A$2:$B958,2,FALSE)</f>
-        <v>CphlC1C2</v>
-      </c>
-      <c r="G44" s="2"/>
-    </row>
-    <row r="45" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>589</v>
-      </c>
-      <c r="B45" s="4">
-        <v>1</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>590</v>
-      </c>
-      <c r="D45" t="str">
-        <f>VLOOKUP(C45,'MASTER KEY'!$A$2:$B959,2,FALSE)</f>
-        <v>CphlideA</v>
-      </c>
-      <c r="G45" s="2"/>
-    </row>
-    <row r="46" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>591</v>
-      </c>
-      <c r="B46" s="4">
-        <v>1</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="D46" t="str">
-        <f>VLOOKUP(C46,'MASTER KEY'!$A$2:$B960,2,FALSE)</f>
-        <v>Diadchr</v>
-      </c>
-      <c r="G46" s="2"/>
-    </row>
-    <row r="47" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>593</v>
-      </c>
-      <c r="B47" s="4">
-        <v>1</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>594</v>
-      </c>
-      <c r="D47" t="str">
-        <f>VLOOKUP(C47,'MASTER KEY'!$A$2:$B961,2,FALSE)</f>
-        <v>Diadino</v>
-      </c>
-      <c r="G47" s="2"/>
-    </row>
-    <row r="48" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>595</v>
-      </c>
-      <c r="B48" s="4">
-        <v>1</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="D48" t="str">
-        <f>VLOOKUP(C48,'MASTER KEY'!$A$2:$B962,2,FALSE)</f>
-        <v>Diato</v>
-      </c>
-      <c r="G48" s="2"/>
-    </row>
-    <row r="49" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>597</v>
-      </c>
-      <c r="B49" s="4">
-        <v>1</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>598</v>
-      </c>
-      <c r="D49" t="str">
-        <f>VLOOKUP(C49,'MASTER KEY'!$A$2:$B963,2,FALSE)</f>
-        <v>Dino</v>
-      </c>
-      <c r="G49" s="2"/>
-    </row>
-    <row r="50" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>599</v>
-      </c>
-      <c r="B50" s="4">
-        <v>1</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>600</v>
-      </c>
-      <c r="D50" t="str">
-        <f>VLOOKUP(C50,'MASTER KEY'!$A$2:$B964,2,FALSE)</f>
-        <v>DvCphlA+CphlA</v>
-      </c>
-      <c r="G50" s="2"/>
-    </row>
-    <row r="51" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>601</v>
-      </c>
-      <c r="B51" s="4">
-        <v>1</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="D51" t="str">
-        <f>VLOOKUP(C51,'MASTER KEY'!$A$2:$B965,2,FALSE)</f>
-        <v>DvCphlA</v>
-      </c>
-      <c r="G51" s="2"/>
-    </row>
-    <row r="52" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>603</v>
-      </c>
-      <c r="B52" s="4">
-        <v>1</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="D52" t="str">
-        <f>VLOOKUP(C52,'MASTER KEY'!$A$2:$B966,2,FALSE)</f>
-        <v>DvCphlB+CphlB</v>
-      </c>
-      <c r="G52" s="2"/>
-    </row>
-    <row r="53" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>605</v>
-      </c>
-      <c r="B53" s="4">
-        <v>1</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>606</v>
-      </c>
-      <c r="D53" t="str">
-        <f>VLOOKUP(C53,'MASTER KEY'!$A$2:$B967,2,FALSE)</f>
-        <v>DvCphlB</v>
-      </c>
-      <c r="G53" s="2"/>
-    </row>
-    <row r="54" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>607</v>
-      </c>
-      <c r="B54" s="4">
-        <v>1</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="D54" t="str">
-        <f>VLOOKUP(C54,'MASTER KEY'!$A$2:$B968,2,FALSE)</f>
-        <v>Echin</v>
-      </c>
-      <c r="G54" s="2"/>
-    </row>
-    <row r="55" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>609</v>
-      </c>
-      <c r="B55" s="4">
-        <v>1</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="D55" t="str">
-        <f>VLOOKUP(C55,'MASTER KEY'!$A$2:$B969,2,FALSE)</f>
-        <v>Fuco</v>
-      </c>
-      <c r="G55" s="2"/>
-    </row>
-    <row r="56" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>611</v>
-      </c>
-      <c r="B56" s="4">
-        <v>1</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="D56" t="str">
-        <f>VLOOKUP(C56,'MASTER KEY'!$A$2:$B970,2,FALSE)</f>
-        <v>Gyro</v>
-      </c>
-      <c r="G56" s="2"/>
-    </row>
-    <row r="57" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>613</v>
-      </c>
-      <c r="B57" s="4">
-        <v>1</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>614</v>
-      </c>
-      <c r="D57" t="str">
-        <f>VLOOKUP(C57,'MASTER KEY'!$A$2:$B971,2,FALSE)</f>
-        <v>Hexfuco</v>
-      </c>
-      <c r="G57" s="2"/>
-    </row>
-    <row r="58" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>615</v>
-      </c>
-      <c r="B58" s="4">
-        <v>1</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>616</v>
-      </c>
-      <c r="D58" t="str">
-        <f>VLOOKUP(C58,'MASTER KEY'!$A$2:$B972,2,FALSE)</f>
-        <v>Ketohexfuco</v>
-      </c>
-      <c r="G58" s="2"/>
-    </row>
-    <row r="59" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>617</v>
-      </c>
-      <c r="B59" s="4">
-        <v>1</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="D59" t="str">
-        <f>VLOOKUP(C59,'MASTER KEY'!$A$2:$B973,2,FALSE)</f>
-        <v>Lut</v>
-      </c>
-      <c r="G59" s="2"/>
-    </row>
-    <row r="60" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>619</v>
-      </c>
-      <c r="B60" s="4">
-        <v>1</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>620</v>
-      </c>
-      <c r="D60" t="str">
-        <f>VLOOKUP(C60,'MASTER KEY'!$A$2:$B974,2,FALSE)</f>
-        <v>Lyco</v>
-      </c>
-      <c r="G60" s="2"/>
-    </row>
-    <row r="61" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>621</v>
-      </c>
-      <c r="B61" s="4">
-        <v>1</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>622</v>
-      </c>
-      <c r="D61" t="str">
-        <f>VLOOKUP(C61,'MASTER KEY'!$A$2:$B975,2,FALSE)</f>
-        <v>MgDvp</v>
-      </c>
-      <c r="G61" s="2"/>
-    </row>
-    <row r="62" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>623</v>
-      </c>
-      <c r="B62" s="4">
-        <v>1</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>624</v>
-      </c>
-      <c r="D62" t="str">
-        <f>VLOOKUP(C62,'MASTER KEY'!$A$2:$B976,2,FALSE)</f>
-        <v>Neo</v>
-      </c>
-      <c r="G62" s="2"/>
-    </row>
-    <row r="63" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>625</v>
-      </c>
-      <c r="B63" s="4">
-        <v>1</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>626</v>
-      </c>
-      <c r="D63" t="str">
-        <f>VLOOKUP(C63,'MASTER KEY'!$A$2:$B977,2,FALSE)</f>
-        <v>Perid</v>
-      </c>
-      <c r="G63" s="2"/>
-    </row>
-    <row r="64" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>627</v>
-      </c>
-      <c r="B64" s="4">
-        <v>1</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>628</v>
-      </c>
-      <c r="D64" t="str">
-        <f>VLOOKUP(C64,'MASTER KEY'!$A$2:$B978,2,FALSE)</f>
-        <v>PhideA</v>
-      </c>
-      <c r="G64" s="2"/>
-    </row>
-    <row r="65" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>629</v>
-      </c>
-      <c r="B65" s="4">
-        <v>1</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>630</v>
-      </c>
-      <c r="D65" t="str">
-        <f>VLOOKUP(C65,'MASTER KEY'!$A$2:$B979,2,FALSE)</f>
-        <v>PhytinA</v>
-      </c>
-      <c r="G65" s="2"/>
-    </row>
-    <row r="66" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>631</v>
-      </c>
-      <c r="B66" s="4">
-        <v>1</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="D66" t="str">
-        <f>VLOOKUP(C66,'MASTER KEY'!$A$2:$B980,2,FALSE)</f>
-        <v>PhytinB</v>
-      </c>
-      <c r="G66" s="2"/>
-    </row>
-    <row r="67" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>633</v>
-      </c>
-      <c r="B67" s="4">
-        <v>1</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>634</v>
-      </c>
-      <c r="D67" t="str">
-        <f>VLOOKUP(C67,'MASTER KEY'!$A$2:$B981,2,FALSE)</f>
-        <v>Pras</v>
-      </c>
-      <c r="G67" s="2"/>
-    </row>
-    <row r="68" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>635</v>
-      </c>
-      <c r="B68" s="4">
-        <v>1</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>636</v>
-      </c>
-      <c r="D68" t="str">
-        <f>VLOOKUP(C68,'MASTER KEY'!$A$2:$B982,2,FALSE)</f>
-        <v>PyrophideA</v>
-      </c>
-      <c r="G68" s="2"/>
-    </row>
-    <row r="69" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>637</v>
-      </c>
-      <c r="B69" s="4">
-        <v>1</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>638</v>
-      </c>
-      <c r="D69" t="str">
-        <f>VLOOKUP(C69,'MASTER KEY'!$A$2:$B983,2,FALSE)</f>
-        <v>PyrophytinA</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>639</v>
-      </c>
-      <c r="B70" s="4">
-        <v>1</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>640</v>
-      </c>
-      <c r="D70" t="str">
-        <f>VLOOKUP(C70,'MASTER KEY'!$A$2:$B984,2,FALSE)</f>
-        <v>Viola</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>641</v>
-      </c>
-      <c r="B71" s="4">
-        <v>1</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>642</v>
-      </c>
-      <c r="D71" t="str">
-        <f>VLOOKUP(C71,'MASTER KEY'!$A$2:$B985,2,FALSE)</f>
-        <v>Zea</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>643</v>
-      </c>
-      <c r="B72" s="4">
-        <v>1</v>
-      </c>
-      <c r="C72" t="s">
-        <v>504</v>
-      </c>
-      <c r="D72" t="e">
-        <f>VLOOKUP(C72,'MASTER KEY'!$A$2:$B986,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>644</v>
-      </c>
-      <c r="B73" s="4">
-        <v>1</v>
-      </c>
-      <c r="C73" t="s">
-        <v>504</v>
-      </c>
-      <c r="D73" t="e">
-        <f>VLOOKUP(C73,'MASTER KEY'!$A$2:$B987,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L369"/>
+  <dimension ref="A1:L372"/>
   <sheetViews>
     <sheetView zoomScale="66" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A352" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A369" sqref="A369"/>
+      <selection pane="bottomLeft" activeCell="A370" sqref="A370:A372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20707,8 +19922,8 @@
         <v>2053</v>
       </c>
       <c r="J359" s="55"/>
-      <c r="K359" s="55" t="s">
-        <v>2053</v>
+      <c r="K359" s="2" t="s">
+        <v>1732</v>
       </c>
       <c r="L359" s="55" t="s">
         <v>2053</v>
@@ -20743,8 +19958,8 @@
         <v>2053</v>
       </c>
       <c r="J360" s="55"/>
-      <c r="K360" s="55" t="s">
-        <v>2053</v>
+      <c r="K360" s="2" t="s">
+        <v>1732</v>
       </c>
       <c r="L360" s="55" t="s">
         <v>2053</v>
@@ -20779,8 +19994,8 @@
         <v>2053</v>
       </c>
       <c r="J361" s="55"/>
-      <c r="K361" s="55" t="s">
-        <v>2053</v>
+      <c r="K361" s="2" t="s">
+        <v>1732</v>
       </c>
       <c r="L361" s="55" t="s">
         <v>2053</v>
@@ -20815,8 +20030,8 @@
         <v>2053</v>
       </c>
       <c r="J362" s="55"/>
-      <c r="K362" s="55" t="s">
-        <v>2053</v>
+      <c r="K362" s="2" t="s">
+        <v>1732</v>
       </c>
       <c r="L362" s="55" t="s">
         <v>2053</v>
@@ -20851,8 +20066,8 @@
         <v>2053</v>
       </c>
       <c r="J363" s="55"/>
-      <c r="K363" s="55" t="s">
-        <v>2053</v>
+      <c r="K363" s="2" t="s">
+        <v>1732</v>
       </c>
       <c r="L363" s="55" t="s">
         <v>2053</v>
@@ -20887,8 +20102,8 @@
         <v>2053</v>
       </c>
       <c r="J364" s="55"/>
-      <c r="K364" s="55" t="s">
-        <v>2053</v>
+      <c r="K364" s="2" t="s">
+        <v>1732</v>
       </c>
       <c r="L364" s="55" t="s">
         <v>2053</v>
@@ -20923,8 +20138,8 @@
         <v>2053</v>
       </c>
       <c r="J365" s="55"/>
-      <c r="K365" s="55" t="s">
-        <v>2053</v>
+      <c r="K365" s="2" t="s">
+        <v>1732</v>
       </c>
       <c r="L365" s="55" t="s">
         <v>2053</v>
@@ -20959,8 +20174,8 @@
         <v>2053</v>
       </c>
       <c r="J366" s="59"/>
-      <c r="K366" s="59" t="s">
-        <v>2053</v>
+      <c r="K366" s="2" t="s">
+        <v>1732</v>
       </c>
       <c r="L366" s="59" t="s">
         <v>2053</v>
@@ -20995,8 +20210,8 @@
         <v>2053</v>
       </c>
       <c r="J367" s="55"/>
-      <c r="K367" s="55" t="s">
-        <v>2053</v>
+      <c r="K367" s="2" t="s">
+        <v>1732</v>
       </c>
       <c r="L367" s="55" t="s">
         <v>2053</v>
@@ -21031,7 +20246,7 @@
         <v>1732</v>
       </c>
     </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A369" s="6" t="s">
         <v>2091</v>
       </c>
@@ -21049,6 +20264,102 @@
       </c>
       <c r="F369" s="6" t="s">
         <v>1850</v>
+      </c>
+    </row>
+    <row r="370" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A370" s="2" t="s">
+        <v>2102</v>
+      </c>
+      <c r="B370" s="56" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C370" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="D370" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="E370" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="F370" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="G370" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="H370" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="I370" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="K370" s="2" t="s">
+        <v>1732</v>
+      </c>
+    </row>
+    <row r="371" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A371" s="6" t="s">
+        <v>2103</v>
+      </c>
+      <c r="B371" s="56" t="s">
+        <v>2097</v>
+      </c>
+      <c r="C371" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="D371" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="E371" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="F371" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="G371" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="H371" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="I371" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="K371" s="2" t="s">
+        <v>1732</v>
+      </c>
+    </row>
+    <row r="372" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A372" s="2" t="s">
+        <v>2104</v>
+      </c>
+      <c r="B372" s="56" t="s">
+        <v>2099</v>
+      </c>
+      <c r="C372" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="D372" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="E372" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="F372" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="G372" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="H372" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="I372" s="55" t="s">
+        <v>2053</v>
+      </c>
+      <c r="K372" s="2" t="s">
+        <v>1732</v>
       </c>
     </row>
   </sheetData>
@@ -21058,6 +20369,1167 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:G73"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>525</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="D2" t="str">
+        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B916,2,FALSE)</f>
+        <v>Secchi Depth</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>526</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" t="str">
+        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B917,2,FALSE)</f>
+        <v>Salinity</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>527</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>504</v>
+      </c>
+      <c r="D4" t="e">
+        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B918,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>528</v>
+      </c>
+      <c r="B5" s="25">
+        <v>1.2000000048E-2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="D5" t="str">
+        <f>VLOOKUP(C5,'MASTER KEY'!$A$2:$B919,2,FALSE)</f>
+        <v>Dissolved Inorganic Carbon</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>530</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>504</v>
+      </c>
+      <c r="D6" t="e">
+        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B920,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>531</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D7" t="str">
+        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B921,2,FALSE)</f>
+        <v>Total Alkalinity</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>532</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>504</v>
+      </c>
+      <c r="D8" t="e">
+        <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B922,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>533</v>
+      </c>
+      <c r="B9" s="14">
+        <f>32/1000</f>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D9" t="str">
+        <f>VLOOKUP(C9,'MASTER KEY'!$A$2:$B923,2,FALSE)</f>
+        <v>Dissolved Oxygen</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>534</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>504</v>
+      </c>
+      <c r="D10" t="e">
+        <f>VLOOKUP(C10,'MASTER KEY'!$A$2:$B924,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>535</v>
+      </c>
+      <c r="B11" s="26">
+        <v>1.4E-2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="D11" t="str">
+        <f>VLOOKUP(C11,'MASTER KEY'!$A$2:$B925,2,FALSE)</f>
+        <v>Ammonium</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>536</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>504</v>
+      </c>
+      <c r="D12" t="e">
+        <f>VLOOKUP(C12,'MASTER KEY'!$A$2:$B926,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>537</v>
+      </c>
+      <c r="B13" s="26">
+        <v>1.4E-2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="D13" t="str">
+        <f>VLOOKUP(C13,'MASTER KEY'!$A$2:$B927,2,FALSE)</f>
+        <v>Nitrate</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>538</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>504</v>
+      </c>
+      <c r="D14" t="e">
+        <f>VLOOKUP(C14,'MASTER KEY'!$A$2:$B928,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>539</v>
+      </c>
+      <c r="B15" s="26">
+        <v>1.4E-2</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="D15" t="str">
+        <f>VLOOKUP(C15,'MASTER KEY'!$A$2:$B929,2,FALSE)</f>
+        <v>Nitrite</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>541</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>504</v>
+      </c>
+      <c r="D16" t="e">
+        <f>VLOOKUP(C16,'MASTER KEY'!$A$2:$B930,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>542</v>
+      </c>
+      <c r="B17" s="14">
+        <v>3.1E-2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="D17" t="str">
+        <f>VLOOKUP(C17,'MASTER KEY'!$A$2:$B931,2,FALSE)</f>
+        <v>Filterable Reactive Phosphate</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>543</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>504</v>
+      </c>
+      <c r="D18" t="e">
+        <f>VLOOKUP(C18,'MASTER KEY'!$A$2:$B932,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>544</v>
+      </c>
+      <c r="B19" s="14">
+        <v>2.81E-2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="D19" t="str">
+        <f>VLOOKUP(C19,'MASTER KEY'!$A$2:$B933,2,FALSE)</f>
+        <v>Reactive Silica</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>545</v>
+      </c>
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>504</v>
+      </c>
+      <c r="D20" t="e">
+        <f>VLOOKUP(C20,'MASTER KEY'!$A$2:$B934,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>546</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="D21" t="str">
+        <f>VLOOKUP(C21,'MASTER KEY'!$A$2:$B935,2,FALSE)</f>
+        <v>TSSorganic</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>548</v>
+      </c>
+      <c r="B22" s="4">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="D22" t="str">
+        <f>VLOOKUP(C22,'MASTER KEY'!$A$2:$B936,2,FALSE)</f>
+        <v>TSSinorganic</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>550</v>
+      </c>
+      <c r="B23" s="4">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="D23" t="str">
+        <f>VLOOKUP(C23,'MASTER KEY'!$A$2:$B937,2,FALSE)</f>
+        <v>Total Suspended Solids</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>551</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>504</v>
+      </c>
+      <c r="D24" t="e">
+        <f>VLOOKUP(C24,'MASTER KEY'!$A$2:$B938,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>552</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="D25" t="str">
+        <f>VLOOKUP(C25,'MASTER KEY'!$A$2:$B939,2,FALSE)</f>
+        <v>Prochlorococcus</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>554</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>504</v>
+      </c>
+      <c r="D26" t="e">
+        <f>VLOOKUP(C26,'MASTER KEY'!$A$2:$B940,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>555</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="D27" t="str">
+        <f>VLOOKUP(C27,'MASTER KEY'!$A$2:$B941,2,FALSE)</f>
+        <v>Synechococcus</v>
+      </c>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>557</v>
+      </c>
+      <c r="B28" s="4">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>504</v>
+      </c>
+      <c r="D28" t="e">
+        <f>VLOOKUP(C28,'MASTER KEY'!$A$2:$B942,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>558</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="D29" t="str">
+        <f>VLOOKUP(C29,'MASTER KEY'!$A$2:$B943,2,FALSE)</f>
+        <v>Picoeukaryotes</v>
+      </c>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>560</v>
+      </c>
+      <c r="B30" s="4">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>504</v>
+      </c>
+      <c r="D30" t="e">
+        <f>VLOOKUP(C30,'MASTER KEY'!$A$2:$B944,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>561</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="D31" t="str">
+        <f>VLOOKUP(C31,'MASTER KEY'!$A$2:$B945,2,FALSE)</f>
+        <v>Allo</v>
+      </c>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>563</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="D32" t="str">
+        <f>VLOOKUP(C32,'MASTER KEY'!$A$2:$B946,2,FALSE)</f>
+        <v>AlphaBetaCar</v>
+      </c>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>565</v>
+      </c>
+      <c r="B33" s="4">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="D33" t="str">
+        <f>VLOOKUP(C33,'MASTER KEY'!$A$2:$B947,2,FALSE)</f>
+        <v>Anth</v>
+      </c>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>567</v>
+      </c>
+      <c r="B34" s="4">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="D34" t="str">
+        <f>VLOOKUP(C34,'MASTER KEY'!$A$2:$B948,2,FALSE)</f>
+        <v>Asta</v>
+      </c>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>569</v>
+      </c>
+      <c r="B35" s="4">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="D35" t="str">
+        <f>VLOOKUP(C35,'MASTER KEY'!$A$2:$B949,2,FALSE)</f>
+        <v>BetaBetaCar</v>
+      </c>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>571</v>
+      </c>
+      <c r="B36" s="4">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="D36" t="str">
+        <f>VLOOKUP(C36,'MASTER KEY'!$A$2:$B950,2,FALSE)</f>
+        <v>BetaEpiCar</v>
+      </c>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>573</v>
+      </c>
+      <c r="B37" s="4">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="D37" t="str">
+        <f>VLOOKUP(C37,'MASTER KEY'!$A$2:$B951,2,FALSE)</f>
+        <v>Butfuco</v>
+      </c>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>575</v>
+      </c>
+      <c r="B38" s="4">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="D38" t="str">
+        <f>VLOOKUP(C38,'MASTER KEY'!$A$2:$B952,2,FALSE)</f>
+        <v>Cantha</v>
+      </c>
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>577</v>
+      </c>
+      <c r="B39" s="4">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="D39" t="str">
+        <f>VLOOKUP(C39,'MASTER KEY'!$A$2:$B953,2,FALSE)</f>
+        <v>CphlA</v>
+      </c>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>579</v>
+      </c>
+      <c r="B40" s="4">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="D40" t="str">
+        <f>VLOOKUP(C40,'MASTER KEY'!$A$2:$B954,2,FALSE)</f>
+        <v>CphlB</v>
+      </c>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>581</v>
+      </c>
+      <c r="B41" s="4">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="D41" t="str">
+        <f>VLOOKUP(C41,'MASTER KEY'!$A$2:$B955,2,FALSE)</f>
+        <v>CphlC1</v>
+      </c>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>583</v>
+      </c>
+      <c r="B42" s="4">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="D42" t="str">
+        <f>VLOOKUP(C42,'MASTER KEY'!$A$2:$B956,2,FALSE)</f>
+        <v>CphlC2</v>
+      </c>
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>585</v>
+      </c>
+      <c r="B43" s="4">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="D43" t="str">
+        <f>VLOOKUP(C43,'MASTER KEY'!$A$2:$B957,2,FALSE)</f>
+        <v>CphlC3</v>
+      </c>
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>587</v>
+      </c>
+      <c r="B44" s="4">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="D44" t="str">
+        <f>VLOOKUP(C44,'MASTER KEY'!$A$2:$B958,2,FALSE)</f>
+        <v>CphlC1C2</v>
+      </c>
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>589</v>
+      </c>
+      <c r="B45" s="4">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="D45" t="str">
+        <f>VLOOKUP(C45,'MASTER KEY'!$A$2:$B959,2,FALSE)</f>
+        <v>CphlideA</v>
+      </c>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>591</v>
+      </c>
+      <c r="B46" s="4">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="D46" t="str">
+        <f>VLOOKUP(C46,'MASTER KEY'!$A$2:$B960,2,FALSE)</f>
+        <v>Diadchr</v>
+      </c>
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>593</v>
+      </c>
+      <c r="B47" s="4">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="D47" t="str">
+        <f>VLOOKUP(C47,'MASTER KEY'!$A$2:$B961,2,FALSE)</f>
+        <v>Diadino</v>
+      </c>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>595</v>
+      </c>
+      <c r="B48" s="4">
+        <v>1</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="D48" t="str">
+        <f>VLOOKUP(C48,'MASTER KEY'!$A$2:$B962,2,FALSE)</f>
+        <v>Diato</v>
+      </c>
+      <c r="G48" s="2"/>
+    </row>
+    <row r="49" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>597</v>
+      </c>
+      <c r="B49" s="4">
+        <v>1</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="D49" t="str">
+        <f>VLOOKUP(C49,'MASTER KEY'!$A$2:$B963,2,FALSE)</f>
+        <v>Dino</v>
+      </c>
+      <c r="G49" s="2"/>
+    </row>
+    <row r="50" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>599</v>
+      </c>
+      <c r="B50" s="4">
+        <v>1</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="D50" t="str">
+        <f>VLOOKUP(C50,'MASTER KEY'!$A$2:$B964,2,FALSE)</f>
+        <v>DvCphlA+CphlA</v>
+      </c>
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>601</v>
+      </c>
+      <c r="B51" s="4">
+        <v>1</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="D51" t="str">
+        <f>VLOOKUP(C51,'MASTER KEY'!$A$2:$B965,2,FALSE)</f>
+        <v>DvCphlA</v>
+      </c>
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>603</v>
+      </c>
+      <c r="B52" s="4">
+        <v>1</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="D52" t="str">
+        <f>VLOOKUP(C52,'MASTER KEY'!$A$2:$B966,2,FALSE)</f>
+        <v>DvCphlB+CphlB</v>
+      </c>
+      <c r="G52" s="2"/>
+    </row>
+    <row r="53" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>605</v>
+      </c>
+      <c r="B53" s="4">
+        <v>1</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="D53" t="str">
+        <f>VLOOKUP(C53,'MASTER KEY'!$A$2:$B967,2,FALSE)</f>
+        <v>DvCphlB</v>
+      </c>
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>607</v>
+      </c>
+      <c r="B54" s="4">
+        <v>1</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="D54" t="str">
+        <f>VLOOKUP(C54,'MASTER KEY'!$A$2:$B968,2,FALSE)</f>
+        <v>Echin</v>
+      </c>
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>609</v>
+      </c>
+      <c r="B55" s="4">
+        <v>1</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="D55" t="str">
+        <f>VLOOKUP(C55,'MASTER KEY'!$A$2:$B969,2,FALSE)</f>
+        <v>Fuco</v>
+      </c>
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>611</v>
+      </c>
+      <c r="B56" s="4">
+        <v>1</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="D56" t="str">
+        <f>VLOOKUP(C56,'MASTER KEY'!$A$2:$B970,2,FALSE)</f>
+        <v>Gyro</v>
+      </c>
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>613</v>
+      </c>
+      <c r="B57" s="4">
+        <v>1</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="D57" t="str">
+        <f>VLOOKUP(C57,'MASTER KEY'!$A$2:$B971,2,FALSE)</f>
+        <v>Hexfuco</v>
+      </c>
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>615</v>
+      </c>
+      <c r="B58" s="4">
+        <v>1</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="D58" t="str">
+        <f>VLOOKUP(C58,'MASTER KEY'!$A$2:$B972,2,FALSE)</f>
+        <v>Ketohexfuco</v>
+      </c>
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>617</v>
+      </c>
+      <c r="B59" s="4">
+        <v>1</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="D59" t="str">
+        <f>VLOOKUP(C59,'MASTER KEY'!$A$2:$B973,2,FALSE)</f>
+        <v>Lut</v>
+      </c>
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>619</v>
+      </c>
+      <c r="B60" s="4">
+        <v>1</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="D60" t="str">
+        <f>VLOOKUP(C60,'MASTER KEY'!$A$2:$B974,2,FALSE)</f>
+        <v>Lyco</v>
+      </c>
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>621</v>
+      </c>
+      <c r="B61" s="4">
+        <v>1</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="D61" t="str">
+        <f>VLOOKUP(C61,'MASTER KEY'!$A$2:$B975,2,FALSE)</f>
+        <v>MgDvp</v>
+      </c>
+      <c r="G61" s="2"/>
+    </row>
+    <row r="62" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>623</v>
+      </c>
+      <c r="B62" s="4">
+        <v>1</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="D62" t="str">
+        <f>VLOOKUP(C62,'MASTER KEY'!$A$2:$B976,2,FALSE)</f>
+        <v>Neo</v>
+      </c>
+      <c r="G62" s="2"/>
+    </row>
+    <row r="63" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>625</v>
+      </c>
+      <c r="B63" s="4">
+        <v>1</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="D63" t="str">
+        <f>VLOOKUP(C63,'MASTER KEY'!$A$2:$B977,2,FALSE)</f>
+        <v>Perid</v>
+      </c>
+      <c r="G63" s="2"/>
+    </row>
+    <row r="64" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>627</v>
+      </c>
+      <c r="B64" s="4">
+        <v>1</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="D64" t="str">
+        <f>VLOOKUP(C64,'MASTER KEY'!$A$2:$B978,2,FALSE)</f>
+        <v>PhideA</v>
+      </c>
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>629</v>
+      </c>
+      <c r="B65" s="4">
+        <v>1</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="D65" t="str">
+        <f>VLOOKUP(C65,'MASTER KEY'!$A$2:$B979,2,FALSE)</f>
+        <v>PhytinA</v>
+      </c>
+      <c r="G65" s="2"/>
+    </row>
+    <row r="66" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>631</v>
+      </c>
+      <c r="B66" s="4">
+        <v>1</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D66" t="str">
+        <f>VLOOKUP(C66,'MASTER KEY'!$A$2:$B980,2,FALSE)</f>
+        <v>PhytinB</v>
+      </c>
+      <c r="G66" s="2"/>
+    </row>
+    <row r="67" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>633</v>
+      </c>
+      <c r="B67" s="4">
+        <v>1</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="D67" t="str">
+        <f>VLOOKUP(C67,'MASTER KEY'!$A$2:$B981,2,FALSE)</f>
+        <v>Pras</v>
+      </c>
+      <c r="G67" s="2"/>
+    </row>
+    <row r="68" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>635</v>
+      </c>
+      <c r="B68" s="4">
+        <v>1</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="D68" t="str">
+        <f>VLOOKUP(C68,'MASTER KEY'!$A$2:$B982,2,FALSE)</f>
+        <v>PyrophideA</v>
+      </c>
+      <c r="G68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>637</v>
+      </c>
+      <c r="B69" s="4">
+        <v>1</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="D69" t="str">
+        <f>VLOOKUP(C69,'MASTER KEY'!$A$2:$B983,2,FALSE)</f>
+        <v>PyrophytinA</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>639</v>
+      </c>
+      <c r="B70" s="4">
+        <v>1</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="D70" t="str">
+        <f>VLOOKUP(C70,'MASTER KEY'!$A$2:$B984,2,FALSE)</f>
+        <v>Viola</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>641</v>
+      </c>
+      <c r="B71" s="4">
+        <v>1</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="D71" t="str">
+        <f>VLOOKUP(C71,'MASTER KEY'!$A$2:$B985,2,FALSE)</f>
+        <v>Zea</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>643</v>
+      </c>
+      <c r="B72" s="4">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>504</v>
+      </c>
+      <c r="D72" t="e">
+        <f>VLOOKUP(C72,'MASTER KEY'!$A$2:$B986,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>644</v>
+      </c>
+      <c r="B73" s="4">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>504</v>
+      </c>
+      <c r="D73" t="e">
+        <f>VLOOKUP(C73,'MASTER KEY'!$A$2:$B987,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -21423,7 +21895,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -22085,7 +22557,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -22463,7 +22935,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -23022,7 +23494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -23414,7 +23886,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -23528,7 +24000,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -23834,7 +24306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -24066,7 +24538,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -24234,154 +24706,6 @@
       <c r="D10" t="str">
         <f>VLOOKUP(C10,'MASTER KEY'!$A$2:$B921,2,FALSE)</f>
         <v>Mean Wave Direction</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:E8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D2" t="str">
-        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B913,2,FALSE)</f>
-        <v>Water Surface Height</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>227</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D3" t="e">
-        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B914,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>229</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D4" t="str">
-        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B915,2,FALSE)</f>
-        <v>Current Velocity (x component)</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>231</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D5" t="str">
-        <f>VLOOKUP(C5,'MASTER KEY'!$A$2:$B916,2,FALSE)</f>
-        <v>Current Velocity (y component)</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>233</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D6" t="str">
-        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B917,2,FALSE)</f>
-        <v>Temperature</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>235</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D7" t="str">
-        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B918,2,FALSE)</f>
-        <v>Salinity</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>237</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D8" t="str">
-        <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B919,2,FALSE)</f>
-        <v>Current Velocity</v>
       </c>
     </row>
   </sheetData>
@@ -24456,6 +24780,154 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D2" t="str">
+        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B913,2,FALSE)</f>
+        <v>Water Surface Height</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D3" t="e">
+        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B914,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D4" t="str">
+        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B915,2,FALSE)</f>
+        <v>Current Velocity (x component)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D5" t="str">
+        <f>VLOOKUP(C5,'MASTER KEY'!$A$2:$B916,2,FALSE)</f>
+        <v>Current Velocity (y component)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D6" t="str">
+        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B917,2,FALSE)</f>
+        <v>Temperature</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D7" t="str">
+        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B918,2,FALSE)</f>
+        <v>Salinity</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D8" t="str">
+        <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B919,2,FALSE)</f>
+        <v>Current Velocity</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -24581,7 +25053,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -25781,13 +26253,203 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE367AE7-ACD7-4C91-913C-5067EFA2602D}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="29.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2094</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2076</v>
+      </c>
+      <c r="D2" t="str">
+        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B1221,2,TRUE)</f>
+        <v>eastern wind speed at 10 m height</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2095</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="57" t="s">
+        <v>2077</v>
+      </c>
+      <c r="D3" t="str">
+        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B1222,2,TRUE)</f>
+        <v>northern wind speed at 10 m height</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="62" t="s">
+        <v>2096</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2102</v>
+      </c>
+      <c r="D4" t="str">
+        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B1223,2,TRUE)</f>
+        <v>mslp</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="62" t="s">
+        <v>2097</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>2103</v>
+      </c>
+      <c r="D5" t="str">
+        <f>VLOOKUP(C5,'MASTER KEY'!$A$2:$B1224,2,TRUE)</f>
+        <v>lwsfcdown</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2098</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="57" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D6" t="str">
+        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B1224,2,TRUE)</f>
+        <v>Photosynthetically Active Radiation</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="62" t="s">
+        <v>2099</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2104</v>
+      </c>
+      <c r="D7" t="str">
+        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B1226,2,TRUE)</f>
+        <v>temp_scrn</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>2100</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>2088</v>
+      </c>
+      <c r="D8" t="str">
+        <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B1226,2,TRUE)</f>
+        <v>Precipitation Rate</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2101</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="D9" t="str">
+        <f>VLOOKUP(C9,'MASTER KEY'!$A$2:$B1227,2,TRUE)</f>
+        <v>Relative Humidity</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="12"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="12"/>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="C12" s="58"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="58"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="58"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -26076,7 +26738,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -26160,7 +26822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -33124,7 +33786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -34153,7 +34815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -35032,339 +35694,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:E20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>844</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="D2" t="str">
-        <f>VLOOKUP(C2,'MASTER KEY'!$A$2:$B916,2,FALSE)</f>
-        <v>Wind Speed</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>845</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="D3" t="str">
-        <f>VLOOKUP(C3,'MASTER KEY'!$A$2:$B917,2,FALSE)</f>
-        <v>Wind Direction</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>846</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>847</v>
-      </c>
-      <c r="D4" t="str">
-        <f>VLOOKUP(C4,'MASTER KEY'!$A$2:$B918,2,FALSE)</f>
-        <v>Wind Direction (std)</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>848</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="D5" t="str">
-        <f>VLOOKUP(C5,'MASTER KEY'!$A$2:$B919,2,FALSE)</f>
-        <v>Wind Speed (max)</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>849</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>850</v>
-      </c>
-      <c r="D6" t="str">
-        <f>VLOOKUP(C6,'MASTER KEY'!$A$2:$B920,2,FALSE)</f>
-        <v>Wind Speed (min)</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>851</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="D7" t="str">
-        <f>VLOOKUP(C7,'MASTER KEY'!$A$2:$B921,2,FALSE)</f>
-        <v>Station Level Pressure</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>852</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>853</v>
-      </c>
-      <c r="D8" t="str">
-        <f>VLOOKUP(C8,'MASTER KEY'!$A$2:$B922,2,FALSE)</f>
-        <v>Station Level Pressure (max)</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>854</v>
-      </c>
-      <c r="B9" s="4">
-        <v>1</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>855</v>
-      </c>
-      <c r="D9" t="str">
-        <f>VLOOKUP(C9,'MASTER KEY'!$A$2:$B923,2,FALSE)</f>
-        <v>Station Level Pressure (min)</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>856</v>
-      </c>
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>857</v>
-      </c>
-      <c r="D10" t="str">
-        <f>VLOOKUP(C10,'MASTER KEY'!$A$2:$B924,2,FALSE)</f>
-        <v>Station Level Pressure (std)</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>858</v>
-      </c>
-      <c r="B11" s="4">
-        <v>1</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>859</v>
-      </c>
-      <c r="D11" t="str">
-        <f>VLOOKUP(C11,'MASTER KEY'!$A$2:$B925,2,FALSE)</f>
-        <v>Surface Solar Irradiance</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>860</v>
-      </c>
-      <c r="B12" s="4">
-        <v>1</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>861</v>
-      </c>
-      <c r="D12" t="str">
-        <f>VLOOKUP(C12,'MASTER KEY'!$A$2:$B926,2,FALSE)</f>
-        <v>Surface Solar Irradiance (max)</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>862</v>
-      </c>
-      <c r="B13" s="4">
-        <v>1</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>863</v>
-      </c>
-      <c r="D13" t="str">
-        <f>VLOOKUP(C13,'MASTER KEY'!$A$2:$B927,2,FALSE)</f>
-        <v>Surface Solar Irradiance (min)</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>864</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>865</v>
-      </c>
-      <c r="D14" t="str">
-        <f>VLOOKUP(C14,'MASTER KEY'!$A$2:$B928,2,FALSE)</f>
-        <v>Surface Solar Irradiance (std)</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>866</v>
-      </c>
-      <c r="B15" s="4">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="D15" t="str">
-        <f>VLOOKUP(C15,'MASTER KEY'!$A$2:$B929,2,FALSE)</f>
-        <v>Surface Photosynthetically Active Photon Flux</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>867</v>
-      </c>
-      <c r="B16" s="4">
-        <v>1</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>868</v>
-      </c>
-      <c r="D16" t="str">
-        <f>VLOOKUP(C16,'MASTER KEY'!$A$2:$B930,2,FALSE)</f>
-        <v>Surface Photosynthetically Active Photon Flux (max)</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>869</v>
-      </c>
-      <c r="B17" s="4">
-        <v>1</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>870</v>
-      </c>
-      <c r="D17" t="str">
-        <f>VLOOKUP(C17,'MASTER KEY'!$A$2:$B931,2,FALSE)</f>
-        <v>Surface Photosynthetically Active Photon Flux (min)</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>871</v>
-      </c>
-      <c r="B18" s="4">
-        <v>1</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>275</v>
-      </c>
-      <c r="D18" t="str">
-        <f>VLOOKUP(C18,'MASTER KEY'!$A$2:$B932,2,FALSE)</f>
-        <v>Surface Photosynthetically Active Photon Flux (std)</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>872</v>
-      </c>
-      <c r="B19" s="4">
-        <f>4*24</f>
-        <v>96</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>873</v>
-      </c>
-      <c r="D19" t="str">
-        <f>VLOOKUP(C19,'MASTER KEY'!$A$2:$B933,2,FALSE)</f>
-        <v>Daily Solar Irradiance</v>
-      </c>
-      <c r="E19" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>875</v>
-      </c>
-      <c r="B20" s="4">
-        <f>4*24</f>
-        <v>96</v>
-      </c>
-      <c r="C20" s="31" t="s">
-        <v>804</v>
-      </c>
-      <c r="D20" t="str">
-        <f>VLOOKUP(C20,'MASTER KEY'!$A$2:$B934,2,FALSE)</f>
-        <v>Daily Surface Photosynthetically Active Photon Flux</v>
-      </c>
-      <c r="E20" t="s">
-        <v>874</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
root path is changeable
</commit_message>
<xml_diff>
--- a/data-governance/variable_key.xlsx
+++ b/data-governance/variable_key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loxte\Downloads\22_04_2024 wamsi work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\AppData\Local\Temp\scp56432\GIS_DATA\csiem-data-hub\git\data-governance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F786E5F0-CC3F-46BF-B84B-C5E67F045F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A79A30-7942-406C-A01C-3AEA4FA2FF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -11536,11 +11536,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L372"/>
+  <dimension ref="A1:V372"/>
   <sheetViews>
-    <sheetView zoomScale="66" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A352" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A370" sqref="A370:A372"/>
+    <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T66" sqref="T66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11557,6 +11557,7 @@
     <col min="10" max="10" width="12.33203125" style="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.109375" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="60" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12454,7 +12455,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>1430</v>
       </c>
@@ -12483,7 +12484,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>1435</v>
       </c>
@@ -12509,7 +12510,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>1439</v>
       </c>
@@ -12538,7 +12539,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>1444</v>
       </c>
@@ -12567,7 +12568,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>1449</v>
       </c>
@@ -12593,7 +12594,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>1453</v>
       </c>
@@ -12622,7 +12623,7 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>1459</v>
       </c>
@@ -12648,7 +12649,7 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>1463</v>
       </c>
@@ -12674,7 +12675,7 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>1467</v>
       </c>
@@ -12700,7 +12701,7 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>1471</v>
       </c>
@@ -12726,7 +12727,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>1476</v>
       </c>
@@ -12752,7 +12753,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>1480</v>
       </c>
@@ -12777,8 +12778,9 @@
       <c r="K44" s="2" t="s">
         <v>1475</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V44" s="28"/>
+    </row>
+    <row r="45" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>1484</v>
       </c>
@@ -12803,8 +12805,9 @@
       <c r="K45" s="2" t="s">
         <v>1475</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V45" s="28"/>
+    </row>
+    <row r="46" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>1488</v>
       </c>
@@ -12829,8 +12832,9 @@
       <c r="K46" s="2" t="s">
         <v>1475</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V46" s="28"/>
+    </row>
+    <row r="47" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>1489</v>
       </c>
@@ -12855,8 +12859,9 @@
       <c r="K47" s="2" t="s">
         <v>1475</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V47" s="28"/>
+    </row>
+    <row r="48" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>1490</v>
       </c>
@@ -12881,8 +12886,9 @@
       <c r="K48" s="2" t="s">
         <v>1325</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V48" s="28"/>
+    </row>
+    <row r="49" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>1494</v>
       </c>
@@ -12904,8 +12910,9 @@
       <c r="K49" s="2" t="s">
         <v>1325</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V49" s="28"/>
+    </row>
+    <row r="50" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>1497</v>
       </c>
@@ -12927,8 +12934,9 @@
       <c r="K50" s="2" t="s">
         <v>1325</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V50" s="28"/>
+    </row>
+    <row r="51" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>1500</v>
       </c>
@@ -12950,8 +12958,9 @@
       <c r="K51" s="2" t="s">
         <v>1325</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V51" s="28"/>
+    </row>
+    <row r="52" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>1503</v>
       </c>
@@ -12973,8 +12982,9 @@
       <c r="K52" s="2" t="s">
         <v>1325</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V52" s="29"/>
+    </row>
+    <row r="53" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>1506</v>
       </c>
@@ -12996,8 +13006,9 @@
       <c r="K53" s="2" t="s">
         <v>1325</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V53" s="43"/>
+    </row>
+    <row r="54" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>1509</v>
       </c>
@@ -13022,8 +13033,9 @@
       <c r="K54" s="2" t="s">
         <v>1325</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V54" s="28"/>
+    </row>
+    <row r="55" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>1513</v>
       </c>
@@ -13045,8 +13057,9 @@
       <c r="K55" s="2" t="s">
         <v>1325</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V55" s="28"/>
+    </row>
+    <row r="56" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>1516</v>
       </c>
@@ -13069,7 +13082,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>1519</v>
       </c>
@@ -13092,7 +13105,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>1522</v>
       </c>
@@ -13115,7 +13128,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>1525</v>
       </c>
@@ -13153,7 +13166,7 @@
         <v>1532</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>1533</v>
       </c>
@@ -13176,7 +13189,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>1536</v>
       </c>
@@ -13199,7 +13212,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>1539</v>
       </c>
@@ -13222,7 +13235,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>1542</v>
       </c>
@@ -13245,7 +13258,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>1545</v>
       </c>
@@ -20365,6 +20378,7 @@
   </sheetData>
   <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="261" orientation="landscape" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -26259,7 +26273,7 @@
   </sheetPr>
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>